<commit_message>
Q4 2021 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\IAD activities\6. MAS_Series\NAP\NAP detailed series as of April 2021\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2022\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$V$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$W$202</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="57">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -201,16 +201,19 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Annual 2000 to 2020</t>
-  </si>
-  <si>
-    <t>Annual 2001 to 2020</t>
-  </si>
-  <si>
     <t>2019 - 2020</t>
   </si>
   <si>
-    <t>As of April 2021</t>
+    <t>2020 - 2021</t>
+  </si>
+  <si>
+    <t>As of January 2022</t>
+  </si>
+  <si>
+    <t>Annual 2000 to 2021</t>
+  </si>
+  <si>
+    <t>Annual 2001 to 2021</t>
   </si>
 </sst>
 </file>
@@ -666,17 +669,17 @@
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.90625" style="1" customWidth="1"/>
-    <col min="2" max="22" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="7.81640625" style="1"/>
+    <col min="2" max="23" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="7.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.25">
@@ -691,7 +694,7 @@
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.25">
@@ -701,7 +704,7 @@
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.25">
@@ -734,6 +737,7 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -802,6 +806,9 @@
       <c r="V10" s="6">
         <v>2020</v>
       </c>
+      <c r="W10" s="6">
+        <v>2021</v>
+      </c>
     </row>
     <row r="11" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -873,7 +880,9 @@
       <c r="V12" s="8">
         <v>5187261.9714157963</v>
       </c>
-      <c r="W12" s="9"/>
+      <c r="W12" s="8">
+        <v>5632103.4840306379</v>
+      </c>
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
@@ -1015,7 +1024,9 @@
       <c r="V13" s="8">
         <v>295851.8987867157</v>
       </c>
-      <c r="W13" s="9"/>
+      <c r="W13" s="8">
+        <v>299982.49492445076</v>
+      </c>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
@@ -1157,7 +1168,9 @@
       <c r="V14" s="8">
         <v>225114.20899515774</v>
       </c>
-      <c r="W14" s="9"/>
+      <c r="W14" s="8">
+        <v>257294.77539498347</v>
+      </c>
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
@@ -1299,7 +1312,9 @@
       <c r="V15" s="8">
         <v>1762575.5823902679</v>
       </c>
-      <c r="W15" s="9"/>
+      <c r="W15" s="8">
+        <v>1867530.4124389882</v>
+      </c>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -1441,7 +1456,9 @@
       <c r="V16" s="8">
         <v>391697.16867923428</v>
       </c>
-      <c r="W16" s="9"/>
+      <c r="W16" s="8">
+        <v>412757.46236997534</v>
+      </c>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
@@ -1583,7 +1600,9 @@
       <c r="V17" s="8">
         <v>579360.10760281922</v>
       </c>
-      <c r="W17" s="9"/>
+      <c r="W17" s="8">
+        <v>683353.34894295968</v>
+      </c>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
@@ -1725,7 +1744,9 @@
       <c r="V18" s="8">
         <v>1047014.8287783978</v>
       </c>
-      <c r="W18" s="9"/>
+      <c r="W18" s="8">
+        <v>1150802.966305272</v>
+      </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
@@ -1867,7 +1888,9 @@
       <c r="V19" s="8">
         <v>400195.43112914567</v>
       </c>
-      <c r="W19" s="9"/>
+      <c r="W19" s="8">
+        <v>437110.30860957375</v>
+      </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
@@ -2009,7 +2032,9 @@
       <c r="V20" s="8">
         <v>178195.76610595698</v>
       </c>
-      <c r="W20" s="9"/>
+      <c r="W20" s="8">
+        <v>184825.88143029207</v>
+      </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
@@ -2151,7 +2176,9 @@
       <c r="V21" s="8">
         <v>680164.75369730848</v>
       </c>
-      <c r="W21" s="9"/>
+      <c r="W21" s="8">
+        <v>745883.19731785997</v>
+      </c>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
@@ -2293,7 +2320,9 @@
       <c r="V22" s="8">
         <v>802777.8630523493</v>
       </c>
-      <c r="W22" s="9"/>
+      <c r="W22" s="8">
+        <v>875019.66109271836</v>
+      </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
@@ -2435,7 +2464,9 @@
       <c r="V23" s="8">
         <v>1928279.7309242343</v>
       </c>
-      <c r="W23" s="9"/>
+      <c r="W23" s="8">
+        <v>2062814.7003930295</v>
+      </c>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
@@ -2675,7 +2706,9 @@
       <c r="V25" s="12">
         <v>13478489.311557382</v>
       </c>
-      <c r="W25" s="9"/>
+      <c r="W25" s="12">
+        <v>14609478.693250742</v>
+      </c>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
@@ -2773,6 +2806,7 @@
       <c r="T26" s="13"/>
       <c r="U26" s="13"/>
       <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
@@ -2802,7 +2836,7 @@
       <c r="T28" s="15"/>
       <c r="U28" s="15"/>
       <c r="V28" s="15"/>
-      <c r="W28" s="9"/>
+      <c r="W28" s="15"/>
       <c r="X28" s="9"/>
       <c r="Y28" s="9"/>
       <c r="Z28" s="9"/>
@@ -2880,27 +2914,27 @@
     <row r="29" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="G29" s="16"/>
       <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
+      <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="17"/>
+      <c r="K29" s="16"/>
       <c r="L29" s="16"/>
-      <c r="M29" s="17"/>
+      <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="17"/>
+      <c r="O29" s="16"/>
       <c r="P29" s="16"/>
-      <c r="Q29" s="17"/>
+      <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
-      <c r="S29" s="17"/>
+      <c r="S29" s="16"/>
       <c r="T29" s="16"/>
       <c r="U29" s="16"/>
       <c r="V29" s="16"/>
-      <c r="W29" s="9"/>
+      <c r="W29" s="16"/>
       <c r="X29" s="9"/>
       <c r="Y29" s="9"/>
       <c r="Z29" s="9"/>
@@ -2987,7 +3021,7 @@
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.25">
@@ -2997,7 +3031,7 @@
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.25">
@@ -3030,6 +3064,7 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
+      <c r="W38" s="4"/>
     </row>
     <row r="39" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
@@ -3098,6 +3133,9 @@
       <c r="V39" s="18">
         <v>2020</v>
       </c>
+      <c r="W39" s="18">
+        <v>2021</v>
+      </c>
     </row>
     <row r="40" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -3169,7 +3207,9 @@
       <c r="V41" s="8">
         <v>4990476.0164997969</v>
       </c>
-      <c r="W41" s="11"/>
+      <c r="W41" s="8">
+        <v>5160173.8791846409</v>
+      </c>
       <c r="X41" s="11"/>
       <c r="Y41" s="11"/>
       <c r="Z41" s="9"/>
@@ -3311,7 +3351,9 @@
       <c r="V42" s="8">
         <v>227166.4378541495</v>
       </c>
-      <c r="W42" s="11"/>
+      <c r="W42" s="8">
+        <v>208961.2716971749</v>
+      </c>
       <c r="X42" s="11"/>
       <c r="Y42" s="11"/>
       <c r="Z42" s="9"/>
@@ -3453,7 +3495,9 @@
       <c r="V43" s="8">
         <v>217057.15162785241</v>
       </c>
-      <c r="W43" s="11"/>
+      <c r="W43" s="8">
+        <v>242898.28903540334</v>
+      </c>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
       <c r="Z43" s="9"/>
@@ -3595,7 +3639,9 @@
       <c r="V44" s="8">
         <v>1713596.9583538044</v>
       </c>
-      <c r="W44" s="11"/>
+      <c r="W44" s="8">
+        <v>1767793.3319551856</v>
+      </c>
       <c r="X44" s="11"/>
       <c r="Y44" s="11"/>
       <c r="Z44" s="9"/>
@@ -3737,7 +3783,9 @@
       <c r="V45" s="8">
         <v>367819.82440719137</v>
       </c>
-      <c r="W45" s="11"/>
+      <c r="W45" s="8">
+        <v>378436.6145325703</v>
+      </c>
       <c r="X45" s="11"/>
       <c r="Y45" s="11"/>
       <c r="Z45" s="9"/>
@@ -3879,7 +3927,9 @@
       <c r="V46" s="8">
         <v>547731.32275075302</v>
       </c>
-      <c r="W46" s="11"/>
+      <c r="W46" s="8">
+        <v>626548.71848102636</v>
+      </c>
       <c r="X46" s="11"/>
       <c r="Y46" s="11"/>
       <c r="Z46" s="9"/>
@@ -4021,7 +4071,9 @@
       <c r="V47" s="8">
         <v>1003155.32973727</v>
       </c>
-      <c r="W47" s="11"/>
+      <c r="W47" s="8">
+        <v>1004403.7526797585</v>
+      </c>
       <c r="X47" s="11"/>
       <c r="Y47" s="11"/>
       <c r="Z47" s="9"/>
@@ -4163,7 +4215,9 @@
       <c r="V48" s="8">
         <v>398847.72476703022</v>
       </c>
-      <c r="W48" s="11"/>
+      <c r="W48" s="8">
+        <v>434574.80500570603</v>
+      </c>
       <c r="X48" s="11"/>
       <c r="Y48" s="11"/>
       <c r="Z48" s="9"/>
@@ -4305,7 +4359,9 @@
       <c r="V49" s="8">
         <v>173506.74147744116</v>
       </c>
-      <c r="W49" s="11"/>
+      <c r="W49" s="8">
+        <v>180006.07552330429</v>
+      </c>
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
       <c r="Z49" s="9"/>
@@ -4447,7 +4503,9 @@
       <c r="V50" s="8">
         <v>663622.15162884607</v>
       </c>
-      <c r="W50" s="11"/>
+      <c r="W50" s="8">
+        <v>720464.2344993935</v>
+      </c>
       <c r="X50" s="11"/>
       <c r="Y50" s="11"/>
       <c r="Z50" s="9"/>
@@ -4589,7 +4647,9 @@
       <c r="V51" s="8">
         <v>760722.52207531454</v>
       </c>
-      <c r="W51" s="11"/>
+      <c r="W51" s="8">
+        <v>799755.89912864054</v>
+      </c>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
       <c r="Z51" s="9"/>
@@ -4731,7 +4791,9 @@
       <c r="V52" s="8">
         <v>1850006.4392533624</v>
       </c>
-      <c r="W52" s="11"/>
+      <c r="W52" s="8">
+        <v>1932441.0057125338</v>
+      </c>
       <c r="X52" s="11"/>
       <c r="Y52" s="11"/>
       <c r="Z52" s="9"/>
@@ -4971,7 +5033,9 @@
       <c r="V54" s="12">
         <v>12913708.620432809</v>
       </c>
-      <c r="W54" s="9"/>
+      <c r="W54" s="12">
+        <v>13456457.877435338</v>
+      </c>
       <c r="X54" s="9"/>
       <c r="Y54" s="9"/>
       <c r="Z54" s="9"/>
@@ -5069,6 +5133,7 @@
       <c r="T55" s="13"/>
       <c r="U55" s="13"/>
       <c r="V55" s="13"/>
+      <c r="W55" s="13"/>
     </row>
     <row r="56" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
@@ -5196,7 +5261,7 @@
       <c r="T58" s="17"/>
       <c r="U58" s="17"/>
       <c r="V58" s="17"/>
-      <c r="W58" s="9"/>
+      <c r="W58" s="17"/>
       <c r="X58" s="9"/>
       <c r="Y58" s="9"/>
       <c r="Z58" s="9"/>
@@ -5283,7 +5348,7 @@
     </row>
     <row r="61" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:96" x14ac:dyDescent="0.25">
@@ -5293,7 +5358,7 @@
     </row>
     <row r="64" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:91" x14ac:dyDescent="0.25">
@@ -5325,6 +5390,8 @@
       <c r="S67" s="4"/>
       <c r="T67" s="4"/>
       <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
     </row>
     <row r="68" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
@@ -5388,8 +5455,12 @@
         <v>49</v>
       </c>
       <c r="U68" s="18" t="s">
-        <v>54</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="V68" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W68" s="18"/>
     </row>
     <row r="69" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
@@ -5458,7 +5529,10 @@
       <c r="U70" s="19">
         <v>7.5498144820556945</v>
       </c>
-      <c r="W70" s="9"/>
+      <c r="V70" s="19">
+        <v>8.5756515685177135</v>
+      </c>
+      <c r="W70" s="19"/>
       <c r="X70" s="9"/>
       <c r="Y70" s="9"/>
       <c r="Z70" s="9"/>
@@ -5592,7 +5666,10 @@
       <c r="U71" s="19">
         <v>-13.838786359368001</v>
       </c>
-      <c r="W71" s="9"/>
+      <c r="V71" s="19">
+        <v>1.396170230671018</v>
+      </c>
+      <c r="W71" s="19"/>
       <c r="X71" s="9"/>
       <c r="Y71" s="9"/>
       <c r="Z71" s="9"/>
@@ -5726,7 +5803,10 @@
       <c r="U72" s="19">
         <v>-15.04970159191565</v>
       </c>
-      <c r="W72" s="9"/>
+      <c r="V72" s="19">
+        <v>14.295217766781647</v>
+      </c>
+      <c r="W72" s="19"/>
       <c r="X72" s="9"/>
       <c r="Y72" s="9"/>
       <c r="Z72" s="9"/>
@@ -5860,7 +5940,10 @@
       <c r="U73" s="19">
         <v>6.7523833936099038</v>
       </c>
-      <c r="W73" s="9"/>
+      <c r="V73" s="19">
+        <v>5.954628618330716</v>
+      </c>
+      <c r="W73" s="19"/>
       <c r="X73" s="9"/>
       <c r="Y73" s="9"/>
       <c r="Z73" s="9"/>
@@ -5994,7 +6077,10 @@
       <c r="U74" s="19">
         <v>-9.5908164811772849</v>
       </c>
-      <c r="W74" s="9"/>
+      <c r="V74" s="19">
+        <v>5.3766775393742137</v>
+      </c>
+      <c r="W74" s="19"/>
       <c r="X74" s="9"/>
       <c r="Y74" s="9"/>
       <c r="Z74" s="9"/>
@@ -6128,7 +6214,10 @@
       <c r="U75" s="19">
         <v>0.51654490153920563</v>
       </c>
-      <c r="W75" s="9"/>
+      <c r="V75" s="19">
+        <v>17.949672401578781</v>
+      </c>
+      <c r="W75" s="19"/>
       <c r="X75" s="9"/>
       <c r="Y75" s="9"/>
       <c r="Z75" s="9"/>
@@ -6262,7 +6351,10 @@
       <c r="U76" s="19">
         <v>-31.097464782956422</v>
       </c>
-      <c r="W76" s="9"/>
+      <c r="V76" s="19">
+        <v>9.9127667225084934</v>
+      </c>
+      <c r="W76" s="19"/>
       <c r="X76" s="9"/>
       <c r="Y76" s="9"/>
       <c r="Z76" s="9"/>
@@ -6396,7 +6488,10 @@
       <c r="U77" s="19">
         <v>6.4934075079146538</v>
       </c>
-      <c r="W77" s="9"/>
+      <c r="V77" s="19">
+        <v>9.224212624385359</v>
+      </c>
+      <c r="W77" s="19"/>
       <c r="X77" s="9"/>
       <c r="Y77" s="9"/>
       <c r="Z77" s="9"/>
@@ -6530,7 +6625,10 @@
       <c r="U78" s="19">
         <v>-43.69025979567126</v>
       </c>
-      <c r="W78" s="9"/>
+      <c r="V78" s="19">
+        <v>3.7206918375337636</v>
+      </c>
+      <c r="W78" s="19"/>
       <c r="X78" s="9"/>
       <c r="Y78" s="9"/>
       <c r="Z78" s="9"/>
@@ -6664,7 +6762,10 @@
       <c r="U79" s="19">
         <v>-9.6199626624786703</v>
       </c>
-      <c r="W79" s="9"/>
+      <c r="V79" s="19">
+        <v>9.6621360138573067</v>
+      </c>
+      <c r="W79" s="19"/>
       <c r="X79" s="9"/>
       <c r="Y79" s="9"/>
       <c r="Z79" s="9"/>
@@ -6798,7 +6899,10 @@
       <c r="U80" s="19">
         <v>-41.560620885590204</v>
       </c>
-      <c r="W80" s="9"/>
+      <c r="V80" s="19">
+        <v>8.998977346695753</v>
+      </c>
+      <c r="W80" s="19"/>
       <c r="X80" s="9"/>
       <c r="Y80" s="9"/>
       <c r="Z80" s="9"/>
@@ -6932,7 +7036,10 @@
       <c r="U81" s="19">
         <v>3.7792532319091947</v>
       </c>
-      <c r="W81" s="9"/>
+      <c r="V81" s="19">
+        <v>6.9769425727620842</v>
+      </c>
+      <c r="W81" s="19"/>
       <c r="X81" s="9"/>
       <c r="Y81" s="9"/>
       <c r="Z81" s="9"/>
@@ -7024,6 +7131,7 @@
       <c r="S82" s="9"/>
       <c r="T82" s="9"/>
       <c r="U82" s="9"/>
+      <c r="V82" s="9"/>
       <c r="W82" s="9"/>
       <c r="X82" s="9"/>
       <c r="Y82" s="9"/>
@@ -7158,7 +7266,10 @@
       <c r="U83" s="19">
         <v>-5.6678646172965017</v>
       </c>
-      <c r="W83" s="9"/>
+      <c r="V83" s="19">
+        <v>8.391069322016449</v>
+      </c>
+      <c r="W83" s="19"/>
       <c r="X83" s="9"/>
       <c r="Y83" s="9"/>
       <c r="Z83" s="9"/>
@@ -7250,6 +7361,8 @@
       <c r="S84" s="13"/>
       <c r="T84" s="13"/>
       <c r="U84" s="13"/>
+      <c r="V84" s="13"/>
+      <c r="W84" s="13"/>
     </row>
     <row r="85" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
@@ -7278,6 +7391,7 @@
       <c r="S86" s="9"/>
       <c r="T86" s="9"/>
       <c r="U86" s="9"/>
+      <c r="V86" s="9"/>
       <c r="W86" s="9"/>
       <c r="X86" s="9"/>
       <c r="Y86" s="9"/>
@@ -7370,6 +7484,7 @@
       <c r="S87" s="9"/>
       <c r="T87" s="9"/>
       <c r="U87" s="9"/>
+      <c r="V87" s="9"/>
       <c r="W87" s="9"/>
       <c r="X87" s="9"/>
       <c r="Y87" s="9"/>
@@ -7452,7 +7567,7 @@
     </row>
     <row r="90" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="92" spans="1:91" x14ac:dyDescent="0.25">
@@ -7462,7 +7577,7 @@
     </row>
     <row r="93" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:91" x14ac:dyDescent="0.25">
@@ -7494,6 +7609,8 @@
       <c r="S96" s="4"/>
       <c r="T96" s="4"/>
       <c r="U96" s="4"/>
+      <c r="V96" s="4"/>
+      <c r="W96" s="4"/>
     </row>
     <row r="97" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
@@ -7557,8 +7674,12 @@
         <v>49</v>
       </c>
       <c r="U97" s="18" t="s">
-        <v>54</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="V97" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W97" s="18"/>
     </row>
     <row r="98" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
@@ -7627,7 +7748,10 @@
       <c r="U99" s="19">
         <v>4.9545029080488234</v>
       </c>
-      <c r="W99" s="9"/>
+      <c r="V99" s="19">
+        <v>3.4004343899014771</v>
+      </c>
+      <c r="W99" s="19"/>
       <c r="X99" s="9"/>
       <c r="Y99" s="9"/>
       <c r="Z99" s="9"/>
@@ -7761,7 +7885,10 @@
       <c r="U100" s="19">
         <v>-25.580801619082678</v>
       </c>
-      <c r="W100" s="9"/>
+      <c r="V100" s="19">
+        <v>-8.0140210538772862</v>
+      </c>
+      <c r="W100" s="19"/>
       <c r="X100" s="9"/>
       <c r="Y100" s="9"/>
       <c r="Z100" s="9"/>
@@ -7895,7 +8022,10 @@
       <c r="U101" s="19">
         <v>-16.371864699764103</v>
       </c>
-      <c r="W101" s="9"/>
+      <c r="V101" s="19">
+        <v>11.905222755275034</v>
+      </c>
+      <c r="W101" s="19"/>
       <c r="X101" s="9"/>
       <c r="Y101" s="9"/>
       <c r="Z101" s="9"/>
@@ -8029,7 +8159,10 @@
       <c r="U102" s="19">
         <v>5.7621111064719344</v>
       </c>
-      <c r="W102" s="9"/>
+      <c r="V102" s="19">
+        <v>3.1627258286829516</v>
+      </c>
+      <c r="W102" s="19"/>
       <c r="X102" s="9"/>
       <c r="Y102" s="9"/>
       <c r="Z102" s="9"/>
@@ -8163,7 +8296,10 @@
       <c r="U103" s="19">
         <v>-12.851017258553398</v>
       </c>
-      <c r="W103" s="9"/>
+      <c r="V103" s="19">
+        <v>2.8864105251775953</v>
+      </c>
+      <c r="W103" s="19"/>
       <c r="X103" s="9"/>
       <c r="Y103" s="9"/>
       <c r="Z103" s="9"/>
@@ -8297,7 +8433,10 @@
       <c r="U104" s="19">
         <v>-2.1666201913902654</v>
       </c>
-      <c r="W104" s="9"/>
+      <c r="V104" s="19">
+        <v>14.389791574169195</v>
+      </c>
+      <c r="W104" s="19"/>
       <c r="X104" s="9"/>
       <c r="Y104" s="9"/>
       <c r="Z104" s="9"/>
@@ -8431,7 +8570,10 @@
       <c r="U105" s="19">
         <v>-33.492609599448215</v>
       </c>
-      <c r="W105" s="9"/>
+      <c r="V105" s="19">
+        <v>0.12444961467885207</v>
+      </c>
+      <c r="W105" s="19"/>
       <c r="X105" s="9"/>
       <c r="Y105" s="9"/>
       <c r="Z105" s="9"/>
@@ -8565,7 +8707,10 @@
       <c r="U106" s="19">
         <v>6.1070679110874835</v>
       </c>
-      <c r="W106" s="9"/>
+      <c r="V106" s="19">
+        <v>8.9575740364431766</v>
+      </c>
+      <c r="W106" s="19"/>
       <c r="X106" s="9"/>
       <c r="Y106" s="9"/>
       <c r="Z106" s="9"/>
@@ -8699,7 +8844,10 @@
       <c r="U107" s="19">
         <v>-44.129355147563786</v>
       </c>
-      <c r="W107" s="9"/>
+      <c r="V107" s="19">
+        <v>3.7458683106605122</v>
+      </c>
+      <c r="W107" s="19"/>
       <c r="X107" s="9"/>
       <c r="Y107" s="9"/>
       <c r="Z107" s="9"/>
@@ -8833,7 +8981,10 @@
       <c r="U108" s="19">
         <v>-11.661888427384952</v>
       </c>
-      <c r="W108" s="9"/>
+      <c r="V108" s="19">
+        <v>8.5654287957431592</v>
+      </c>
+      <c r="W108" s="19"/>
       <c r="X108" s="9"/>
       <c r="Y108" s="9"/>
       <c r="Z108" s="9"/>
@@ -8967,7 +9118,10 @@
       <c r="U109" s="19">
         <v>-43.060821179582796</v>
       </c>
-      <c r="W109" s="9"/>
+      <c r="V109" s="19">
+        <v>5.1310926021803169</v>
+      </c>
+      <c r="W109" s="19"/>
       <c r="X109" s="9"/>
       <c r="Y109" s="9"/>
       <c r="Z109" s="9"/>
@@ -9101,7 +9255,10 @@
       <c r="U110" s="19">
         <v>1.4499579376626315</v>
       </c>
-      <c r="W110" s="9"/>
+      <c r="V110" s="19">
+        <v>4.4559070017313473</v>
+      </c>
+      <c r="W110" s="19"/>
       <c r="X110" s="9"/>
       <c r="Y110" s="9"/>
       <c r="Z110" s="9"/>
@@ -9193,6 +9350,7 @@
       <c r="S111" s="9"/>
       <c r="T111" s="9"/>
       <c r="U111" s="9"/>
+      <c r="V111" s="9"/>
       <c r="W111" s="9"/>
       <c r="X111" s="9"/>
       <c r="Y111" s="9"/>
@@ -9327,7 +9485,10 @@
       <c r="U112" s="19">
         <v>-7.9397645330107736</v>
       </c>
-      <c r="W112" s="9"/>
+      <c r="V112" s="19">
+        <v>4.2028922361138115</v>
+      </c>
+      <c r="W112" s="19"/>
       <c r="X112" s="9"/>
       <c r="Y112" s="9"/>
       <c r="Z112" s="9"/>
@@ -9419,6 +9580,8 @@
       <c r="S113" s="13"/>
       <c r="T113" s="13"/>
       <c r="U113" s="13"/>
+      <c r="V113" s="13"/>
+      <c r="W113" s="13"/>
     </row>
     <row r="114" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
@@ -9447,6 +9610,7 @@
       <c r="S115" s="9"/>
       <c r="T115" s="9"/>
       <c r="U115" s="9"/>
+      <c r="V115" s="9"/>
       <c r="W115" s="9"/>
       <c r="X115" s="9"/>
       <c r="Y115" s="9"/>
@@ -9619,7 +9783,7 @@
     </row>
     <row r="118" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="120" spans="1:96" x14ac:dyDescent="0.25">
@@ -9629,7 +9793,7 @@
     </row>
     <row r="121" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:96" x14ac:dyDescent="0.25">
@@ -9662,6 +9826,7 @@
       <c r="T124" s="4"/>
       <c r="U124" s="4"/>
       <c r="V124" s="4"/>
+      <c r="W124" s="4"/>
     </row>
     <row r="125" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
@@ -9730,6 +9895,9 @@
       <c r="V125" s="18">
         <v>2020</v>
       </c>
+      <c r="W125" s="18">
+        <v>2021</v>
+      </c>
     </row>
     <row r="126" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
@@ -9801,7 +9969,9 @@
       <c r="V127" s="19">
         <v>103.94323015009739</v>
       </c>
-      <c r="W127" s="9"/>
+      <c r="W127" s="19">
+        <v>109.14561439004389</v>
+      </c>
       <c r="X127" s="9"/>
       <c r="Y127" s="9"/>
       <c r="Z127" s="9"/>
@@ -9943,7 +10113,9 @@
       <c r="V128" s="19">
         <v>130.23574326444526</v>
       </c>
-      <c r="W128" s="9"/>
+      <c r="W128" s="19">
+        <v>143.55889609974383</v>
+      </c>
       <c r="X128" s="9"/>
       <c r="Y128" s="9"/>
       <c r="Z128" s="9"/>
@@ -10085,7 +10257,9 @@
       <c r="V129" s="19">
         <v>103.71195203976475</v>
       </c>
-      <c r="W129" s="9"/>
+      <c r="W129" s="19">
+        <v>105.92696079365211</v>
+      </c>
       <c r="X129" s="9"/>
       <c r="Y129" s="9"/>
       <c r="Z129" s="9"/>
@@ -10227,7 +10401,9 @@
       <c r="V130" s="19">
         <v>102.85823476738167</v>
       </c>
-      <c r="W130" s="9"/>
+      <c r="W130" s="19">
+        <v>105.64189708609733</v>
+      </c>
       <c r="X130" s="9"/>
       <c r="Y130" s="9"/>
       <c r="Z130" s="9"/>
@@ -10369,7 +10545,9 @@
       <c r="V131" s="19">
         <v>106.49158709988664</v>
       </c>
-      <c r="W131" s="9"/>
+      <c r="W131" s="19">
+        <v>109.06911395975698</v>
+      </c>
       <c r="X131" s="9"/>
       <c r="Y131" s="9"/>
       <c r="Z131" s="9"/>
@@ -10511,7 +10689,9 @@
       <c r="V132" s="19">
         <v>105.77450723344135</v>
       </c>
-      <c r="W132" s="9"/>
+      <c r="W132" s="19">
+        <v>109.0662751014235</v>
+      </c>
       <c r="X132" s="9"/>
       <c r="Y132" s="9"/>
       <c r="Z132" s="9"/>
@@ -10653,7 +10833,9 @@
       <c r="V133" s="19">
         <v>104.37215431558488</v>
       </c>
-      <c r="W133" s="9"/>
+      <c r="W133" s="19">
+        <v>114.57573343736709</v>
+      </c>
       <c r="X133" s="9"/>
       <c r="Y133" s="9"/>
       <c r="Z133" s="9"/>
@@ -10795,7 +10977,9 @@
       <c r="V134" s="19">
         <v>100.33789997495978</v>
       </c>
-      <c r="W134" s="9"/>
+      <c r="W134" s="19">
+        <v>100.58344468539413</v>
+      </c>
       <c r="X134" s="9"/>
       <c r="Y134" s="9"/>
       <c r="Z134" s="9"/>
@@ -10937,7 +11121,9 @@
       <c r="V135" s="19">
         <v>102.70250284720233</v>
       </c>
-      <c r="W135" s="9"/>
+      <c r="W135" s="19">
+        <v>102.67757957223161</v>
+      </c>
       <c r="X135" s="9"/>
       <c r="Y135" s="9"/>
       <c r="Z135" s="9"/>
@@ -11079,7 +11265,9 @@
       <c r="V136" s="19">
         <v>102.49277424327367</v>
       </c>
-      <c r="W136" s="9"/>
+      <c r="W136" s="19">
+        <v>103.5281366654</v>
+      </c>
       <c r="X136" s="9"/>
       <c r="Y136" s="9"/>
       <c r="Z136" s="9"/>
@@ -11221,7 +11409,9 @@
       <c r="V137" s="19">
         <v>105.52834177464658</v>
       </c>
-      <c r="W137" s="9"/>
+      <c r="W137" s="19">
+        <v>109.41084173884556</v>
+      </c>
       <c r="X137" s="9"/>
       <c r="Y137" s="9"/>
       <c r="Z137" s="9"/>
@@ -11363,7 +11553,9 @@
       <c r="V138" s="19">
         <v>104.23097401231003</v>
       </c>
-      <c r="W138" s="9"/>
+      <c r="W138" s="19">
+        <v>106.74658084231783</v>
+      </c>
       <c r="X138" s="9"/>
       <c r="Y138" s="9"/>
       <c r="Z138" s="9"/>
@@ -11603,7 +11795,9 @@
       <c r="V140" s="19">
         <v>104.37349724796287</v>
       </c>
-      <c r="W140" s="9"/>
+      <c r="W140" s="19">
+        <v>108.56853137963493</v>
+      </c>
       <c r="X140" s="9"/>
       <c r="Y140" s="9"/>
       <c r="Z140" s="9"/>
@@ -11701,6 +11895,7 @@
       <c r="T141" s="13"/>
       <c r="U141" s="13"/>
       <c r="V141" s="13"/>
+      <c r="W141" s="13"/>
     </row>
     <row r="142" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A142" s="14" t="s">
@@ -11719,7 +11914,7 @@
     </row>
     <row r="147" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="149" spans="1:96" x14ac:dyDescent="0.25">
@@ -11729,7 +11924,7 @@
     </row>
     <row r="150" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="151" spans="1:96" x14ac:dyDescent="0.25">
@@ -11762,6 +11957,7 @@
       <c r="T153" s="4"/>
       <c r="U153" s="4"/>
       <c r="V153" s="4"/>
+      <c r="W153" s="4"/>
     </row>
     <row r="154" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
@@ -11830,6 +12026,9 @@
       <c r="V154" s="18">
         <v>2020</v>
       </c>
+      <c r="W154" s="18">
+        <v>2021</v>
+      </c>
     </row>
     <row r="155" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
@@ -11901,7 +12100,9 @@
       <c r="V156" s="19">
         <v>38.485484919796477</v>
       </c>
-      <c r="W156" s="9"/>
+      <c r="W156" s="19">
+        <v>38.551022950822642</v>
+      </c>
       <c r="X156" s="9"/>
       <c r="Y156" s="9"/>
       <c r="Z156" s="9"/>
@@ -12043,7 +12244,9 @@
       <c r="V157" s="19">
         <v>2.1949930140392806</v>
       </c>
-      <c r="W157" s="9"/>
+      <c r="W157" s="19">
+        <v>2.0533415409479057</v>
+      </c>
       <c r="X157" s="9"/>
       <c r="Y157" s="9"/>
       <c r="Z157" s="9"/>
@@ -12185,7 +12388,9 @@
       <c r="V158" s="19">
         <v>1.6701738881235699</v>
       </c>
-      <c r="W158" s="9"/>
+      <c r="W158" s="19">
+        <v>1.7611495988138715</v>
+      </c>
       <c r="X158" s="9"/>
       <c r="Y158" s="9"/>
       <c r="Z158" s="9"/>
@@ -12327,7 +12532,9 @@
       <c r="V159" s="19">
         <v>13.076952035558723</v>
       </c>
-      <c r="W159" s="9"/>
+      <c r="W159" s="19">
+        <v>12.783005141050968</v>
+      </c>
       <c r="X159" s="9"/>
       <c r="Y159" s="9"/>
       <c r="Z159" s="9"/>
@@ -12469,7 +12676,9 @@
       <c r="V160" s="19">
         <v>2.9060910286389903</v>
       </c>
-      <c r="W160" s="9"/>
+      <c r="W160" s="19">
+        <v>2.8252716680483623</v>
+      </c>
       <c r="X160" s="9"/>
       <c r="Y160" s="9"/>
       <c r="Z160" s="9"/>
@@ -12611,7 +12820,9 @@
       <c r="V161" s="19">
         <v>4.298405364361094</v>
       </c>
-      <c r="W161" s="9"/>
+      <c r="W161" s="19">
+        <v>4.677465659734005</v>
+      </c>
       <c r="X161" s="9"/>
       <c r="Y161" s="9"/>
       <c r="Z161" s="9"/>
@@ -12753,7 +12964,9 @@
       <c r="V162" s="19">
         <v>7.7680428761449942</v>
       </c>
-      <c r="W162" s="9"/>
+      <c r="W162" s="19">
+        <v>7.8770980845258878</v>
+      </c>
       <c r="X162" s="9"/>
       <c r="Y162" s="9"/>
       <c r="Z162" s="9"/>
@@ -12895,7 +13108,9 @@
       <c r="V163" s="19">
         <v>2.9691415846284093</v>
       </c>
-      <c r="W163" s="9"/>
+      <c r="W163" s="19">
+        <v>2.9919637639877537</v>
+      </c>
       <c r="X163" s="9"/>
       <c r="Y163" s="9"/>
       <c r="Z163" s="9"/>
@@ -13037,7 +13252,9 @@
       <c r="V164" s="19">
         <v>1.3220752117461687</v>
       </c>
-      <c r="W164" s="9"/>
+      <c r="W164" s="19">
+        <v>1.2651093533931335</v>
+      </c>
       <c r="X164" s="9"/>
       <c r="Y164" s="9"/>
       <c r="Z164" s="9"/>
@@ -13179,7 +13396,9 @@
       <c r="V165" s="19">
         <v>5.0462981271505596</v>
       </c>
-      <c r="W165" s="9"/>
+      <c r="W165" s="19">
+        <v>5.1054744182107026</v>
+      </c>
       <c r="X165" s="9"/>
       <c r="Y165" s="9"/>
       <c r="Z165" s="9"/>
@@ -13321,7 +13540,9 @@
       <c r="V166" s="19">
         <v>5.9559928749877953</v>
       </c>
-      <c r="W166" s="9"/>
+      <c r="W166" s="19">
+        <v>5.9893968803757396</v>
+      </c>
       <c r="X166" s="9"/>
       <c r="Y166" s="9"/>
       <c r="Z166" s="9"/>
@@ -13463,7 +13684,9 @@
       <c r="V167" s="19">
         <v>14.306349074823949</v>
       </c>
-      <c r="W167" s="9"/>
+      <c r="W167" s="19">
+        <v>14.119700940089016</v>
+      </c>
       <c r="X167" s="9"/>
       <c r="Y167" s="9"/>
       <c r="Z167" s="9"/>
@@ -13703,7 +13926,9 @@
       <c r="V169" s="19">
         <v>100</v>
       </c>
-      <c r="W169" s="9"/>
+      <c r="W169" s="19">
+        <v>100</v>
+      </c>
       <c r="X169" s="9"/>
       <c r="Y169" s="9"/>
       <c r="Z169" s="9"/>
@@ -13801,6 +14026,7 @@
       <c r="T170" s="13"/>
       <c r="U170" s="13"/>
       <c r="V170" s="13"/>
+      <c r="W170" s="13"/>
     </row>
     <row r="171" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A171" s="14" t="s">
@@ -14015,7 +14241,7 @@
     </row>
     <row r="176" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="178" spans="1:96" x14ac:dyDescent="0.25">
@@ -14025,7 +14251,7 @@
     </row>
     <row r="179" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="180" spans="1:96" x14ac:dyDescent="0.25">
@@ -14058,6 +14284,7 @@
       <c r="T182" s="4"/>
       <c r="U182" s="4"/>
       <c r="V182" s="4"/>
+      <c r="W182" s="4"/>
     </row>
     <row r="183" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
@@ -14126,6 +14353,9 @@
       <c r="V183" s="18">
         <v>2020</v>
       </c>
+      <c r="W183" s="18">
+        <v>2021</v>
+      </c>
     </row>
     <row r="184" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
@@ -14197,7 +14427,9 @@
       <c r="V185" s="19">
         <v>38.644793398881404</v>
       </c>
-      <c r="W185" s="9"/>
+      <c r="W185" s="19">
+        <v>38.347193044297015</v>
+      </c>
       <c r="X185" s="9"/>
       <c r="Y185" s="9"/>
       <c r="Z185" s="9"/>
@@ -14339,7 +14571,9 @@
       <c r="V186" s="19">
         <v>1.7591107599772986</v>
       </c>
-      <c r="W186" s="9"/>
+      <c r="W186" s="19">
+        <v>1.5528698086854991</v>
+      </c>
       <c r="X186" s="9"/>
       <c r="Y186" s="9"/>
       <c r="Z186" s="9"/>
@@ -14481,7 +14715,9 @@
       <c r="V187" s="19">
         <v>1.6808273905484605</v>
       </c>
-      <c r="W187" s="9"/>
+      <c r="W187" s="19">
+        <v>1.8050685495973717</v>
+      </c>
       <c r="X187" s="9"/>
       <c r="Y187" s="9"/>
       <c r="Z187" s="9"/>
@@ -14623,7 +14859,9 @@
       <c r="V188" s="19">
         <v>13.269595967516668</v>
       </c>
-      <c r="W188" s="9"/>
+      <c r="W188" s="19">
+        <v>13.1371371876364</v>
+      </c>
       <c r="X188" s="9"/>
       <c r="Y188" s="9"/>
       <c r="Z188" s="9"/>
@@ -14765,7 +15003,9 @@
       <c r="V189" s="19">
         <v>2.8482896371473476</v>
       </c>
-      <c r="W189" s="9"/>
+      <c r="W189" s="19">
+        <v>2.8123048277597431</v>
+      </c>
       <c r="X189" s="9"/>
       <c r="Y189" s="9"/>
       <c r="Z189" s="9"/>
@@ -14907,7 +15147,9 @@
       <c r="V190" s="19">
         <v>4.2414719028436281</v>
       </c>
-      <c r="W190" s="9"/>
+      <c r="W190" s="19">
+        <v>4.6561191971006268</v>
+      </c>
       <c r="X190" s="9"/>
       <c r="Y190" s="9"/>
       <c r="Z190" s="9"/>
@@ -15049,7 +15291,9 @@
       <c r="V191" s="19">
         <v>7.7681428257566552</v>
       </c>
-      <c r="W191" s="9"/>
+      <c r="W191" s="19">
+        <v>7.4641020826439615</v>
+      </c>
       <c r="X191" s="9"/>
       <c r="Y191" s="9"/>
       <c r="Z191" s="9"/>
@@ -15191,7 +15435,9 @@
       <c r="V192" s="19">
         <v>3.0885606644085999</v>
       </c>
-      <c r="W192" s="9"/>
+      <c r="W192" s="19">
+        <v>3.2294888369875498</v>
+      </c>
       <c r="X192" s="9"/>
       <c r="Y192" s="9"/>
       <c r="Z192" s="9"/>
@@ -15333,7 +15579,9 @@
       <c r="V193" s="19">
         <v>1.343585693136276</v>
       </c>
-      <c r="W193" s="9"/>
+      <c r="W193" s="19">
+        <v>1.3376928547084457</v>
+      </c>
       <c r="X193" s="9"/>
       <c r="Y193" s="9"/>
       <c r="Z193" s="9"/>
@@ -15475,7 +15723,9 @@
       <c r="V194" s="19">
         <v>5.1388967424805072</v>
       </c>
-      <c r="W194" s="9"/>
+      <c r="W194" s="19">
+        <v>5.3540407220202777</v>
+      </c>
       <c r="X194" s="9"/>
       <c r="Y194" s="9"/>
       <c r="Z194" s="9"/>
@@ -15617,7 +15867,9 @@
       <c r="V195" s="19">
         <v>5.8908137424725213</v>
       </c>
-      <c r="W195" s="9"/>
+      <c r="W195" s="19">
+        <v>5.9432869066511413</v>
+      </c>
       <c r="X195" s="9"/>
       <c r="Y195" s="9"/>
       <c r="Z195" s="9"/>
@@ -15759,7 +16011,9 @@
       <c r="V196" s="19">
         <v>14.325911274830657</v>
       </c>
-      <c r="W196" s="9"/>
+      <c r="W196" s="19">
+        <v>14.360695981911975</v>
+      </c>
       <c r="X196" s="9"/>
       <c r="Y196" s="9"/>
       <c r="Z196" s="9"/>
@@ -15999,7 +16253,9 @@
       <c r="V198" s="19">
         <v>100</v>
       </c>
-      <c r="W198" s="9"/>
+      <c r="W198" s="19">
+        <v>100</v>
+      </c>
       <c r="X198" s="9"/>
       <c r="Y198" s="9"/>
       <c r="Z198" s="9"/>
@@ -16097,6 +16353,7 @@
       <c r="T199" s="13"/>
       <c r="U199" s="13"/>
       <c r="V199" s="13"/>
+      <c r="W199" s="13"/>
     </row>
     <row r="200" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A200" s="14" t="s">
@@ -16292,9 +16549,9 @@
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="21" man="1"/>
-    <brk id="116" max="21" man="1"/>
-    <brk id="144" max="21" man="1"/>
+    <brk id="58" max="22" man="1"/>
+    <brk id="116" max="22" man="1"/>
+    <brk id="144" max="22" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q1 2022 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2022\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\0. IAD activities\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2022\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAABAA97-71B7-4010-9671-8449A2DF7CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10788"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -207,19 +208,19 @@
     <t>2020 - 2021</t>
   </si>
   <si>
-    <t>As of January 2022</t>
-  </si>
-  <si>
     <t>Annual 2000 to 2021</t>
   </si>
   <si>
     <t>Annual 2001 to 2021</t>
   </si>
+  <si>
+    <t>As of April 2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -336,9 +337,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -662,17 +663,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr transitionEvaluation="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -694,7 +695,7 @@
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.25">
@@ -704,7 +705,7 @@
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.25">
@@ -878,10 +879,10 @@
         <v>4823124.9829643108</v>
       </c>
       <c r="V12" s="8">
-        <v>5187261.9714157963</v>
+        <v>5185183.1888882155</v>
       </c>
       <c r="W12" s="8">
-        <v>5632103.4840306379</v>
+        <v>5634346.1664808691</v>
       </c>
       <c r="X12" s="9"/>
       <c r="Y12" s="9"/>
@@ -1022,10 +1023,10 @@
         <v>343370.16191610089</v>
       </c>
       <c r="V13" s="8">
-        <v>295851.8987867157</v>
+        <v>296341.10849450284</v>
       </c>
       <c r="W13" s="8">
-        <v>299982.49492445076</v>
+        <v>302235.82338753087</v>
       </c>
       <c r="X13" s="9"/>
       <c r="Y13" s="9"/>
@@ -1166,10 +1167,10 @@
         <v>264995.1950889611</v>
       </c>
       <c r="V14" s="8">
-        <v>225114.20899515774</v>
+        <v>223790.22761478901</v>
       </c>
       <c r="W14" s="8">
-        <v>257294.77539498347</v>
+        <v>259218.6021169934</v>
       </c>
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
@@ -1310,10 +1311,10 @@
         <v>1651087.8037180891</v>
       </c>
       <c r="V15" s="8">
-        <v>1762575.5823902679</v>
+        <v>1762774.3264463176</v>
       </c>
       <c r="W15" s="8">
-        <v>1867530.4124389882</v>
+        <v>1868331.6070618217</v>
       </c>
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
@@ -1454,10 +1455,10 @@
         <v>433249.3154278791</v>
       </c>
       <c r="V16" s="8">
-        <v>391697.16867923428</v>
+        <v>391353.62540668785</v>
       </c>
       <c r="W16" s="8">
-        <v>412757.46236997534</v>
+        <v>414203.73360744608</v>
       </c>
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
@@ -1598,10 +1599,10 @@
         <v>576382.83147349558</v>
       </c>
       <c r="V17" s="8">
-        <v>579360.10760281922</v>
+        <v>578101.21421777958</v>
       </c>
       <c r="W17" s="8">
-        <v>683353.34894295968</v>
+        <v>678637.19846265065</v>
       </c>
       <c r="X17" s="9"/>
       <c r="Y17" s="9"/>
@@ -1742,10 +1743,10 @@
         <v>1519559.2230101433</v>
       </c>
       <c r="V18" s="8">
-        <v>1047014.8287783978</v>
+        <v>1048819.36805525</v>
       </c>
       <c r="W18" s="8">
-        <v>1150802.966305272</v>
+        <v>1152774.4022722465</v>
       </c>
       <c r="X18" s="9"/>
       <c r="Y18" s="9"/>
@@ -1886,10 +1887,10 @@
         <v>375793.61999417935</v>
       </c>
       <c r="V19" s="8">
-        <v>400195.43112914567</v>
+        <v>399933.10936427652</v>
       </c>
       <c r="W19" s="8">
-        <v>437110.30860957375</v>
+        <v>437321.43397174275</v>
       </c>
       <c r="X19" s="9"/>
       <c r="Y19" s="9"/>
@@ -2030,10 +2031,10 @@
         <v>316456.38118617784</v>
       </c>
       <c r="V20" s="8">
-        <v>178195.76610595698</v>
+        <v>179132.86171854523</v>
       </c>
       <c r="W20" s="8">
-        <v>184825.88143029207</v>
+        <v>183997.94027457573</v>
       </c>
       <c r="X20" s="9"/>
       <c r="Y20" s="9"/>
@@ -2174,10 +2175,10 @@
         <v>752560.82397626725</v>
       </c>
       <c r="V21" s="8">
-        <v>680164.75369730848</v>
+        <v>683780.56383788679</v>
       </c>
       <c r="W21" s="8">
-        <v>745883.19731785997</v>
+        <v>752093.81384420488</v>
       </c>
       <c r="X21" s="9"/>
       <c r="Y21" s="9"/>
@@ -2318,10 +2319,10 @@
         <v>1373693.3472217587</v>
       </c>
       <c r="V22" s="8">
-        <v>802777.8630523493</v>
+        <v>800801.04835374421</v>
       </c>
       <c r="W22" s="8">
-        <v>875019.66109271836</v>
+        <v>869606.76566889707</v>
       </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
@@ -2462,10 +2463,10 @@
         <v>1858058.9769857223</v>
       </c>
       <c r="V23" s="8">
-        <v>1928279.7309242343</v>
+        <v>1926064.7495240266</v>
       </c>
       <c r="W23" s="8">
-        <v>2062814.7003930295</v>
+        <v>2057381.6883361312</v>
       </c>
       <c r="X23" s="9"/>
       <c r="Y23" s="9"/>
@@ -2704,10 +2705,10 @@
         <v>14288332.662963087</v>
       </c>
       <c r="V25" s="12">
-        <v>13478489.311557382</v>
+        <v>13476075.391922025</v>
       </c>
       <c r="W25" s="12">
-        <v>14609478.693250742</v>
+        <v>14610149.175485112</v>
       </c>
       <c r="X25" s="9"/>
       <c r="Y25" s="9"/>
@@ -3021,7 +3022,7 @@
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.25">
@@ -3031,7 +3032,7 @@
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.25">
@@ -3205,10 +3206,10 @@
         <v>4754894.624075328</v>
       </c>
       <c r="V41" s="8">
-        <v>4990476.0164997969</v>
+        <v>4988487.6893982869</v>
       </c>
       <c r="W41" s="8">
-        <v>5160173.8791846409</v>
+        <v>5162218.5407364136</v>
       </c>
       <c r="X41" s="11"/>
       <c r="Y41" s="11"/>
@@ -3349,10 +3350,10 @@
         <v>305252.46548799134</v>
       </c>
       <c r="V42" s="8">
-        <v>227166.4378541495</v>
+        <v>227535.55311407984</v>
       </c>
       <c r="W42" s="8">
-        <v>208961.2716971749</v>
+        <v>210446.92231700796</v>
       </c>
       <c r="X42" s="11"/>
       <c r="Y42" s="11"/>
@@ -3493,10 +3494,10 @@
         <v>259550.39036633901</v>
       </c>
       <c r="V43" s="8">
-        <v>217057.15162785241</v>
+        <v>215763.31724636882</v>
       </c>
       <c r="W43" s="8">
-        <v>242898.28903540334</v>
+        <v>244612.98470551503</v>
       </c>
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
@@ -3637,10 +3638,10 @@
         <v>1620237.0966561991</v>
       </c>
       <c r="V44" s="8">
-        <v>1713596.9583538044</v>
+        <v>1713781.8027433495</v>
       </c>
       <c r="W44" s="8">
-        <v>1767793.3319551856</v>
+        <v>1768542.564013296</v>
       </c>
       <c r="X44" s="11"/>
       <c r="Y44" s="11"/>
@@ -3781,10 +3782,10 @@
         <v>422058.6550028224</v>
       </c>
       <c r="V45" s="8">
-        <v>367819.82440719137</v>
+        <v>367491.58253879054</v>
       </c>
       <c r="W45" s="8">
-        <v>378436.6145325703</v>
+        <v>379738.97216163675</v>
       </c>
       <c r="X45" s="11"/>
       <c r="Y45" s="11"/>
@@ -3925,10 +3926,10 @@
         <v>559861.39272942755</v>
       </c>
       <c r="V46" s="8">
-        <v>547731.32275075302</v>
+        <v>546536.12766820076</v>
       </c>
       <c r="W46" s="8">
-        <v>626548.71848102636</v>
+        <v>622266.79420143808</v>
       </c>
       <c r="X46" s="11"/>
       <c r="Y46" s="11"/>
@@ -4069,10 +4070,10 @@
         <v>1508336.627998183</v>
       </c>
       <c r="V47" s="8">
-        <v>1003155.32973727</v>
+        <v>1004873.0160331208</v>
       </c>
       <c r="W47" s="8">
-        <v>1004403.7526797585</v>
+        <v>1006139.3356681818</v>
       </c>
       <c r="X47" s="11"/>
       <c r="Y47" s="11"/>
@@ -4213,10 +4214,10 @@
         <v>375891.75972824451</v>
       </c>
       <c r="V48" s="8">
-        <v>398847.72476703022</v>
+        <v>398567.82879521081</v>
       </c>
       <c r="W48" s="8">
-        <v>434574.80500570603</v>
+        <v>434764.13408027322</v>
       </c>
       <c r="X48" s="11"/>
       <c r="Y48" s="11"/>
@@ -4357,10 +4358,10 @@
         <v>310550.81239119702</v>
       </c>
       <c r="V49" s="8">
-        <v>173506.74147744116</v>
+        <v>174422.40301803884</v>
       </c>
       <c r="W49" s="8">
-        <v>180006.07552330429</v>
+        <v>179203.54632360791</v>
       </c>
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
@@ -4501,10 +4502,10 @@
         <v>751229.72385858651</v>
       </c>
       <c r="V50" s="8">
-        <v>663622.15162884607</v>
+        <v>667131.28156042565</v>
       </c>
       <c r="W50" s="8">
-        <v>720464.2344993935</v>
+        <v>726545.81311060337</v>
       </c>
       <c r="X50" s="11"/>
       <c r="Y50" s="11"/>
@@ -4645,10 +4646,10 @@
         <v>1336026.5072922606</v>
       </c>
       <c r="V51" s="8">
-        <v>760722.52207531454</v>
+        <v>758838.55098614178</v>
       </c>
       <c r="W51" s="8">
-        <v>799755.89912864054</v>
+        <v>794633.07511604822</v>
       </c>
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
@@ -4789,10 +4790,10 @@
         <v>1823565.5064441971</v>
       </c>
       <c r="V52" s="8">
-        <v>1850006.4392533624</v>
+        <v>1847927.8003300345</v>
       </c>
       <c r="W52" s="8">
-        <v>1932441.0057125338</v>
+        <v>1927418.831095702</v>
       </c>
       <c r="X52" s="11"/>
       <c r="Y52" s="11"/>
@@ -5031,10 +5032,10 @@
         <v>14027455.562030775</v>
       </c>
       <c r="V54" s="12">
-        <v>12913708.620432809</v>
+        <v>12911356.95343205</v>
       </c>
       <c r="W54" s="12">
-        <v>13456457.877435338</v>
+        <v>13456531.513529725</v>
       </c>
       <c r="X54" s="9"/>
       <c r="Y54" s="9"/>
@@ -5348,7 +5349,7 @@
     </row>
     <row r="61" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:96" x14ac:dyDescent="0.25">
@@ -5358,7 +5359,7 @@
     </row>
     <row r="64" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:91" x14ac:dyDescent="0.25">
@@ -5527,10 +5528,10 @@
         <v>6.6142485814555414</v>
       </c>
       <c r="U70" s="19">
-        <v>7.5498144820556945</v>
+        <v>7.506714157371519</v>
       </c>
       <c r="V70" s="19">
-        <v>8.5756515685177135</v>
+        <v>8.6624321886101114</v>
       </c>
       <c r="W70" s="19"/>
       <c r="X70" s="9"/>
@@ -5664,10 +5665,10 @@
         <v>9.4019889874057867</v>
       </c>
       <c r="U71" s="19">
-        <v>-13.838786359368001</v>
+        <v>-13.696313377715427</v>
       </c>
       <c r="V71" s="19">
-        <v>1.396170230671018</v>
+        <v>1.9891654326916921</v>
       </c>
       <c r="W71" s="19"/>
       <c r="X71" s="9"/>
@@ -5801,10 +5802,10 @@
         <v>6.0239524300981628</v>
       </c>
       <c r="U72" s="19">
-        <v>-15.04970159191565</v>
+        <v>-15.549326266213711</v>
       </c>
       <c r="V72" s="19">
-        <v>14.295217766781647</v>
+        <v>15.831064153161961</v>
       </c>
       <c r="W72" s="19"/>
       <c r="X72" s="9"/>
@@ -5938,10 +5939,10 @@
         <v>8.2588997123142178</v>
       </c>
       <c r="U73" s="19">
-        <v>6.7523833936099038</v>
+        <v>6.7644205521184944</v>
       </c>
       <c r="V73" s="19">
-        <v>5.954628618330716</v>
+        <v>5.9881335365431312</v>
       </c>
       <c r="W73" s="19"/>
       <c r="X73" s="9"/>
@@ -6075,10 +6076,10 @@
         <v>7.6588443214021993</v>
       </c>
       <c r="U74" s="19">
-        <v>-9.5908164811772849</v>
+        <v>-9.6701110721467387</v>
       </c>
       <c r="V74" s="19">
-        <v>5.3766775393742137</v>
+        <v>5.8387368143102805</v>
       </c>
       <c r="W74" s="19"/>
       <c r="X74" s="9"/>
@@ -6212,10 +6213,10 @@
         <v>9.2617138932869665</v>
       </c>
       <c r="U75" s="19">
-        <v>0.51654490153920563</v>
+        <v>0.29813218757593063</v>
       </c>
       <c r="V75" s="19">
-        <v>17.949672401578781</v>
+        <v>17.390723591699214</v>
       </c>
       <c r="W75" s="19"/>
       <c r="X75" s="9"/>
@@ -6349,10 +6350,10 @@
         <v>5.912782587866559</v>
       </c>
       <c r="U76" s="19">
-        <v>-31.097464782956422</v>
+        <v>-30.978710656790966</v>
       </c>
       <c r="V76" s="19">
-        <v>9.9127667225084934</v>
+        <v>9.9116241922336883</v>
       </c>
       <c r="W76" s="19"/>
       <c r="X76" s="9"/>
@@ -6486,10 +6487,10 @@
         <v>6.968021805468581</v>
       </c>
       <c r="U77" s="19">
-        <v>6.4934075079146538</v>
+        <v>6.4236027664522624</v>
       </c>
       <c r="V77" s="19">
-        <v>9.224212624385359</v>
+        <v>9.3486444937999096</v>
       </c>
       <c r="W77" s="19"/>
       <c r="X77" s="9"/>
@@ -6623,10 +6624,10 @@
         <v>9.2223247268291288</v>
       </c>
       <c r="U78" s="19">
-        <v>-43.69025979567126</v>
+        <v>-43.394138223062825</v>
       </c>
       <c r="V78" s="19">
-        <v>3.7206918375337636</v>
+        <v>2.7159051161001173</v>
       </c>
       <c r="W78" s="19"/>
       <c r="X78" s="9"/>
@@ -6760,10 +6761,10 @@
         <v>8.0439744736823258</v>
       </c>
       <c r="U79" s="19">
-        <v>-9.6199626624786703</v>
+        <v>-9.1394951673101588</v>
       </c>
       <c r="V79" s="19">
-        <v>9.6621360138573067</v>
+        <v>9.9905223428541348</v>
       </c>
       <c r="W79" s="19"/>
       <c r="X79" s="9"/>
@@ -6897,10 +6898,10 @@
         <v>9.6352422840770799</v>
       </c>
       <c r="U80" s="19">
-        <v>-41.560620885590204</v>
+        <v>-41.704525979300023</v>
       </c>
       <c r="V80" s="19">
-        <v>8.998977346695753</v>
+        <v>8.592111293635412</v>
       </c>
       <c r="W80" s="19"/>
       <c r="X80" s="9"/>
@@ -7034,10 +7035,10 @@
         <v>10.465668548462489</v>
       </c>
       <c r="U81" s="19">
-        <v>3.7792532319091947</v>
+        <v>3.6600438081157307</v>
       </c>
       <c r="V81" s="19">
-        <v>6.9769425727620842</v>
+        <v>6.8178880717564567</v>
       </c>
       <c r="W81" s="19"/>
       <c r="X81" s="9"/>
@@ -7264,10 +7265,10 @@
         <v>7.8357857803208475</v>
       </c>
       <c r="U83" s="19">
-        <v>-5.6678646172965017</v>
+        <v>-5.6847589582409483</v>
       </c>
       <c r="V83" s="19">
-        <v>8.391069322016449</v>
+        <v>8.4154603664720327</v>
       </c>
       <c r="W83" s="19"/>
       <c r="X83" s="9"/>
@@ -7567,7 +7568,7 @@
     </row>
     <row r="90" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:91" x14ac:dyDescent="0.25">
@@ -7577,7 +7578,7 @@
     </row>
     <row r="93" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="1:91" x14ac:dyDescent="0.25">
@@ -7746,10 +7747,10 @@
         <v>5.106029642679232</v>
       </c>
       <c r="U99" s="19">
-        <v>4.9545029080488234</v>
+        <v>4.9126864797426606</v>
       </c>
       <c r="V99" s="19">
-        <v>3.4004343899014771</v>
+        <v>3.4826356634565911</v>
       </c>
       <c r="W99" s="19"/>
       <c r="X99" s="9"/>
@@ -7883,10 +7884,10 @@
         <v>-2.7427814888135629</v>
       </c>
       <c r="U100" s="19">
-        <v>-25.580801619082678</v>
+        <v>-25.459880315682142</v>
       </c>
       <c r="V100" s="19">
-        <v>-8.0140210538772862</v>
+        <v>-7.5103123723720273</v>
       </c>
       <c r="W100" s="19"/>
       <c r="X100" s="9"/>
@@ -8020,10 +8021,10 @@
         <v>3.8454989048987187</v>
       </c>
       <c r="U101" s="19">
-        <v>-16.371864699764103</v>
+        <v>-16.870355331836535</v>
       </c>
       <c r="V101" s="19">
-        <v>11.905222755275034</v>
+        <v>13.37097882408078</v>
       </c>
       <c r="W101" s="19"/>
       <c r="X101" s="9"/>
@@ -8157,10 +8158,10 @@
         <v>6.2360735522843953</v>
       </c>
       <c r="U102" s="19">
-        <v>5.7621111064719344</v>
+        <v>5.7735195842759879</v>
       </c>
       <c r="V102" s="19">
-        <v>3.1627258286829516</v>
+        <v>3.1953169990653407</v>
       </c>
       <c r="W102" s="19"/>
       <c r="X102" s="9"/>
@@ -8294,10 +8295,10 @@
         <v>4.8780584651914012</v>
       </c>
       <c r="U103" s="19">
-        <v>-12.851017258553398</v>
+        <v>-12.928788882120415</v>
       </c>
       <c r="V103" s="19">
-        <v>2.8864105251775953</v>
+        <v>3.332699360958415</v>
       </c>
       <c r="W103" s="19"/>
       <c r="X103" s="9"/>
@@ -8431,10 +8432,10 @@
         <v>6.1298358868845213</v>
       </c>
       <c r="U104" s="19">
-        <v>-2.1666201913902654</v>
+        <v>-2.3801007239066223</v>
       </c>
       <c r="V104" s="19">
-        <v>14.389791574169195</v>
+        <v>13.856479507830997</v>
       </c>
       <c r="W104" s="19"/>
       <c r="X104" s="9"/>
@@ -8568,10 +8569,10 @@
         <v>5.1305713732099605</v>
       </c>
       <c r="U105" s="19">
-        <v>-33.492609599448215</v>
+        <v>-33.378730093775104</v>
       </c>
       <c r="V105" s="19">
-        <v>0.12444961467885207</v>
+        <v>0.12601787637407824</v>
       </c>
       <c r="W105" s="19"/>
       <c r="X105" s="9"/>
@@ -8705,10 +8706,10 @@
         <v>6.9959568545352226</v>
       </c>
       <c r="U106" s="19">
-        <v>6.1070679110874835</v>
+        <v>6.0326060574885219</v>
       </c>
       <c r="V106" s="19">
-        <v>8.9575740364431766</v>
+        <v>9.081592308761202</v>
       </c>
       <c r="W106" s="19"/>
       <c r="X106" s="9"/>
@@ -8842,10 +8843,10 @@
         <v>7.1840660884528518</v>
       </c>
       <c r="U107" s="19">
-        <v>-44.129355147563786</v>
+        <v>-43.834504352118365</v>
       </c>
       <c r="V107" s="19">
-        <v>3.7458683106605122</v>
+        <v>2.7411291341253872</v>
       </c>
       <c r="W107" s="19"/>
       <c r="X107" s="9"/>
@@ -8979,10 +8980,10 @@
         <v>7.8528705222744577</v>
       </c>
       <c r="U108" s="19">
-        <v>-11.661888427384952</v>
+        <v>-11.19477033818643</v>
       </c>
       <c r="V108" s="19">
-        <v>8.5654287957431592</v>
+        <v>8.9059729610050198</v>
       </c>
       <c r="W108" s="19"/>
       <c r="X108" s="9"/>
@@ -9116,10 +9117,10 @@
         <v>6.6290305046446321</v>
       </c>
       <c r="U109" s="19">
-        <v>-43.060821179582796</v>
+        <v>-43.201834181861557</v>
       </c>
       <c r="V109" s="19">
-        <v>5.1310926021803169</v>
+        <v>4.7170144536528937</v>
       </c>
       <c r="W109" s="19"/>
       <c r="X109" s="9"/>
@@ -9253,10 +9254,10 @@
         <v>8.414956309980326</v>
       </c>
       <c r="U110" s="19">
-        <v>1.4499579376626315</v>
+        <v>1.3359703174766508</v>
       </c>
       <c r="V110" s="19">
-        <v>4.4559070017313473</v>
+        <v>4.3016307645499268</v>
       </c>
       <c r="W110" s="19"/>
       <c r="X110" s="9"/>
@@ -9483,10 +9484,10 @@
         <v>5.8669145456771616</v>
       </c>
       <c r="U112" s="19">
-        <v>-7.9397645330107736</v>
+        <v>-7.9565292769114677</v>
       </c>
       <c r="V112" s="19">
-        <v>4.2028922361138115</v>
+        <v>4.2224420102703277</v>
       </c>
       <c r="W112" s="19"/>
       <c r="X112" s="9"/>
@@ -9783,7 +9784,7 @@
     </row>
     <row r="118" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:96" x14ac:dyDescent="0.25">
@@ -9793,7 +9794,7 @@
     </row>
     <row r="121" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="122" spans="1:96" x14ac:dyDescent="0.25">
@@ -9967,10 +9968,10 @@
         <v>101.43494996805005</v>
       </c>
       <c r="V127" s="19">
-        <v>103.94323015009739</v>
+        <v>103.94298857162569</v>
       </c>
       <c r="W127" s="19">
-        <v>109.14561439004389</v>
+        <v>109.14582794236185</v>
       </c>
       <c r="X127" s="9"/>
       <c r="Y127" s="9"/>
@@ -10111,10 +10112,10 @@
         <v>112.48726897821211</v>
       </c>
       <c r="V128" s="19">
-        <v>130.23574326444526</v>
+        <v>130.23947442003748</v>
       </c>
       <c r="W128" s="19">
-        <v>143.55889609974383</v>
+        <v>143.61617649711036</v>
       </c>
       <c r="X128" s="9"/>
       <c r="Y128" s="9"/>
@@ -10255,10 +10256,10 @@
         <v>102.09778329169032</v>
       </c>
       <c r="V129" s="19">
-        <v>103.71195203976475</v>
+        <v>103.72023867210693</v>
       </c>
       <c r="W129" s="19">
-        <v>105.92696079365211</v>
+        <v>105.97090846549368</v>
       </c>
       <c r="X129" s="9"/>
       <c r="Y129" s="9"/>
@@ -10399,10 +10400,10 @@
         <v>101.90408595912035</v>
       </c>
       <c r="V130" s="19">
-        <v>102.85823476738167</v>
+        <v>102.85873753733077</v>
       </c>
       <c r="W130" s="19">
-        <v>105.64189708609733</v>
+        <v>105.6424450889142</v>
       </c>
       <c r="X130" s="9"/>
       <c r="Y130" s="9"/>
@@ -10543,10 +10544,10 @@
         <v>102.65144673433646</v>
       </c>
       <c r="V131" s="19">
-        <v>106.49158709988664</v>
+        <v>106.49322161423345</v>
       </c>
       <c r="W131" s="19">
-        <v>109.06911395975698</v>
+        <v>109.07590844564126</v>
       </c>
       <c r="X131" s="9"/>
       <c r="Y131" s="9"/>
@@ -10687,10 +10688,10 @@
         <v>102.95098732625998</v>
       </c>
       <c r="V132" s="19">
-        <v>105.77450723344135</v>
+        <v>105.77548032995577</v>
       </c>
       <c r="W132" s="19">
-        <v>109.0662751014235</v>
+        <v>109.05888033661724</v>
       </c>
       <c r="X132" s="9"/>
       <c r="Y132" s="9"/>
@@ -10831,10 +10832,10 @@
         <v>100.74403782309884</v>
       </c>
       <c r="V133" s="19">
-        <v>104.37215431558488</v>
+        <v>104.37332392461028</v>
       </c>
       <c r="W133" s="19">
-        <v>114.57573343736709</v>
+        <v>114.57403178722593</v>
       </c>
       <c r="X133" s="9"/>
       <c r="Y133" s="9"/>
@@ -10975,10 +10976,10 @@
         <v>99.97389149096108</v>
       </c>
       <c r="V134" s="19">
-        <v>100.33789997495978</v>
+        <v>100.34254660572898</v>
       </c>
       <c r="W134" s="19">
-        <v>100.58344468539413</v>
+        <v>100.58820396877479</v>
       </c>
       <c r="X134" s="9"/>
       <c r="Y134" s="9"/>
@@ -11119,10 +11120,10 @@
         <v>101.90164332513214</v>
       </c>
       <c r="V135" s="19">
-        <v>102.70250284720233</v>
+        <v>102.70060417641376</v>
       </c>
       <c r="W135" s="19">
-        <v>102.67757957223161</v>
+        <v>102.67539010768796</v>
       </c>
       <c r="X135" s="9"/>
       <c r="Y135" s="9"/>
@@ -11263,10 +11264,10 @@
         <v>100.17718949016603</v>
       </c>
       <c r="V136" s="19">
-        <v>102.49277424327367</v>
+        <v>102.49565306524353</v>
       </c>
       <c r="W136" s="19">
-        <v>103.5281366654</v>
+        <v>103.51636473193911</v>
       </c>
       <c r="X136" s="9"/>
       <c r="Y136" s="9"/>
@@ -11407,10 +11408,10 @@
         <v>102.81931830872411</v>
       </c>
       <c r="V137" s="19">
-        <v>105.52834177464658</v>
+        <v>105.52983204570596</v>
       </c>
       <c r="W137" s="19">
-        <v>109.41084173884556</v>
+        <v>109.43500754003975</v>
       </c>
       <c r="X137" s="9"/>
       <c r="Y137" s="9"/>
@@ -11551,10 +11552,10 @@
         <v>101.89153997592248</v>
       </c>
       <c r="V138" s="19">
-        <v>104.23097401231003</v>
+        <v>104.22835508941621</v>
       </c>
       <c r="W138" s="19">
-        <v>106.74658084231783</v>
+        <v>106.74284463468418</v>
       </c>
       <c r="X138" s="9"/>
       <c r="Y138" s="9"/>
@@ -11793,10 +11794,10 @@
         <v>101.85976066563667</v>
       </c>
       <c r="V140" s="19">
-        <v>104.37349724796287</v>
+        <v>104.37381168011055</v>
       </c>
       <c r="W140" s="19">
-        <v>108.56853137963493</v>
+        <v>108.57291985527991</v>
       </c>
       <c r="X140" s="9"/>
       <c r="Y140" s="9"/>
@@ -11914,7 +11915,7 @@
     </row>
     <row r="147" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:96" x14ac:dyDescent="0.25">
@@ -11924,7 +11925,7 @@
     </row>
     <row r="150" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="151" spans="1:96" x14ac:dyDescent="0.25">
@@ -12098,10 +12099,10 @@
         <v>33.755687921981099</v>
       </c>
       <c r="V156" s="19">
-        <v>38.485484919796477</v>
+        <v>38.476952956172788</v>
       </c>
       <c r="W156" s="19">
-        <v>38.551022950822642</v>
+        <v>38.564603953085836</v>
       </c>
       <c r="X156" s="9"/>
       <c r="Y156" s="9"/>
@@ -12242,10 +12243,10 @@
         <v>2.403150668560186</v>
       </c>
       <c r="V157" s="19">
-        <v>2.1949930140392806</v>
+        <v>2.1990164040796243</v>
       </c>
       <c r="W157" s="19">
-        <v>2.0533415409479057</v>
+        <v>2.0686703452327722</v>
       </c>
       <c r="X157" s="9"/>
       <c r="Y157" s="9"/>
@@ -12386,10 +12387,10 @@
         <v>1.8546264378058435</v>
       </c>
       <c r="V158" s="19">
-        <v>1.6701738881235699</v>
+        <v>1.6606483794898905</v>
       </c>
       <c r="W158" s="19">
-        <v>1.7611495988138715</v>
+        <v>1.7742365187615299</v>
       </c>
       <c r="X158" s="9"/>
       <c r="Y158" s="9"/>
@@ -12530,10 +12531,10 @@
         <v>11.555496660557802</v>
       </c>
       <c r="V159" s="19">
-        <v>13.076952035558723</v>
+        <v>13.080769253509661</v>
       </c>
       <c r="W159" s="19">
-        <v>12.783005141050968</v>
+        <v>12.787902331598103</v>
       </c>
       <c r="X159" s="9"/>
       <c r="Y159" s="9"/>
@@ -12674,10 +12675,10 @@
         <v>3.0321894488844627</v>
       </c>
       <c r="V160" s="19">
-        <v>2.9060910286389903</v>
+        <v>2.904062303193089</v>
       </c>
       <c r="W160" s="19">
-        <v>2.8252716680483623</v>
+        <v>2.8350410980228267</v>
       </c>
       <c r="X160" s="9"/>
       <c r="Y160" s="9"/>
@@ -12818,10 +12819,10 @@
         <v>4.0339404538609509</v>
       </c>
       <c r="V161" s="19">
-        <v>4.298405364361094</v>
+        <v>4.2898336303781086</v>
       </c>
       <c r="W161" s="19">
-        <v>4.677465659734005</v>
+        <v>4.6449710424679314</v>
       </c>
       <c r="X161" s="9"/>
       <c r="Y161" s="9"/>
@@ -12962,10 +12963,10 @@
         <v>10.63496531648515</v>
       </c>
       <c r="V162" s="19">
-        <v>7.7680428761449942</v>
+        <v>7.7828250254814142</v>
       </c>
       <c r="W162" s="19">
-        <v>7.8770980845258878</v>
+        <v>7.8902301983783145</v>
       </c>
       <c r="X162" s="9"/>
       <c r="Y162" s="9"/>
@@ -13106,10 +13107,10 @@
         <v>2.6300732832759226</v>
       </c>
       <c r="V163" s="19">
-        <v>2.9691415846284093</v>
+        <v>2.9677268621100827</v>
       </c>
       <c r="W163" s="19">
-        <v>2.9919637639877537</v>
+        <v>2.9932715177579428</v>
       </c>
       <c r="X163" s="9"/>
       <c r="Y163" s="9"/>
@@ -13250,10 +13251,10 @@
         <v>2.2147887276341711</v>
       </c>
       <c r="V164" s="19">
-        <v>1.3220752117461687</v>
+        <v>1.3292658026083988</v>
       </c>
       <c r="W164" s="19">
-        <v>1.2651093533931335</v>
+        <v>1.2593844050772076</v>
       </c>
       <c r="X164" s="9"/>
       <c r="Y164" s="9"/>
@@ -13394,10 +13395,10 @@
         <v>5.2669604055831289</v>
       </c>
       <c r="V165" s="19">
-        <v>5.0462981271505596</v>
+        <v>5.0740333810225335</v>
       </c>
       <c r="W165" s="19">
-        <v>5.1054744182107026</v>
+        <v>5.1477490394565573</v>
       </c>
       <c r="X165" s="9"/>
       <c r="Y165" s="9"/>
@@ -13538,10 +13539,10 @@
         <v>9.6140912982976747</v>
       </c>
       <c r="V166" s="19">
-        <v>5.9559928749877953</v>
+        <v>5.9423906817393508</v>
       </c>
       <c r="W166" s="19">
-        <v>5.9893968803757396</v>
+        <v>5.9520731460294813</v>
       </c>
       <c r="X166" s="9"/>
       <c r="Y166" s="9"/>
@@ -13682,10 +13683,10 @@
         <v>13.0040293770736</v>
       </c>
       <c r="V167" s="19">
-        <v>14.306349074823949</v>
+        <v>14.292475320215031</v>
       </c>
       <c r="W167" s="19">
-        <v>14.119700940089016</v>
+        <v>14.081866404131485</v>
       </c>
       <c r="X167" s="9"/>
       <c r="Y167" s="9"/>
@@ -14241,7 +14242,7 @@
     </row>
     <row r="176" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:96" x14ac:dyDescent="0.25">
@@ -14251,7 +14252,7 @@
     </row>
     <row r="179" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="180" spans="1:96" x14ac:dyDescent="0.25">
@@ -14425,10 +14426,10 @@
         <v>33.897057118083325</v>
       </c>
       <c r="V185" s="19">
-        <v>38.644793398881404</v>
+        <v>38.636432308319577</v>
       </c>
       <c r="W185" s="19">
-        <v>38.347193044297015</v>
+        <v>38.362177768811492</v>
       </c>
       <c r="X185" s="9"/>
       <c r="Y185" s="9"/>
@@ -14569,10 +14570,10 @@
         <v>2.1761071645398209</v>
       </c>
       <c r="V186" s="19">
-        <v>1.7591107599772986</v>
+        <v>1.7622900051074581</v>
       </c>
       <c r="W186" s="19">
-        <v>1.5528698086854991</v>
+        <v>1.5639016793102767</v>
       </c>
       <c r="X186" s="9"/>
       <c r="Y186" s="9"/>
@@ -14713,10 +14714,10 @@
         <v>1.8503027097008569</v>
       </c>
       <c r="V187" s="19">
-        <v>1.6808273905484605</v>
+        <v>1.6711126338197584</v>
       </c>
       <c r="W187" s="19">
-        <v>1.8050685495973717</v>
+        <v>1.8178011507614094</v>
       </c>
       <c r="X187" s="9"/>
       <c r="Y187" s="9"/>
@@ -14857,10 +14858,10 @@
         <v>11.550470357873193</v>
       </c>
       <c r="V188" s="19">
-        <v>13.269595967516668</v>
+        <v>13.273444525811815</v>
       </c>
       <c r="W188" s="19">
-        <v>13.1371371876364</v>
+        <v>13.142633094086198</v>
       </c>
       <c r="X188" s="9"/>
       <c r="Y188" s="9"/>
@@ -15001,10 +15002,10 @@
         <v>3.0088040780912682</v>
       </c>
       <c r="V189" s="19">
-        <v>2.8482896371473476</v>
+        <v>2.8462661505234372</v>
       </c>
       <c r="W189" s="19">
-        <v>2.8123048277597431</v>
+        <v>2.8219676948687131</v>
       </c>
       <c r="X189" s="9"/>
       <c r="Y189" s="9"/>
@@ -15145,10 +15146,10 @@
         <v>3.991182793298941</v>
       </c>
       <c r="V190" s="19">
-        <v>4.2414719028436281</v>
+        <v>4.2329875135465338</v>
       </c>
       <c r="W190" s="19">
-        <v>4.6561191971006268</v>
+        <v>4.6242733023423357</v>
       </c>
       <c r="X190" s="9"/>
       <c r="Y190" s="9"/>
@@ -15289,10 +15290,10 @@
         <v>10.75274572304415</v>
       </c>
       <c r="V191" s="19">
-        <v>7.7681428257566552</v>
+        <v>7.7828613960363722</v>
       </c>
       <c r="W191" s="19">
-        <v>7.4641020826439615</v>
+        <v>7.4769589374243255</v>
       </c>
       <c r="X191" s="9"/>
       <c r="Y191" s="9"/>
@@ -15433,10 +15434,10 @@
         <v>2.6796859777314177</v>
       </c>
       <c r="V192" s="19">
-        <v>3.0885606644085999</v>
+        <v>3.0869553853459606</v>
       </c>
       <c r="W192" s="19">
-        <v>3.2294888369875498</v>
+        <v>3.2308781326238809</v>
       </c>
       <c r="X192" s="9"/>
       <c r="Y192" s="9"/>
@@ -15577,10 +15578,10 @@
         <v>2.2138784259049049</v>
       </c>
       <c r="V193" s="19">
-        <v>1.343585693136276</v>
+        <v>1.3509223209236307</v>
       </c>
       <c r="W193" s="19">
-        <v>1.3376928547084457</v>
+        <v>1.3317216709478934</v>
       </c>
       <c r="X193" s="9"/>
       <c r="Y193" s="9"/>
@@ -15721,10 +15722,10 @@
         <v>5.3554240149724626</v>
       </c>
       <c r="V194" s="19">
-        <v>5.1388967424805072</v>
+        <v>5.1670113681048155</v>
       </c>
       <c r="W194" s="19">
-        <v>5.3540407220202777</v>
+        <v>5.3992056748063622</v>
       </c>
       <c r="X194" s="9"/>
       <c r="Y194" s="9"/>
@@ -15865,10 +15866,10 @@
         <v>9.5243681320836924</v>
       </c>
       <c r="V195" s="19">
-        <v>5.8908137424725213</v>
+        <v>5.8772951109869993</v>
       </c>
       <c r="W195" s="19">
-        <v>5.9432869066511413</v>
+        <v>5.9051849603078841</v>
       </c>
       <c r="X195" s="9"/>
       <c r="Y195" s="9"/>
@@ -16009,10 +16010,10 @@
         <v>12.999973504675975</v>
       </c>
       <c r="V196" s="19">
-        <v>14.325911274830657</v>
+        <v>14.312421281473634</v>
       </c>
       <c r="W196" s="19">
-        <v>14.360695981911975</v>
+        <v>14.323295933709213</v>
       </c>
       <c r="X196" s="9"/>
       <c r="Y196" s="9"/>

</xml_diff>

<commit_message>
Q4 2022 SNA Update - Revision
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2023\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2023\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7671BE1E-65FF-4971-B9B1-90D926AC7448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400864C-D78F-4127-BFBC-E04CE38224AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="1395" windowWidth="13830" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -211,13 +211,13 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>As of January 2023</t>
-  </si>
-  <si>
     <t>Annual 2000 to 2022</t>
   </si>
   <si>
     <t>Annual 2001 to 2022</t>
+  </si>
+  <si>
+    <t>As of April 2023</t>
   </si>
 </sst>
 </file>
@@ -298,10 +298,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
@@ -337,9 +338,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 3" xfId="4" xr:uid="{F2E22CA8-8632-45CB-A932-A36F72CD193E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
@@ -658,7 +660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,10 +674,10 @@
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y11" sqref="Y11"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -697,7 +699,7 @@
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.2">
@@ -707,7 +709,7 @@
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.2">
@@ -888,10 +890,10 @@
         <v>5185183.1888882155</v>
       </c>
       <c r="W12" s="8">
-        <v>5634346.1664808691</v>
+        <v>5631917.6611599475</v>
       </c>
       <c r="X12" s="8">
-        <v>6334730.8313580817</v>
+        <v>6332133.7395619042</v>
       </c>
       <c r="Y12" s="9"/>
       <c r="Z12" s="9"/>
@@ -1034,10 +1036,10 @@
         <v>296341.10849450284</v>
       </c>
       <c r="W13" s="8">
-        <v>302235.82338753087</v>
+        <v>301917.11163271719</v>
       </c>
       <c r="X13" s="8">
-        <v>328522.86582235509</v>
+        <v>329167.74690513348</v>
       </c>
       <c r="Y13" s="9"/>
       <c r="Z13" s="9"/>
@@ -1180,10 +1182,10 @@
         <v>223790.22761478901</v>
       </c>
       <c r="W14" s="8">
-        <v>259218.6021169934</v>
+        <v>259081.0383612804</v>
       </c>
       <c r="X14" s="8">
-        <v>278756.03918630292</v>
+        <v>279315.48708031955</v>
       </c>
       <c r="Y14" s="9"/>
       <c r="Z14" s="9"/>
@@ -1326,10 +1328,10 @@
         <v>1762774.3264463176</v>
       </c>
       <c r="W15" s="8">
-        <v>1868331.6070618217</v>
+        <v>1868389.5245533392</v>
       </c>
       <c r="X15" s="8">
-        <v>2085429.4725546623</v>
+        <v>2086180.117886059</v>
       </c>
       <c r="Y15" s="9"/>
       <c r="Z15" s="9"/>
@@ -1472,10 +1474,10 @@
         <v>391353.62540668785</v>
       </c>
       <c r="W16" s="8">
-        <v>414203.73360744608</v>
+        <v>414184.46497346624</v>
       </c>
       <c r="X16" s="8">
-        <v>464435.19302279036</v>
+        <v>465276.59060639073</v>
       </c>
       <c r="Y16" s="9"/>
       <c r="Z16" s="9"/>
@@ -1618,10 +1620,10 @@
         <v>578101.21421777958</v>
       </c>
       <c r="W17" s="8">
-        <v>678637.19846265065</v>
+        <v>680588.98821395624</v>
       </c>
       <c r="X17" s="8">
-        <v>716064.02696786367</v>
+        <v>717176.35769040021</v>
       </c>
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
@@ -1764,10 +1766,10 @@
         <v>1048819.36805525</v>
       </c>
       <c r="W18" s="8">
-        <v>1152774.4022722465</v>
+        <v>1152839.6629508231</v>
       </c>
       <c r="X18" s="8">
-        <v>1516316.5564867058</v>
+        <v>1516541.5231672169</v>
       </c>
       <c r="Y18" s="9"/>
       <c r="Z18" s="9"/>
@@ -1910,10 +1912,10 @@
         <v>399933.10936427652</v>
       </c>
       <c r="W19" s="8">
-        <v>437321.43397174275</v>
+        <v>437277.79155718104</v>
       </c>
       <c r="X19" s="8">
-        <v>472367.61901399633</v>
+        <v>472423.64602658915</v>
       </c>
       <c r="Y19" s="9"/>
       <c r="Z19" s="9"/>
@@ -2056,10 +2058,10 @@
         <v>179132.86171854523</v>
       </c>
       <c r="W20" s="8">
-        <v>183997.94027457573</v>
+        <v>184086.01566947822</v>
       </c>
       <c r="X20" s="8">
-        <v>235922.59279847995</v>
+        <v>236550.09149463687</v>
       </c>
       <c r="Y20" s="9"/>
       <c r="Z20" s="9"/>
@@ -2202,10 +2204,10 @@
         <v>683780.56383788679</v>
       </c>
       <c r="W21" s="8">
-        <v>752093.81384420488</v>
+        <v>751571.57558303094</v>
       </c>
       <c r="X21" s="8">
-        <v>835311.88880971516</v>
+        <v>833429.42225008144</v>
       </c>
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
@@ -2348,10 +2350,10 @@
         <v>800801.04835374421</v>
       </c>
       <c r="W22" s="8">
-        <v>869606.76566889707</v>
+        <v>868805.98865425971</v>
       </c>
       <c r="X22" s="8">
-        <v>1161141.9594095454</v>
+        <v>1161512.316140129</v>
       </c>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
@@ -2494,10 +2496,10 @@
         <v>1926064.7495240266</v>
       </c>
       <c r="W23" s="8">
-        <v>2057381.6883361312</v>
+        <v>2057886.6796678836</v>
       </c>
       <c r="X23" s="8">
-        <v>2298055.6220726361</v>
+        <v>2295052.1911296258</v>
       </c>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
@@ -2738,10 +2740,10 @@
         <v>13476075.391922025</v>
       </c>
       <c r="W25" s="11">
-        <v>14610149.175485112</v>
+        <v>14608546.502977364</v>
       </c>
       <c r="X25" s="11">
-        <v>16727054.667503137</v>
+        <v>16724759.229938485</v>
       </c>
       <c r="Y25" s="9"/>
       <c r="Z25" s="9"/>
@@ -3055,7 +3057,7 @@
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.2">
@@ -3065,7 +3067,7 @@
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.2">
@@ -3246,10 +3248,10 @@
         <v>4988487.6893982869</v>
       </c>
       <c r="W41" s="8">
-        <v>5162218.5407364136</v>
+        <v>5159981.5267388932</v>
       </c>
       <c r="X41" s="8">
-        <v>5458983.1159343701</v>
+        <v>5455159.0229229797</v>
       </c>
       <c r="Y41"/>
       <c r="Z41" s="9"/>
@@ -3392,10 +3394,10 @@
         <v>227535.55311407984</v>
       </c>
       <c r="W42" s="8">
-        <v>210446.92231700796</v>
+        <v>210217.82575502741</v>
       </c>
       <c r="X42" s="8">
-        <v>211825.41741461604</v>
+        <v>212289.07465789252</v>
       </c>
       <c r="Y42"/>
       <c r="Z42" s="9"/>
@@ -3538,10 +3540,10 @@
         <v>215763.31724636882</v>
       </c>
       <c r="W43" s="8">
-        <v>244612.98470551503</v>
+        <v>244485.73965628369</v>
       </c>
       <c r="X43" s="8">
-        <v>255946.95292845464</v>
+        <v>256454.83999876378</v>
       </c>
       <c r="Y43"/>
       <c r="Z43" s="9"/>
@@ -3684,10 +3686,10 @@
         <v>1713781.8027433495</v>
       </c>
       <c r="W44" s="8">
-        <v>1768542.564013296</v>
+        <v>1768543.9657307984</v>
       </c>
       <c r="X44" s="8">
-        <v>1851001.6959430911</v>
+        <v>1851506.0393151762</v>
       </c>
       <c r="Y44"/>
       <c r="Z44" s="9"/>
@@ -3830,10 +3832,10 @@
         <v>367491.58253879054</v>
       </c>
       <c r="W45" s="8">
-        <v>379738.97216163675</v>
+        <v>379727.26651260047</v>
       </c>
       <c r="X45" s="8">
-        <v>412342.00504807866</v>
+        <v>413086.03240013786</v>
       </c>
       <c r="Y45"/>
       <c r="Z45" s="9"/>
@@ -3976,10 +3978,10 @@
         <v>546536.12766820076</v>
       </c>
       <c r="W46" s="8">
-        <v>622266.79420143808</v>
+        <v>624079.48523468187</v>
       </c>
       <c r="X46" s="8">
-        <v>639375.51267636195</v>
+        <v>640402.80102581426</v>
       </c>
       <c r="Y46"/>
       <c r="Z46" s="9"/>
@@ -4122,10 +4124,10 @@
         <v>1004873.0160331208</v>
       </c>
       <c r="W47" s="8">
-        <v>1006139.3356681818</v>
+        <v>1006192.5085302058</v>
       </c>
       <c r="X47" s="8">
-        <v>1172635.5771431166</v>
+        <v>1172803.2083973573</v>
       </c>
       <c r="Y47"/>
       <c r="Z47" s="9"/>
@@ -4268,10 +4270,10 @@
         <v>398567.82879521081</v>
       </c>
       <c r="W48" s="8">
-        <v>434764.13408027322</v>
+        <v>434718.13045070309</v>
       </c>
       <c r="X48" s="8">
-        <v>466730.48079463182</v>
+        <v>466812.65729031921</v>
       </c>
       <c r="Y48"/>
       <c r="Z48" s="9"/>
@@ -4414,10 +4416,10 @@
         <v>174422.40301803884</v>
       </c>
       <c r="W49" s="8">
-        <v>179203.54632360791</v>
+        <v>179288.73530703833</v>
       </c>
       <c r="X49" s="8">
-        <v>224521.47003161907</v>
+        <v>225117.50566663369</v>
       </c>
       <c r="Y49"/>
       <c r="Z49" s="9"/>
@@ -4560,10 +4562,10 @@
         <v>667131.28156042565</v>
       </c>
       <c r="W50" s="8">
-        <v>726545.81311060337</v>
+        <v>726064.34423630452</v>
       </c>
       <c r="X50" s="8">
-        <v>791941.50539112114</v>
+        <v>790083.71505532251</v>
       </c>
       <c r="Y50"/>
       <c r="Z50" s="9"/>
@@ -4706,10 +4708,10 @@
         <v>758838.55098614178</v>
       </c>
       <c r="W51" s="8">
-        <v>794633.07511604822</v>
+        <v>793898.30837798945</v>
       </c>
       <c r="X51" s="8">
-        <v>1015668.7175197232</v>
+        <v>1016009.2133631294</v>
       </c>
       <c r="Y51"/>
       <c r="Z51" s="9"/>
@@ -4852,10 +4854,10 @@
         <v>1847927.8003300345</v>
       </c>
       <c r="W52" s="8">
-        <v>1927418.831095702</v>
+        <v>1927919.2276264182</v>
       </c>
       <c r="X52" s="8">
-        <v>2077374.9975844396</v>
+        <v>2070492.9913601633</v>
       </c>
       <c r="Y52"/>
       <c r="Z52" s="9"/>
@@ -5096,10 +5098,10 @@
         <v>12911356.95343205</v>
       </c>
       <c r="W54" s="11">
-        <v>13456531.513529725</v>
+        <v>13455117.064156944</v>
       </c>
       <c r="X54" s="11">
-        <v>14578347.448409623</v>
+        <v>14570217.10145369</v>
       </c>
       <c r="Y54" s="9"/>
       <c r="Z54" s="9"/>
@@ -5413,7 +5415,7 @@
     </row>
     <row r="61" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:96" x14ac:dyDescent="0.2">
@@ -5423,7 +5425,7 @@
     </row>
     <row r="64" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:91" x14ac:dyDescent="0.2">
@@ -5599,10 +5601,10 @@
         <v>7.506714157371519</v>
       </c>
       <c r="V70" s="18">
-        <v>8.6624321886101114</v>
+        <v>8.6155967108178118</v>
       </c>
       <c r="W70" s="18">
-        <v>12.430628935152257</v>
+        <v>12.432995660269299</v>
       </c>
       <c r="X70" s="18"/>
       <c r="Y70" s="9"/>
@@ -5738,10 +5740,10 @@
         <v>-13.696313377715427</v>
       </c>
       <c r="V71" s="18">
-        <v>1.9891654326916921</v>
+        <v>1.8816164812712088</v>
       </c>
       <c r="W71" s="18">
-        <v>8.6975270304468779</v>
+        <v>9.0258664456113138</v>
       </c>
       <c r="X71" s="18"/>
       <c r="Y71" s="9"/>
@@ -5877,10 +5879,10 @@
         <v>-15.549326266213711</v>
       </c>
       <c r="V72" s="18">
-        <v>15.831064153161961</v>
+        <v>15.769594196596287</v>
       </c>
       <c r="W72" s="18">
-        <v>7.5370505472025116</v>
+        <v>7.8100847700103913</v>
       </c>
       <c r="X72" s="18"/>
       <c r="Y72" s="9"/>
@@ -6016,10 +6018,10 @@
         <v>6.7644205521184944</v>
       </c>
       <c r="V73" s="18">
-        <v>5.9881335365431312</v>
+        <v>5.9914191239633965</v>
       </c>
       <c r="W73" s="18">
-        <v>11.619878648536769</v>
+        <v>11.656594648526792</v>
       </c>
       <c r="X73" s="18"/>
       <c r="Y73" s="9"/>
@@ -6155,10 +6157,10 @@
         <v>-9.6701110721467387</v>
       </c>
       <c r="V74" s="18">
-        <v>5.8387368143102805</v>
+        <v>5.8338132278838515</v>
       </c>
       <c r="W74" s="18">
-        <v>12.127234821825667</v>
+        <v>12.335596806171267</v>
       </c>
       <c r="X74" s="18"/>
       <c r="Y74" s="9"/>
@@ -6294,10 +6296,10 @@
         <v>0.29813218757593063</v>
       </c>
       <c r="V75" s="18">
-        <v>17.390723591699214</v>
+        <v>17.728344358323383</v>
       </c>
       <c r="W75" s="18">
-        <v>5.5149980858694221</v>
+        <v>5.3758391790115212</v>
       </c>
       <c r="X75" s="18"/>
       <c r="Y75" s="9"/>
@@ -6433,10 +6435,10 @@
         <v>-30.978710656790966</v>
       </c>
       <c r="V76" s="18">
-        <v>9.9116241922336883</v>
+        <v>9.9178464913791942</v>
       </c>
       <c r="W76" s="18">
-        <v>31.536279214552053</v>
+        <v>31.548347259796572</v>
       </c>
       <c r="X76" s="18"/>
       <c r="Y76" s="9"/>
@@ -6572,10 +6574,10 @@
         <v>6.4236027664522624</v>
       </c>
       <c r="V77" s="18">
-        <v>9.3486444937999096</v>
+        <v>9.3377320653113003</v>
       </c>
       <c r="W77" s="18">
-        <v>8.0138274321395357</v>
+        <v>8.0374204105474689</v>
       </c>
       <c r="X77" s="18"/>
       <c r="Y77" s="9"/>
@@ -6711,10 +6713,10 @@
         <v>-43.394138223062825</v>
       </c>
       <c r="V78" s="18">
-        <v>2.7159051161001173</v>
+        <v>2.7650727529354242</v>
       </c>
       <c r="W78" s="18">
-        <v>28.220235751779796</v>
+        <v>28.499761719736796</v>
       </c>
       <c r="X78" s="18"/>
       <c r="Y78" s="9"/>
@@ -6850,10 +6852,10 @@
         <v>-9.1394951673101588</v>
       </c>
       <c r="V79" s="18">
-        <v>9.9905223428541348</v>
+        <v>9.9141472177346515</v>
       </c>
       <c r="W79" s="18">
-        <v>11.064853005525293</v>
+        <v>10.891557015517691</v>
       </c>
       <c r="X79" s="18"/>
       <c r="Y79" s="9"/>
@@ -6989,10 +6991,10 @@
         <v>-41.704525979300023</v>
       </c>
       <c r="V80" s="18">
-        <v>8.592111293635412</v>
+        <v>8.4921142948448249</v>
       </c>
       <c r="W80" s="18">
-        <v>33.524945440874177</v>
+        <v>33.69064340121065</v>
       </c>
       <c r="X80" s="18"/>
       <c r="Y80" s="9"/>
@@ -7128,10 +7130,10 @@
         <v>3.6600438081157307</v>
       </c>
       <c r="V81" s="18">
-        <v>6.8178880717564567</v>
+        <v>6.8441068856295288</v>
       </c>
       <c r="W81" s="18">
-        <v>11.698069206163964</v>
+        <v>11.524711919512384</v>
       </c>
       <c r="X81" s="18"/>
       <c r="Y81" s="9"/>
@@ -7360,10 +7362,10 @@
         <v>-5.6847589582409483</v>
       </c>
       <c r="V83" s="18">
-        <v>8.4154603664720327</v>
+        <v>8.4035676420612475</v>
       </c>
       <c r="W83" s="18">
-        <v>14.489280476136798</v>
+        <v>14.486127874048378</v>
       </c>
       <c r="X83" s="18"/>
       <c r="Y83" s="9"/>
@@ -7663,7 +7665,7 @@
     </row>
     <row r="90" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="1:91" x14ac:dyDescent="0.2">
@@ -7673,7 +7675,7 @@
     </row>
     <row r="93" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:91" x14ac:dyDescent="0.2">
@@ -7849,10 +7851,10 @@
         <v>4.9126864797426606</v>
       </c>
       <c r="V99" s="18">
-        <v>3.4826356634565911</v>
+        <v>3.4377921329759289</v>
       </c>
       <c r="W99" s="18">
-        <v>5.7487797708700299</v>
+        <v>5.7205145920481471</v>
       </c>
       <c r="X99" s="18"/>
       <c r="Y99" s="9"/>
@@ -7988,10 +7990,10 @@
         <v>-25.459880315682142</v>
       </c>
       <c r="V100" s="18">
-        <v>-7.5103123723720273</v>
+        <v>-7.6109984229013321</v>
       </c>
       <c r="W100" s="18">
-        <v>0.655032196446939</v>
+        <v>0.98528699715446066</v>
       </c>
       <c r="X100" s="18"/>
       <c r="Y100" s="9"/>
@@ -8127,10 +8129,10 @@
         <v>-16.870355331836535</v>
       </c>
       <c r="V101" s="18">
-        <v>13.37097882408078</v>
+        <v>13.312004457698535</v>
       </c>
       <c r="W101" s="18">
-        <v>4.6334286941408038</v>
+        <v>4.8956230982253288</v>
       </c>
       <c r="X101" s="18"/>
       <c r="Y101" s="9"/>
@@ -8266,10 +8268,10 @@
         <v>5.7735195842759879</v>
       </c>
       <c r="V102" s="18">
-        <v>3.1953169990653407</v>
+        <v>3.1953987899619278</v>
       </c>
       <c r="W102" s="18">
-        <v>4.6625472073837528</v>
+        <v>4.6909816884363522</v>
       </c>
       <c r="X102" s="18"/>
       <c r="Y102" s="9"/>
@@ -8405,10 +8407,10 @@
         <v>-12.928788882120415</v>
       </c>
       <c r="V103" s="18">
-        <v>3.332699360958415</v>
+        <v>3.3295140773784766</v>
       </c>
       <c r="W103" s="18">
-        <v>8.5856431065927978</v>
+        <v>8.7849277177019474</v>
       </c>
       <c r="X103" s="18"/>
       <c r="Y103" s="9"/>
@@ -8544,10 +8546,10 @@
         <v>-2.3801007239066223</v>
       </c>
       <c r="V104" s="18">
-        <v>13.856479507830997</v>
+        <v>14.188148530513487</v>
       </c>
       <c r="W104" s="18">
-        <v>2.749418518608195</v>
+        <v>2.6155828187484929</v>
       </c>
       <c r="X104" s="18"/>
       <c r="Y104" s="9"/>
@@ -8683,10 +8685,10 @@
         <v>-33.378730093775104</v>
       </c>
       <c r="V105" s="18">
-        <v>0.12601787637407824</v>
+        <v>0.1313093770090461</v>
       </c>
       <c r="W105" s="18">
-        <v>16.548030235232176</v>
+        <v>16.558531141374516</v>
       </c>
       <c r="X105" s="18"/>
       <c r="Y105" s="9"/>
@@ -8822,10 +8824,10 @@
         <v>6.0326060574885219</v>
       </c>
       <c r="V106" s="18">
-        <v>9.081592308761202</v>
+        <v>9.0700500752324302</v>
       </c>
       <c r="W106" s="18">
-        <v>7.3525721669709867</v>
+        <v>7.3828360474272046</v>
       </c>
       <c r="X106" s="18"/>
       <c r="Y106" s="9"/>
@@ -8961,10 +8963,10 @@
         <v>-43.834504352118365</v>
       </c>
       <c r="V107" s="18">
-        <v>2.7411291341253872</v>
+        <v>2.7899697543418256</v>
       </c>
       <c r="W107" s="18">
-        <v>25.288519472809725</v>
+        <v>25.561433227308996</v>
       </c>
       <c r="X107" s="18"/>
       <c r="Y107" s="9"/>
@@ -9100,10 +9102,10 @@
         <v>-11.19477033818643</v>
       </c>
       <c r="V108" s="18">
-        <v>8.9059729610050198</v>
+        <v>8.8338029267693656</v>
       </c>
       <c r="W108" s="18">
-        <v>9.0009041550367357</v>
+        <v>8.8173136895126589</v>
       </c>
       <c r="X108" s="18"/>
       <c r="Y108" s="9"/>
@@ -9239,10 +9241,10 @@
         <v>-43.201834181861557</v>
       </c>
       <c r="V109" s="18">
-        <v>4.7170144536528937</v>
+        <v>4.6201866452733782</v>
       </c>
       <c r="W109" s="18">
-        <v>27.816063706056411</v>
+        <v>27.977248803934842</v>
       </c>
       <c r="X109" s="18"/>
       <c r="Y109" s="9"/>
@@ -9378,10 +9380,10 @@
         <v>1.3359703174766508</v>
       </c>
       <c r="V110" s="18">
-        <v>4.3016307645499268</v>
+        <v>4.3287095568396978</v>
       </c>
       <c r="W110" s="18">
-        <v>7.7801546850867993</v>
+        <v>7.3952145759382546</v>
       </c>
       <c r="X110" s="18"/>
       <c r="Y110" s="9"/>
@@ -9610,10 +9612,10 @@
         <v>-7.9565292769114677</v>
       </c>
       <c r="V112" s="18">
-        <v>4.2224420102703277</v>
+        <v>4.2114869311265863</v>
       </c>
       <c r="W112" s="18">
-        <v>8.3365905527139574</v>
+        <v>8.2875535900557793</v>
       </c>
       <c r="X112" s="18"/>
       <c r="Y112" s="9"/>
@@ -9910,7 +9912,7 @@
     </row>
     <row r="118" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:96" x14ac:dyDescent="0.2">
@@ -9920,7 +9922,7 @@
     </row>
     <row r="121" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="122" spans="1:96" x14ac:dyDescent="0.2">
@@ -10101,10 +10103,10 @@
         <v>103.94298857162569</v>
       </c>
       <c r="W127" s="18">
-        <v>109.14582794236185</v>
+        <v>109.14608186047747</v>
       </c>
       <c r="X127" s="18">
-        <v>116.04232320974704</v>
+        <v>116.07606144850794</v>
       </c>
       <c r="Y127" s="9"/>
       <c r="Z127" s="9"/>
@@ -10247,10 +10249,10 @@
         <v>130.23947442003748</v>
       </c>
       <c r="W128" s="18">
-        <v>143.61617649711036</v>
+        <v>143.6210799670954</v>
       </c>
       <c r="X128" s="18">
-        <v>155.09133409581418</v>
+        <v>155.05637651659322</v>
       </c>
       <c r="Y128" s="9"/>
       <c r="Z128" s="9"/>
@@ -10393,10 +10395,10 @@
         <v>103.72023867210693</v>
       </c>
       <c r="W129" s="18">
-        <v>105.97090846549368</v>
+        <v>105.96979550852981</v>
       </c>
       <c r="X129" s="18">
-        <v>108.91164594728508</v>
+        <v>108.91410241337849</v>
       </c>
       <c r="Y129" s="9"/>
       <c r="Z129" s="9"/>
@@ -10539,10 +10541,10 @@
         <v>102.85873753733077</v>
       </c>
       <c r="W130" s="18">
-        <v>105.6424450889142</v>
+        <v>105.64563622715949</v>
       </c>
       <c r="X130" s="18">
-        <v>112.66491419891054</v>
+        <v>112.67476711324595</v>
       </c>
       <c r="Y130" s="9"/>
       <c r="Z130" s="9"/>
@@ -10685,10 +10687,10 @@
         <v>106.49322161423345</v>
       </c>
       <c r="W131" s="18">
-        <v>109.07590844564126</v>
+        <v>109.07419653513935</v>
       </c>
       <c r="X131" s="18">
-        <v>112.63349048531634</v>
+        <v>112.63430716914151</v>
       </c>
       <c r="Y131" s="9"/>
       <c r="Z131" s="9"/>
@@ -10831,10 +10833,10 @@
         <v>105.77548032995577</v>
       </c>
       <c r="W132" s="18">
-        <v>109.05888033661724</v>
+        <v>109.05485668352392</v>
       </c>
       <c r="X132" s="18">
-        <v>111.99428391783277</v>
+        <v>111.98832305880113</v>
       </c>
       <c r="Y132" s="9"/>
       <c r="Z132" s="9"/>
@@ -10977,10 +10979,10 @@
         <v>104.37332392461028</v>
       </c>
       <c r="W133" s="18">
-        <v>114.57403178722593</v>
+        <v>114.57446295588424</v>
       </c>
       <c r="X133" s="18">
-        <v>129.30842164800225</v>
+        <v>129.30912128383244</v>
       </c>
       <c r="Y133" s="9"/>
       <c r="Z133" s="9"/>
@@ -11123,10 +11125,10 @@
         <v>100.34254660572898</v>
       </c>
       <c r="W134" s="18">
-        <v>100.58820396877479</v>
+        <v>100.58880937489867</v>
       </c>
       <c r="X134" s="18">
-        <v>101.20779303073735</v>
+        <v>101.20197870572743</v>
       </c>
       <c r="Y134" s="9"/>
       <c r="Z134" s="9"/>
@@ -11269,10 +11271,10 @@
         <v>102.70060417641376</v>
       </c>
       <c r="W135" s="18">
-        <v>102.67539010768796</v>
+        <v>102.67572882045511</v>
       </c>
       <c r="X135" s="18">
-        <v>105.07796549045187</v>
+        <v>105.07849702498622</v>
       </c>
       <c r="Y135" s="9"/>
       <c r="Z135" s="9"/>
@@ -11415,10 +11417,10 @@
         <v>102.49565306524353</v>
       </c>
       <c r="W136" s="18">
-        <v>103.51636473193911</v>
+        <v>103.5130813886138</v>
       </c>
       <c r="X136" s="18">
-        <v>105.47646298664122</v>
+        <v>105.48621701331027</v>
       </c>
       <c r="Y136" s="9"/>
       <c r="Z136" s="9"/>
@@ -11561,10 +11563,10 @@
         <v>105.52983204570596</v>
       </c>
       <c r="W137" s="18">
-        <v>109.43500754003975</v>
+        <v>109.4354251024056</v>
       </c>
       <c r="X137" s="18">
-        <v>114.32290267293747</v>
+        <v>114.32104166608532</v>
       </c>
       <c r="Y137" s="9"/>
       <c r="Z137" s="9"/>
@@ -11707,10 +11709,10 @@
         <v>104.22835508941621</v>
       </c>
       <c r="W138" s="18">
-        <v>106.74284463468418</v>
+        <v>106.74133284107947</v>
       </c>
       <c r="X138" s="18">
-        <v>110.62305191623096</v>
+        <v>110.84568751048722</v>
       </c>
       <c r="Y138" s="9"/>
       <c r="Z138" s="9"/>
@@ -11951,10 +11953,10 @@
         <v>104.37381168011055</v>
       </c>
       <c r="W140" s="18">
-        <v>108.57291985527991</v>
+        <v>108.5724221745572</v>
       </c>
       <c r="X140" s="18">
-        <v>114.73903147594359</v>
+        <v>114.78730284856107</v>
       </c>
       <c r="Y140" s="9"/>
       <c r="Z140" s="9"/>
@@ -12072,7 +12074,7 @@
     </row>
     <row r="147" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="149" spans="1:96" x14ac:dyDescent="0.2">
@@ -12082,7 +12084,7 @@
     </row>
     <row r="150" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="151" spans="1:96" x14ac:dyDescent="0.2">
@@ -12263,10 +12265,10 @@
         <v>38.476952956172788</v>
       </c>
       <c r="W156" s="18">
-        <v>38.564603953085836</v>
+        <v>38.552210926748309</v>
       </c>
       <c r="X156" s="18">
-        <v>37.871167143759166</v>
+        <v>37.860836455133793</v>
       </c>
       <c r="Y156" s="9"/>
       <c r="Z156" s="9"/>
@@ -12409,10 +12411,10 @@
         <v>2.1990164040796243</v>
       </c>
       <c r="W157" s="18">
-        <v>2.0686703452327722</v>
+        <v>2.0667156145286842</v>
       </c>
       <c r="X157" s="18">
-        <v>1.9640209968381359</v>
+        <v>1.9681464012701617</v>
       </c>
       <c r="Y157" s="9"/>
       <c r="Z157" s="9"/>
@@ -12555,10 +12557,10 @@
         <v>1.6606483794898905</v>
       </c>
       <c r="W158" s="18">
-        <v>1.7742365187615299</v>
+        <v>1.7734895001941304</v>
       </c>
       <c r="X158" s="18">
-        <v>1.6664980459940895</v>
+        <v>1.6700717973884214</v>
       </c>
       <c r="Y158" s="9"/>
       <c r="Z158" s="9"/>
@@ -12701,10 +12703,10 @@
         <v>13.080769253509661</v>
       </c>
       <c r="W159" s="18">
-        <v>12.787902331598103</v>
+        <v>12.789701728180441</v>
       </c>
       <c r="X159" s="18">
-        <v>12.467403939356863</v>
+        <v>12.47360329200824</v>
       </c>
       <c r="Y159" s="9"/>
       <c r="Z159" s="9"/>
@@ -12847,10 +12849,10 @@
         <v>2.904062303193089</v>
       </c>
       <c r="W160" s="18">
-        <v>2.8350410980228267</v>
+        <v>2.8352202246065437</v>
       </c>
       <c r="X160" s="18">
-        <v>2.7765509365201178</v>
+        <v>2.7819628624220383</v>
       </c>
       <c r="Y160" s="9"/>
       <c r="Z160" s="9"/>
@@ -12993,10 +12995,10 @@
         <v>4.2898336303781086</v>
       </c>
       <c r="W161" s="18">
-        <v>4.6449710424679314</v>
+        <v>4.6588412343092838</v>
       </c>
       <c r="X161" s="18">
-        <v>4.2808733587689716</v>
+        <v>4.2881117021200792</v>
       </c>
       <c r="Y161" s="9"/>
       <c r="Z161" s="9"/>
@@ -13139,10 +13141,10 @@
         <v>7.7828250254814142</v>
       </c>
       <c r="W162" s="18">
-        <v>7.8902301983783145</v>
+        <v>7.891542548164276</v>
       </c>
       <c r="X162" s="18">
-        <v>9.0650541092124488</v>
+        <v>9.067643380195884</v>
       </c>
       <c r="Y162" s="9"/>
       <c r="Z162" s="9"/>
@@ -13285,10 +13287,10 @@
         <v>2.9677268621100827</v>
       </c>
       <c r="W163" s="18">
-        <v>2.9932715177579428</v>
+        <v>2.9933011574290407</v>
       </c>
       <c r="X163" s="18">
-        <v>2.8239736666354012</v>
+        <v>2.824696245437829</v>
       </c>
       <c r="Y163" s="9"/>
       <c r="Z163" s="9"/>
@@ -13431,10 +13433,10 @@
         <v>1.3292658026083988</v>
       </c>
       <c r="W164" s="18">
-        <v>1.2593844050772076</v>
+        <v>1.2601254726605395</v>
       </c>
       <c r="X164" s="18">
-        <v>1.4104251913328405</v>
+        <v>1.4143706838613002</v>
       </c>
       <c r="Y164" s="9"/>
       <c r="Z164" s="9"/>
@@ -13577,10 +13579,10 @@
         <v>5.0740333810225335</v>
       </c>
       <c r="W165" s="18">
-        <v>5.1477490394565573</v>
+        <v>5.144738906296074</v>
       </c>
       <c r="X165" s="18">
-        <v>4.9937774785451996</v>
+        <v>4.9832072963907583</v>
       </c>
       <c r="Y165" s="9"/>
       <c r="Z165" s="9"/>
@@ -13723,10 +13725,10 @@
         <v>5.9423906817393508</v>
       </c>
       <c r="W166" s="18">
-        <v>5.9520731460294813</v>
+        <v>5.9472445700000929</v>
       </c>
       <c r="X166" s="18">
-        <v>6.9417000332125429</v>
+        <v>6.9448671886465254</v>
       </c>
       <c r="Y166" s="9"/>
       <c r="Z166" s="9"/>
@@ -13869,10 +13871,10 @@
         <v>14.292475320215031</v>
       </c>
       <c r="W167" s="18">
-        <v>14.081866404131485</v>
+        <v>14.086868116882581</v>
       </c>
       <c r="X167" s="18">
-        <v>13.738555099824213</v>
+        <v>13.722482695124977</v>
       </c>
       <c r="Y167" s="9"/>
       <c r="Z167" s="9"/>
@@ -14430,7 +14432,7 @@
     </row>
     <row r="176" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="178" spans="1:96" x14ac:dyDescent="0.2">
@@ -14440,7 +14442,7 @@
     </row>
     <row r="179" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="180" spans="1:96" x14ac:dyDescent="0.2">
@@ -14621,10 +14623,10 @@
         <v>38.636432308319577</v>
       </c>
       <c r="W185" s="18">
-        <v>38.362177768811492</v>
+        <v>38.349584787222376</v>
       </c>
       <c r="X185" s="18">
-        <v>37.445829407296095</v>
+        <v>37.440478648590016</v>
       </c>
       <c r="Y185" s="9"/>
       <c r="Z185" s="9"/>
@@ -14767,10 +14769,10 @@
         <v>1.7622900051074581</v>
       </c>
       <c r="W186" s="18">
-        <v>1.5639016793102767</v>
+        <v>1.562363409791701</v>
       </c>
       <c r="X186" s="18">
-        <v>1.4530139178273216</v>
+        <v>1.4570069421732375</v>
       </c>
       <c r="Y186" s="9"/>
       <c r="Z186" s="9"/>
@@ -14913,10 +14915,10 @@
         <v>1.6711126338197584</v>
       </c>
       <c r="W187" s="18">
-        <v>1.8178011507614094</v>
+        <v>1.8170465443780399</v>
       </c>
       <c r="X187" s="18">
-        <v>1.7556650630958612</v>
+        <v>1.7601305334920299</v>
       </c>
       <c r="Y187" s="9"/>
       <c r="Z187" s="9"/>
@@ -15059,10 +15061,10 @@
         <v>13.273444525811815</v>
       </c>
       <c r="W188" s="18">
-        <v>13.142633094086198</v>
+        <v>13.144025111769697</v>
       </c>
       <c r="X188" s="18">
-        <v>12.696923999743332</v>
+        <v>12.707470495621159</v>
       </c>
       <c r="Y188" s="9"/>
       <c r="Z188" s="9"/>
@@ -15205,10 +15207,10 @@
         <v>2.8462661505234372</v>
       </c>
       <c r="W189" s="18">
-        <v>2.8219676948687131</v>
+        <v>2.8221773523186586</v>
       </c>
       <c r="X189" s="18">
-        <v>2.8284550529975316</v>
+        <v>2.8351398577233535</v>
       </c>
       <c r="Y189" s="9"/>
       <c r="Z189" s="9"/>
@@ -15351,10 +15353,10 @@
         <v>4.2329875135465338</v>
       </c>
       <c r="W190" s="18">
-        <v>4.6242733023423357</v>
+        <v>4.6382315535341254</v>
       </c>
       <c r="X190" s="18">
-        <v>4.3857886837929119</v>
+        <v>4.3952866080624178</v>
       </c>
       <c r="Y190" s="9"/>
       <c r="Z190" s="9"/>
@@ -15497,10 +15499,10 @@
         <v>7.7828613960363722</v>
       </c>
       <c r="W191" s="18">
-        <v>7.4769589374243255</v>
+        <v>7.4781401286399793</v>
       </c>
       <c r="X191" s="18">
-        <v>8.0436797194804228</v>
+        <v>8.0493186905248315</v>
       </c>
       <c r="Y191" s="9"/>
       <c r="Z191" s="9"/>
@@ -15643,10 +15645,10 @@
         <v>3.0869553853459606</v>
       </c>
       <c r="W192" s="18">
-        <v>3.2308781326238809</v>
+        <v>3.23087586958829</v>
       </c>
       <c r="X192" s="18">
-        <v>3.2015321520241877</v>
+        <v>3.2038826466336228</v>
       </c>
       <c r="Y192" s="9"/>
       <c r="Z192" s="9"/>
@@ -15789,10 +15791,10 @@
         <v>1.3509223209236307</v>
       </c>
       <c r="W193" s="18">
-        <v>1.3317216709478934</v>
+        <v>1.3324948006929289</v>
       </c>
       <c r="X193" s="18">
-        <v>1.540102338939058</v>
+        <v>1.545052514311358</v>
       </c>
       <c r="Y193" s="9"/>
       <c r="Z193" s="9"/>
@@ -15935,10 +15937,10 @@
         <v>5.1670113681048155</v>
       </c>
       <c r="W194" s="18">
-        <v>5.3992056748063622</v>
+        <v>5.3961949255013595</v>
       </c>
       <c r="X194" s="18">
-        <v>5.4323132864933568</v>
+        <v>5.4225939775220979</v>
       </c>
       <c r="Y194" s="9"/>
       <c r="Z194" s="9"/>
@@ -16081,10 +16083,10 @@
         <v>5.8772951109869993</v>
       </c>
       <c r="W195" s="18">
-        <v>5.9051849603078841</v>
+        <v>5.9003448620514298</v>
       </c>
       <c r="X195" s="18">
-        <v>6.9669674228441041</v>
+        <v>6.973192000425037</v>
       </c>
       <c r="Y195" s="9"/>
       <c r="Z195" s="9"/>
@@ -16227,10 +16229,10 @@
         <v>14.312421281473634</v>
       </c>
       <c r="W196" s="18">
-        <v>14.323295933709213</v>
+        <v>14.32852065451142</v>
       </c>
       <c r="X196" s="18">
-        <v>14.249728955465827</v>
+        <v>14.210447084920839</v>
       </c>
       <c r="Y196" s="9"/>
       <c r="Z196" s="9"/>

</xml_diff>

<commit_message>
Q4 2023 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2023\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2024\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400864C-D78F-4127-BFBC-E04CE38224AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42466AC0-7B75-4DED-A854-D88C81F844C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="975" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$X$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$Y$202</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="59">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -211,13 +211,16 @@
     <t>2021 - 2022</t>
   </si>
   <si>
-    <t>Annual 2000 to 2022</t>
+    <t>2022 - 2023</t>
   </si>
   <si>
-    <t>Annual 2001 to 2022</t>
+    <t>As of January 2024</t>
   </si>
   <si>
-    <t>As of April 2023</t>
+    <t>Annual 2000 to 2023</t>
+  </si>
+  <si>
+    <t>Annual 2001 to 2023</t>
   </si>
 </sst>
 </file>
@@ -372,9 +375,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -412,7 +415,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -518,7 +521,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -660,7 +663,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -674,17 +677,17 @@
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:X1048576"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
-    <col min="2" max="24" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="7.77734375" style="1"/>
+    <col min="2" max="25" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" x14ac:dyDescent="0.2">
@@ -699,7 +702,7 @@
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.2">
@@ -709,7 +712,7 @@
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:96" x14ac:dyDescent="0.2">
@@ -744,6 +747,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
@@ -818,6 +822,9 @@
       <c r="X10" s="6">
         <v>2022</v>
       </c>
+      <c r="Y10" s="6">
+        <v>2023</v>
+      </c>
     </row>
     <row r="11" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
@@ -895,7 +902,9 @@
       <c r="X12" s="8">
         <v>6332133.7395619042</v>
       </c>
-      <c r="Y12" s="9"/>
+      <c r="Y12" s="8">
+        <v>6846247.7146898005</v>
+      </c>
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
@@ -1041,7 +1050,9 @@
       <c r="X13" s="8">
         <v>329167.74690513348</v>
       </c>
-      <c r="Y13" s="9"/>
+      <c r="Y13" s="8">
+        <v>355136.62934378185</v>
+      </c>
       <c r="Z13" s="9"/>
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
@@ -1187,7 +1198,9 @@
       <c r="X14" s="8">
         <v>279315.48708031955</v>
       </c>
-      <c r="Y14" s="9"/>
+      <c r="Y14" s="8">
+        <v>263849.95596516988</v>
+      </c>
       <c r="Z14" s="9"/>
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
@@ -1333,7 +1346,9 @@
       <c r="X15" s="8">
         <v>2086180.117886059</v>
       </c>
-      <c r="Y15" s="9"/>
+      <c r="Y15" s="8">
+        <v>2291054.1968541136</v>
+      </c>
       <c r="Z15" s="9"/>
       <c r="AA15" s="9"/>
       <c r="AB15" s="9"/>
@@ -1479,7 +1494,9 @@
       <c r="X16" s="8">
         <v>465276.59060639073</v>
       </c>
-      <c r="Y16" s="9"/>
+      <c r="Y16" s="8">
+        <v>482024.65746953094</v>
+      </c>
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
@@ -1625,7 +1642,9 @@
       <c r="X17" s="8">
         <v>717176.35769040021</v>
       </c>
-      <c r="Y17" s="9"/>
+      <c r="Y17" s="8">
+        <v>798368.39141860767</v>
+      </c>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
       <c r="AB17" s="9"/>
@@ -1771,7 +1790,9 @@
       <c r="X18" s="8">
         <v>1516541.5231672169</v>
       </c>
-      <c r="Y18" s="9"/>
+      <c r="Y18" s="8">
+        <v>1804864.973114013</v>
+      </c>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
@@ -1917,7 +1938,9 @@
       <c r="X19" s="8">
         <v>472423.64602658915</v>
       </c>
-      <c r="Y19" s="9"/>
+      <c r="Y19" s="8">
+        <v>498157.24030570779</v>
+      </c>
       <c r="Z19" s="9"/>
       <c r="AA19" s="9"/>
       <c r="AB19" s="9"/>
@@ -2063,7 +2086,9 @@
       <c r="X20" s="8">
         <v>236550.09149463687</v>
       </c>
-      <c r="Y20" s="9"/>
+      <c r="Y20" s="8">
+        <v>287219.46670092957</v>
+      </c>
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
       <c r="AB20" s="9"/>
@@ -2209,7 +2234,9 @@
       <c r="X21" s="8">
         <v>833429.42225008144</v>
       </c>
-      <c r="Y21" s="9"/>
+      <c r="Y21" s="8">
+        <v>923978.21699643123</v>
+      </c>
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9"/>
@@ -2355,7 +2382,9 @@
       <c r="X22" s="8">
         <v>1161512.316140129</v>
       </c>
-      <c r="Y22" s="9"/>
+      <c r="Y22" s="8">
+        <v>1478990.4199602341</v>
+      </c>
       <c r="Z22" s="9"/>
       <c r="AA22" s="9"/>
       <c r="AB22" s="9"/>
@@ -2501,7 +2530,9 @@
       <c r="X23" s="8">
         <v>2295052.1911296258</v>
       </c>
-      <c r="Y23" s="9"/>
+      <c r="Y23" s="8">
+        <v>2581871.5220405483</v>
+      </c>
       <c r="Z23" s="9"/>
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
@@ -2745,7 +2776,9 @@
       <c r="X25" s="11">
         <v>16724759.229938485</v>
       </c>
-      <c r="Y25" s="9"/>
+      <c r="Y25" s="11">
+        <v>18611763.384858873</v>
+      </c>
       <c r="Z25" s="9"/>
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
@@ -2843,6 +2876,7 @@
       <c r="V26" s="12"/>
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
     </row>
     <row r="27" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
@@ -2874,7 +2908,7 @@
       <c r="V28" s="14"/>
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
-      <c r="Y28" s="9"/>
+      <c r="Y28" s="14"/>
       <c r="Z28" s="9"/>
       <c r="AA28" s="9"/>
       <c r="AB28" s="9"/>
@@ -2972,7 +3006,7 @@
       <c r="V29" s="15"/>
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
-      <c r="Y29" s="9"/>
+      <c r="Y29" s="15"/>
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9"/>
@@ -3057,7 +3091,7 @@
     </row>
     <row r="32" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:96" x14ac:dyDescent="0.2">
@@ -3067,7 +3101,7 @@
     </row>
     <row r="35" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:96" x14ac:dyDescent="0.2">
@@ -3102,6 +3136,7 @@
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
+      <c r="Y38" s="4"/>
     </row>
     <row r="39" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -3176,6 +3211,9 @@
       <c r="X39" s="17">
         <v>2022</v>
       </c>
+      <c r="Y39" s="17">
+        <v>2023</v>
+      </c>
     </row>
     <row r="40" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
@@ -3253,7 +3291,9 @@
       <c r="X41" s="8">
         <v>5455159.0229229797</v>
       </c>
-      <c r="Y41"/>
+      <c r="Y41" s="8">
+        <v>5479666.1405735118</v>
+      </c>
       <c r="Z41" s="9"/>
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
@@ -3399,7 +3439,9 @@
       <c r="X42" s="8">
         <v>212289.07465789252</v>
       </c>
-      <c r="Y42"/>
+      <c r="Y42" s="8">
+        <v>209135.37465100674</v>
+      </c>
       <c r="Z42" s="9"/>
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
@@ -3545,7 +3587,9 @@
       <c r="X43" s="8">
         <v>256454.83999876378</v>
       </c>
-      <c r="Y43"/>
+      <c r="Y43" s="8">
+        <v>232210.01918775839</v>
+      </c>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
@@ -3691,7 +3735,9 @@
       <c r="X44" s="8">
         <v>1851506.0393151762</v>
       </c>
-      <c r="Y44"/>
+      <c r="Y44" s="8">
+        <v>1939960.9296062016</v>
+      </c>
       <c r="Z44" s="9"/>
       <c r="AA44" s="9"/>
       <c r="AB44" s="9"/>
@@ -3837,7 +3883,9 @@
       <c r="X45" s="8">
         <v>413086.03240013786</v>
       </c>
-      <c r="Y45"/>
+      <c r="Y45" s="8">
+        <v>407341.24639938149</v>
+      </c>
       <c r="Z45" s="9"/>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
@@ -3983,7 +4031,9 @@
       <c r="X46" s="8">
         <v>640402.80102581426</v>
       </c>
-      <c r="Y46"/>
+      <c r="Y46" s="8">
+        <v>686399.04521566012</v>
+      </c>
       <c r="Z46" s="9"/>
       <c r="AA46" s="9"/>
       <c r="AB46" s="9"/>
@@ -4129,7 +4179,9 @@
       <c r="X47" s="8">
         <v>1172803.2083973573</v>
       </c>
-      <c r="Y47"/>
+      <c r="Y47" s="8">
+        <v>1373531.1509577949</v>
+      </c>
       <c r="Z47" s="9"/>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9"/>
@@ -4275,7 +4327,9 @@
       <c r="X48" s="8">
         <v>466812.65729031921</v>
       </c>
-      <c r="Y48"/>
+      <c r="Y48" s="8">
+        <v>488949.2762005449</v>
+      </c>
       <c r="Z48" s="9"/>
       <c r="AA48" s="9"/>
       <c r="AB48" s="9"/>
@@ -4421,7 +4475,9 @@
       <c r="X49" s="8">
         <v>225117.50566663369</v>
       </c>
-      <c r="Y49"/>
+      <c r="Y49" s="8">
+        <v>262383.94555467163</v>
+      </c>
       <c r="Z49" s="9"/>
       <c r="AA49" s="9"/>
       <c r="AB49" s="9"/>
@@ -4567,7 +4623,9 @@
       <c r="X50" s="8">
         <v>790083.71505532251</v>
       </c>
-      <c r="Y50"/>
+      <c r="Y50" s="8">
+        <v>845826.74123924901</v>
+      </c>
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
       <c r="AB50" s="9"/>
@@ -4713,7 +4771,9 @@
       <c r="X51" s="8">
         <v>1016009.2133631294</v>
       </c>
-      <c r="Y51"/>
+      <c r="Y51" s="8">
+        <v>1212104.1001562546</v>
+      </c>
       <c r="Z51" s="9"/>
       <c r="AA51" s="9"/>
       <c r="AB51" s="9"/>
@@ -4859,7 +4919,9 @@
       <c r="X52" s="8">
         <v>2070492.9913601633</v>
       </c>
-      <c r="Y52"/>
+      <c r="Y52" s="8">
+        <v>2246452.2737255702</v>
+      </c>
       <c r="Z52" s="9"/>
       <c r="AA52" s="9"/>
       <c r="AB52" s="9"/>
@@ -5103,7 +5165,9 @@
       <c r="X54" s="11">
         <v>14570217.10145369</v>
       </c>
-      <c r="Y54" s="9"/>
+      <c r="Y54" s="11">
+        <v>15383960.243467607</v>
+      </c>
       <c r="Z54" s="9"/>
       <c r="AA54" s="9"/>
       <c r="AB54" s="9"/>
@@ -5201,6 +5265,7 @@
       <c r="V55" s="12"/>
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
+      <c r="Y55" s="12"/>
     </row>
     <row r="56" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
@@ -5330,7 +5395,7 @@
       <c r="V58" s="16"/>
       <c r="W58" s="16"/>
       <c r="X58" s="16"/>
-      <c r="Y58" s="9"/>
+      <c r="Y58" s="16"/>
       <c r="Z58" s="9"/>
       <c r="AA58" s="9"/>
       <c r="AB58" s="9"/>
@@ -5415,7 +5480,7 @@
     </row>
     <row r="61" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:96" x14ac:dyDescent="0.2">
@@ -5425,7 +5490,7 @@
     </row>
     <row r="64" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:91" x14ac:dyDescent="0.2">
@@ -5460,6 +5525,7 @@
       <c r="V67" s="4"/>
       <c r="W67" s="4"/>
       <c r="X67" s="4"/>
+      <c r="Y67" s="4"/>
     </row>
     <row r="68" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -5531,7 +5597,10 @@
       <c r="W68" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X68" s="17"/>
+      <c r="X68" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y68" s="17"/>
     </row>
     <row r="69" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
@@ -5606,8 +5675,10 @@
       <c r="W70" s="18">
         <v>12.432995660269299</v>
       </c>
-      <c r="X70" s="18"/>
-      <c r="Y70" s="9"/>
+      <c r="X70" s="18">
+        <v>8.1191269210852965</v>
+      </c>
+      <c r="Y70" s="18"/>
       <c r="Z70" s="9"/>
       <c r="AA70" s="9"/>
       <c r="AB70" s="9"/>
@@ -5745,8 +5816,10 @@
       <c r="W71" s="18">
         <v>9.0258664456113138</v>
       </c>
-      <c r="X71" s="18"/>
-      <c r="Y71" s="9"/>
+      <c r="X71" s="18">
+        <v>7.8892548503947495</v>
+      </c>
+      <c r="Y71" s="18"/>
       <c r="Z71" s="9"/>
       <c r="AA71" s="9"/>
       <c r="AB71" s="9"/>
@@ -5884,8 +5957,10 @@
       <c r="W72" s="18">
         <v>7.8100847700103913</v>
       </c>
-      <c r="X72" s="18"/>
-      <c r="Y72" s="9"/>
+      <c r="X72" s="18">
+        <v>-5.5369400661633961</v>
+      </c>
+      <c r="Y72" s="18"/>
       <c r="Z72" s="9"/>
       <c r="AA72" s="9"/>
       <c r="AB72" s="9"/>
@@ -6023,8 +6098,10 @@
       <c r="W73" s="18">
         <v>11.656594648526792</v>
       </c>
-      <c r="X73" s="18"/>
-      <c r="Y73" s="9"/>
+      <c r="X73" s="18">
+        <v>9.8205364537581374</v>
+      </c>
+      <c r="Y73" s="18"/>
       <c r="Z73" s="9"/>
       <c r="AA73" s="9"/>
       <c r="AB73" s="9"/>
@@ -6162,8 +6239,10 @@
       <c r="W74" s="18">
         <v>12.335596806171267</v>
       </c>
-      <c r="X74" s="18"/>
-      <c r="Y74" s="9"/>
+      <c r="X74" s="18">
+        <v>3.5995937043195312</v>
+      </c>
+      <c r="Y74" s="18"/>
       <c r="Z74" s="9"/>
       <c r="AA74" s="9"/>
       <c r="AB74" s="9"/>
@@ -6301,8 +6380,10 @@
       <c r="W75" s="18">
         <v>5.3758391790115212</v>
       </c>
-      <c r="X75" s="18"/>
-      <c r="Y75" s="9"/>
+      <c r="X75" s="18">
+        <v>11.321069477203466</v>
+      </c>
+      <c r="Y75" s="18"/>
       <c r="Z75" s="9"/>
       <c r="AA75" s="9"/>
       <c r="AB75" s="9"/>
@@ -6440,8 +6521,10 @@
       <c r="W76" s="18">
         <v>31.548347259796572</v>
       </c>
-      <c r="X76" s="18"/>
-      <c r="Y76" s="9"/>
+      <c r="X76" s="18">
+        <v>19.011906073277032</v>
+      </c>
+      <c r="Y76" s="18"/>
       <c r="Z76" s="9"/>
       <c r="AA76" s="9"/>
       <c r="AB76" s="9"/>
@@ -6579,8 +6662,10 @@
       <c r="W77" s="18">
         <v>8.0374204105474689</v>
       </c>
-      <c r="X77" s="18"/>
-      <c r="Y77" s="9"/>
+      <c r="X77" s="18">
+        <v>5.4471435745344365</v>
+      </c>
+      <c r="Y77" s="18"/>
       <c r="Z77" s="9"/>
       <c r="AA77" s="9"/>
       <c r="AB77" s="9"/>
@@ -6718,8 +6803,10 @@
       <c r="W78" s="18">
         <v>28.499761719736796</v>
       </c>
-      <c r="X78" s="18"/>
-      <c r="Y78" s="9"/>
+      <c r="X78" s="18">
+        <v>21.420146103575476</v>
+      </c>
+      <c r="Y78" s="18"/>
       <c r="Z78" s="9"/>
       <c r="AA78" s="9"/>
       <c r="AB78" s="9"/>
@@ -6857,8 +6944,10 @@
       <c r="W79" s="18">
         <v>10.891557015517691</v>
       </c>
-      <c r="X79" s="18"/>
-      <c r="Y79" s="9"/>
+      <c r="X79" s="18">
+        <v>10.864602608087367</v>
+      </c>
+      <c r="Y79" s="18"/>
       <c r="Z79" s="9"/>
       <c r="AA79" s="9"/>
       <c r="AB79" s="9"/>
@@ -6996,8 +7085,10 @@
       <c r="W80" s="18">
         <v>33.69064340121065</v>
       </c>
-      <c r="X80" s="18"/>
-      <c r="Y80" s="9"/>
+      <c r="X80" s="18">
+        <v>27.333167234518015</v>
+      </c>
+      <c r="Y80" s="18"/>
       <c r="Z80" s="9"/>
       <c r="AA80" s="9"/>
       <c r="AB80" s="9"/>
@@ -7135,8 +7226,10 @@
       <c r="W81" s="18">
         <v>11.524711919512384</v>
       </c>
-      <c r="X81" s="18"/>
-      <c r="Y81" s="9"/>
+      <c r="X81" s="18">
+        <v>12.497290127844536</v>
+      </c>
+      <c r="Y81" s="18"/>
       <c r="Z81" s="9"/>
       <c r="AA81" s="9"/>
       <c r="AB81" s="9"/>
@@ -7367,8 +7460,10 @@
       <c r="W83" s="18">
         <v>14.486127874048378</v>
       </c>
-      <c r="X83" s="18"/>
-      <c r="Y83" s="9"/>
+      <c r="X83" s="18">
+        <v>11.282698477013156</v>
+      </c>
+      <c r="Y83" s="18"/>
       <c r="Z83" s="9"/>
       <c r="AA83" s="9"/>
       <c r="AB83" s="9"/>
@@ -7461,6 +7556,7 @@
       <c r="V84" s="12"/>
       <c r="W84" s="12"/>
       <c r="X84" s="12"/>
+      <c r="Y84" s="12"/>
     </row>
     <row r="85" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
@@ -7665,7 +7761,7 @@
     </row>
     <row r="90" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:91" x14ac:dyDescent="0.2">
@@ -7675,7 +7771,7 @@
     </row>
     <row r="93" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:91" x14ac:dyDescent="0.2">
@@ -7710,6 +7806,7 @@
       <c r="V96" s="4"/>
       <c r="W96" s="4"/>
       <c r="X96" s="4"/>
+      <c r="Y96" s="4"/>
     </row>
     <row r="97" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
@@ -7781,7 +7878,10 @@
       <c r="W97" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="X97" s="17"/>
+      <c r="X97" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y97" s="17"/>
     </row>
     <row r="98" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
@@ -7856,8 +7956,10 @@
       <c r="W99" s="18">
         <v>5.7205145920481471</v>
       </c>
-      <c r="X99" s="18"/>
-      <c r="Y99" s="9"/>
+      <c r="X99" s="18">
+        <v>0.44924662228086731</v>
+      </c>
+      <c r="Y99" s="18"/>
       <c r="Z99" s="9"/>
       <c r="AA99" s="9"/>
       <c r="AB99" s="9"/>
@@ -7995,8 +8097,10 @@
       <c r="W100" s="18">
         <v>0.98528699715446066</v>
       </c>
-      <c r="X100" s="18"/>
-      <c r="Y100" s="9"/>
+      <c r="X100" s="18">
+        <v>-1.4855686812748132</v>
+      </c>
+      <c r="Y100" s="18"/>
       <c r="Z100" s="9"/>
       <c r="AA100" s="9"/>
       <c r="AB100" s="9"/>
@@ -8134,8 +8238,10 @@
       <c r="W101" s="18">
         <v>4.8956230982253288</v>
       </c>
-      <c r="X101" s="18"/>
-      <c r="Y101" s="9"/>
+      <c r="X101" s="18">
+        <v>-9.4538363210935188</v>
+      </c>
+      <c r="Y101" s="18"/>
       <c r="Z101" s="9"/>
       <c r="AA101" s="9"/>
       <c r="AB101" s="9"/>
@@ -8273,8 +8379,10 @@
       <c r="W102" s="18">
         <v>4.6909816884363522</v>
       </c>
-      <c r="X102" s="18"/>
-      <c r="Y102" s="9"/>
+      <c r="X102" s="18">
+        <v>4.7774562120112023</v>
+      </c>
+      <c r="Y102" s="18"/>
       <c r="Z102" s="9"/>
       <c r="AA102" s="9"/>
       <c r="AB102" s="9"/>
@@ -8412,8 +8520,10 @@
       <c r="W103" s="18">
         <v>8.7849277177019474</v>
       </c>
-      <c r="X103" s="18"/>
-      <c r="Y103" s="9"/>
+      <c r="X103" s="18">
+        <v>-1.3906996485399645</v>
+      </c>
+      <c r="Y103" s="18"/>
       <c r="Z103" s="9"/>
       <c r="AA103" s="9"/>
       <c r="AB103" s="9"/>
@@ -8551,8 +8661,10 @@
       <c r="W104" s="18">
         <v>2.6155828187484929</v>
       </c>
-      <c r="X104" s="18"/>
-      <c r="Y104" s="9"/>
+      <c r="X104" s="18">
+        <v>7.1823927247300929</v>
+      </c>
+      <c r="Y104" s="18"/>
       <c r="Z104" s="9"/>
       <c r="AA104" s="9"/>
       <c r="AB104" s="9"/>
@@ -8690,8 +8802,10 @@
       <c r="W105" s="18">
         <v>16.558531141374516</v>
       </c>
-      <c r="X105" s="18"/>
-      <c r="Y105" s="9"/>
+      <c r="X105" s="18">
+        <v>17.11522795326708</v>
+      </c>
+      <c r="Y105" s="18"/>
       <c r="Z105" s="9"/>
       <c r="AA105" s="9"/>
       <c r="AB105" s="9"/>
@@ -8829,8 +8943,10 @@
       <c r="W106" s="18">
         <v>7.3828360474272046</v>
       </c>
-      <c r="X106" s="18"/>
-      <c r="Y106" s="9"/>
+      <c r="X106" s="18">
+        <v>4.7420776974473853</v>
+      </c>
+      <c r="Y106" s="18"/>
       <c r="Z106" s="9"/>
       <c r="AA106" s="9"/>
       <c r="AB106" s="9"/>
@@ -8968,8 +9084,10 @@
       <c r="W107" s="18">
         <v>25.561433227308996</v>
       </c>
-      <c r="X107" s="18"/>
-      <c r="Y107" s="9"/>
+      <c r="X107" s="18">
+        <v>16.554216775670966</v>
+      </c>
+      <c r="Y107" s="18"/>
       <c r="Z107" s="9"/>
       <c r="AA107" s="9"/>
       <c r="AB107" s="9"/>
@@ -9107,8 +9225,10 @@
       <c r="W108" s="18">
         <v>8.8173136895126589</v>
       </c>
-      <c r="X108" s="18"/>
-      <c r="Y108" s="9"/>
+      <c r="X108" s="18">
+        <v>7.0553316214122077</v>
+      </c>
+      <c r="Y108" s="18"/>
       <c r="Z108" s="9"/>
       <c r="AA108" s="9"/>
       <c r="AB108" s="9"/>
@@ -9246,8 +9366,10 @@
       <c r="W109" s="18">
         <v>27.977248803934842</v>
       </c>
-      <c r="X109" s="18"/>
-      <c r="Y109" s="9"/>
+      <c r="X109" s="18">
+        <v>19.300502811783019</v>
+      </c>
+      <c r="Y109" s="18"/>
       <c r="Z109" s="9"/>
       <c r="AA109" s="9"/>
       <c r="AB109" s="9"/>
@@ -9385,8 +9507,10 @@
       <c r="W110" s="18">
         <v>7.3952145759382546</v>
       </c>
-      <c r="X110" s="18"/>
-      <c r="Y110" s="9"/>
+      <c r="X110" s="18">
+        <v>8.4984244380278824</v>
+      </c>
+      <c r="Y110" s="18"/>
       <c r="Z110" s="9"/>
       <c r="AA110" s="9"/>
       <c r="AB110" s="9"/>
@@ -9617,8 +9741,10 @@
       <c r="W112" s="18">
         <v>8.2875535900557793</v>
       </c>
-      <c r="X112" s="18"/>
-      <c r="Y112" s="9"/>
+      <c r="X112" s="18">
+        <v>5.5849760943694378</v>
+      </c>
+      <c r="Y112" s="18"/>
       <c r="Z112" s="9"/>
       <c r="AA112" s="9"/>
       <c r="AB112" s="9"/>
@@ -9711,6 +9837,7 @@
       <c r="V113" s="12"/>
       <c r="W113" s="12"/>
       <c r="X113" s="12"/>
+      <c r="Y113" s="12"/>
     </row>
     <row r="114" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
@@ -9912,7 +10039,7 @@
     </row>
     <row r="118" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:96" x14ac:dyDescent="0.2">
@@ -9922,7 +10049,7 @@
     </row>
     <row r="121" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:96" x14ac:dyDescent="0.2">
@@ -9957,6 +10084,7 @@
       <c r="V124" s="4"/>
       <c r="W124" s="4"/>
       <c r="X124" s="4"/>
+      <c r="Y124" s="4"/>
     </row>
     <row r="125" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
@@ -10031,6 +10159,9 @@
       <c r="X125" s="17">
         <v>2022</v>
       </c>
+      <c r="Y125" s="17">
+        <v>2023</v>
+      </c>
     </row>
     <row r="126" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
@@ -10108,7 +10239,9 @@
       <c r="X127" s="18">
         <v>116.07606144850794</v>
       </c>
-      <c r="Y127" s="9"/>
+      <c r="Y127" s="18">
+        <v>124.93913933912148</v>
+      </c>
       <c r="Z127" s="9"/>
       <c r="AA127" s="9"/>
       <c r="AB127" s="9"/>
@@ -10254,7 +10387,9 @@
       <c r="X128" s="18">
         <v>155.05637651659322</v>
       </c>
-      <c r="Y128" s="9"/>
+      <c r="Y128" s="18">
+        <v>169.81184074497858</v>
+      </c>
       <c r="Z128" s="9"/>
       <c r="AA128" s="9"/>
       <c r="AB128" s="9"/>
@@ -10400,7 +10535,9 @@
       <c r="X129" s="18">
         <v>108.91410241337849</v>
       </c>
-      <c r="Y129" s="9"/>
+      <c r="Y129" s="18">
+        <v>113.62556916712036</v>
+      </c>
       <c r="Z129" s="9"/>
       <c r="AA129" s="9"/>
       <c r="AB129" s="9"/>
@@ -10546,7 +10683,9 @@
       <c r="X130" s="18">
         <v>112.67476711324595</v>
       </c>
-      <c r="Y130" s="9"/>
+      <c r="Y130" s="18">
+        <v>118.09795557682605</v>
+      </c>
       <c r="Z130" s="9"/>
       <c r="AA130" s="9"/>
       <c r="AB130" s="9"/>
@@ -10692,7 +10831,9 @@
       <c r="X131" s="18">
         <v>112.63430716914151</v>
       </c>
-      <c r="Y131" s="9"/>
+      <c r="Y131" s="18">
+        <v>118.33436012932641</v>
+      </c>
       <c r="Z131" s="9"/>
       <c r="AA131" s="9"/>
       <c r="AB131" s="9"/>
@@ -10838,7 +10979,9 @@
       <c r="X132" s="18">
         <v>111.98832305880113</v>
       </c>
-      <c r="Y132" s="9"/>
+      <c r="Y132" s="18">
+        <v>116.31257312832768</v>
+      </c>
       <c r="Z132" s="9"/>
       <c r="AA132" s="9"/>
       <c r="AB132" s="9"/>
@@ -10984,7 +11127,9 @@
       <c r="X133" s="18">
         <v>129.30912128383244</v>
       </c>
-      <c r="Y133" s="9"/>
+      <c r="Y133" s="18">
+        <v>131.40327919431888</v>
+      </c>
       <c r="Z133" s="9"/>
       <c r="AA133" s="9"/>
       <c r="AB133" s="9"/>
@@ -11130,7 +11275,9 @@
       <c r="X134" s="18">
         <v>101.20197870572743</v>
       </c>
-      <c r="Y134" s="9"/>
+      <c r="Y134" s="18">
+        <v>101.88321458960216</v>
+      </c>
       <c r="Z134" s="9"/>
       <c r="AA134" s="9"/>
       <c r="AB134" s="9"/>
@@ -11276,7 +11423,9 @@
       <c r="X135" s="18">
         <v>105.07849702498622</v>
       </c>
-      <c r="Y135" s="9"/>
+      <c r="Y135" s="18">
+        <v>109.46533565297084</v>
+      </c>
       <c r="Z135" s="9"/>
       <c r="AA135" s="9"/>
       <c r="AB135" s="9"/>
@@ -11422,7 +11571,9 @@
       <c r="X136" s="18">
         <v>105.48621701331027</v>
       </c>
-      <c r="Y136" s="9"/>
+      <c r="Y136" s="18">
+        <v>109.23965535100959</v>
+      </c>
       <c r="Z136" s="9"/>
       <c r="AA136" s="9"/>
       <c r="AB136" s="9"/>
@@ -11568,7 +11719,9 @@
       <c r="X137" s="18">
         <v>114.32104166608532</v>
       </c>
-      <c r="Y137" s="9"/>
+      <c r="Y137" s="18">
+        <v>122.01843222620687</v>
+      </c>
       <c r="Z137" s="9"/>
       <c r="AA137" s="9"/>
       <c r="AB137" s="9"/>
@@ -11714,7 +11867,9 @@
       <c r="X138" s="18">
         <v>110.84568751048722</v>
       </c>
-      <c r="Y138" s="9"/>
+      <c r="Y138" s="18">
+        <v>114.93106496131836</v>
+      </c>
       <c r="Z138" s="9"/>
       <c r="AA138" s="9"/>
       <c r="AB138" s="9"/>
@@ -11958,7 +12113,9 @@
       <c r="X140" s="18">
         <v>114.78730284856107</v>
       </c>
-      <c r="Y140" s="9"/>
+      <c r="Y140" s="18">
+        <v>120.98161390375321</v>
+      </c>
       <c r="Z140" s="9"/>
       <c r="AA140" s="9"/>
       <c r="AB140" s="9"/>
@@ -12056,6 +12213,7 @@
       <c r="V141" s="12"/>
       <c r="W141" s="12"/>
       <c r="X141" s="12"/>
+      <c r="Y141" s="12"/>
     </row>
     <row r="142" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
@@ -12074,7 +12232,7 @@
     </row>
     <row r="147" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="149" spans="1:96" x14ac:dyDescent="0.2">
@@ -12084,7 +12242,7 @@
     </row>
     <row r="150" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="151" spans="1:96" x14ac:dyDescent="0.2">
@@ -12119,6 +12277,7 @@
       <c r="V153" s="4"/>
       <c r="W153" s="4"/>
       <c r="X153" s="4"/>
+      <c r="Y153" s="4"/>
     </row>
     <row r="154" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
@@ -12193,6 +12352,9 @@
       <c r="X154" s="17">
         <v>2022</v>
       </c>
+      <c r="Y154" s="17">
+        <v>2023</v>
+      </c>
     </row>
     <row r="155" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
@@ -12270,7 +12432,9 @@
       <c r="X156" s="18">
         <v>37.860836455133793</v>
       </c>
-      <c r="Y156" s="9"/>
+      <c r="Y156" s="18">
+        <v>36.78451940915707</v>
+      </c>
       <c r="Z156" s="9"/>
       <c r="AA156" s="9"/>
       <c r="AB156" s="9"/>
@@ -12416,7 +12580,9 @@
       <c r="X157" s="18">
         <v>1.9681464012701617</v>
       </c>
-      <c r="Y157" s="9"/>
+      <c r="Y157" s="18">
+        <v>1.9081299391152491</v>
+      </c>
       <c r="Z157" s="9"/>
       <c r="AA157" s="9"/>
       <c r="AB157" s="9"/>
@@ -12562,7 +12728,9 @@
       <c r="X158" s="18">
         <v>1.6700717973884214</v>
       </c>
-      <c r="Y158" s="9"/>
+      <c r="Y158" s="18">
+        <v>1.4176515707255246</v>
+      </c>
       <c r="Z158" s="9"/>
       <c r="AA158" s="9"/>
       <c r="AB158" s="9"/>
@@ -12708,7 +12876,9 @@
       <c r="X159" s="18">
         <v>12.47360329200824</v>
       </c>
-      <c r="Y159" s="9"/>
+      <c r="Y159" s="18">
+        <v>12.309710528116549</v>
+      </c>
       <c r="Z159" s="9"/>
       <c r="AA159" s="9"/>
       <c r="AB159" s="9"/>
@@ -12854,7 +13024,9 @@
       <c r="X160" s="18">
         <v>2.7819628624220383</v>
       </c>
-      <c r="Y160" s="9"/>
+      <c r="Y160" s="18">
+        <v>2.5898924647928303</v>
+      </c>
       <c r="Z160" s="9"/>
       <c r="AA160" s="9"/>
       <c r="AB160" s="9"/>
@@ -13000,7 +13172,9 @@
       <c r="X161" s="18">
         <v>4.2881117021200792</v>
       </c>
-      <c r="Y161" s="9"/>
+      <c r="Y161" s="18">
+        <v>4.2895902710008667</v>
+      </c>
       <c r="Z161" s="9"/>
       <c r="AA161" s="9"/>
       <c r="AB161" s="9"/>
@@ -13146,7 +13320,9 @@
       <c r="X162" s="18">
         <v>9.067643380195884</v>
       </c>
-      <c r="Y162" s="9"/>
+      <c r="Y162" s="18">
+        <v>9.6974420735560987</v>
+      </c>
       <c r="Z162" s="9"/>
       <c r="AA162" s="9"/>
       <c r="AB162" s="9"/>
@@ -13292,7 +13468,9 @@
       <c r="X163" s="18">
         <v>2.824696245437829</v>
       </c>
-      <c r="Y163" s="9"/>
+      <c r="Y163" s="18">
+        <v>2.6765719615314416</v>
+      </c>
       <c r="Z163" s="9"/>
       <c r="AA163" s="9"/>
       <c r="AB163" s="9"/>
@@ -13438,7 +13616,9 @@
       <c r="X164" s="18">
         <v>1.4143706838613002</v>
       </c>
-      <c r="Y164" s="9"/>
+      <c r="Y164" s="18">
+        <v>1.5432146904177262</v>
+      </c>
       <c r="Z164" s="9"/>
       <c r="AA164" s="9"/>
       <c r="AB164" s="9"/>
@@ -13584,7 +13764,9 @@
       <c r="X165" s="18">
         <v>4.9832072963907583</v>
       </c>
-      <c r="Y165" s="9"/>
+      <c r="Y165" s="18">
+        <v>4.9644850833860819</v>
+      </c>
       <c r="Z165" s="9"/>
       <c r="AA165" s="9"/>
       <c r="AB165" s="9"/>
@@ -13730,7 +13912,9 @@
       <c r="X166" s="18">
         <v>6.9448671886465254</v>
       </c>
-      <c r="Y166" s="9"/>
+      <c r="Y166" s="18">
+        <v>7.9465356902367947</v>
+      </c>
       <c r="Z166" s="9"/>
       <c r="AA166" s="9"/>
       <c r="AB166" s="9"/>
@@ -13876,7 +14060,9 @@
       <c r="X167" s="18">
         <v>13.722482695124977</v>
       </c>
-      <c r="Y167" s="9"/>
+      <c r="Y167" s="18">
+        <v>13.872256317963746</v>
+      </c>
       <c r="Z167" s="9"/>
       <c r="AA167" s="9"/>
       <c r="AB167" s="9"/>
@@ -14120,7 +14306,9 @@
       <c r="X169" s="18">
         <v>100</v>
       </c>
-      <c r="Y169" s="9"/>
+      <c r="Y169" s="18">
+        <v>100</v>
+      </c>
       <c r="Z169" s="9"/>
       <c r="AA169" s="9"/>
       <c r="AB169" s="9"/>
@@ -14218,6 +14406,7 @@
       <c r="V170" s="12"/>
       <c r="W170" s="12"/>
       <c r="X170" s="12"/>
+      <c r="Y170" s="12"/>
     </row>
     <row r="171" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A171" s="13" t="s">
@@ -14432,7 +14621,7 @@
     </row>
     <row r="176" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="178" spans="1:96" x14ac:dyDescent="0.2">
@@ -14442,7 +14631,7 @@
     </row>
     <row r="179" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="180" spans="1:96" x14ac:dyDescent="0.2">
@@ -14477,6 +14666,7 @@
       <c r="V182" s="4"/>
       <c r="W182" s="4"/>
       <c r="X182" s="4"/>
+      <c r="Y182" s="4"/>
     </row>
     <row r="183" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
@@ -14551,6 +14741,9 @@
       <c r="X183" s="17">
         <v>2022</v>
       </c>
+      <c r="Y183" s="17">
+        <v>2023</v>
+      </c>
     </row>
     <row r="184" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="7"/>
@@ -14628,7 +14821,9 @@
       <c r="X185" s="18">
         <v>37.440478648590016</v>
       </c>
-      <c r="Y185" s="9"/>
+      <c r="Y185" s="18">
+        <v>35.619346734208492</v>
+      </c>
       <c r="Z185" s="9"/>
       <c r="AA185" s="9"/>
       <c r="AB185" s="9"/>
@@ -14774,7 +14969,9 @@
       <c r="X186" s="18">
         <v>1.4570069421732375</v>
       </c>
-      <c r="Y186" s="9"/>
+      <c r="Y186" s="18">
+        <v>1.3594378257692818</v>
+      </c>
       <c r="Z186" s="9"/>
       <c r="AA186" s="9"/>
       <c r="AB186" s="9"/>
@@ -14920,7 +15117,9 @@
       <c r="X187" s="18">
         <v>1.7601305334920299</v>
       </c>
-      <c r="Y187" s="9"/>
+      <c r="Y187" s="18">
+        <v>1.5094294025256614</v>
+      </c>
       <c r="Z187" s="9"/>
       <c r="AA187" s="9"/>
       <c r="AB187" s="9"/>
@@ -15066,7 +15265,9 @@
       <c r="X188" s="18">
         <v>12.707470495621159</v>
       </c>
-      <c r="Y188" s="9"/>
+      <c r="Y188" s="18">
+        <v>12.610283040935153</v>
+      </c>
       <c r="Z188" s="9"/>
       <c r="AA188" s="9"/>
       <c r="AB188" s="9"/>
@@ -15212,7 +15413,9 @@
       <c r="X189" s="18">
         <v>2.8351398577233535</v>
       </c>
-      <c r="Y189" s="9"/>
+      <c r="Y189" s="18">
+        <v>2.6478308572875324</v>
+      </c>
       <c r="Z189" s="9"/>
       <c r="AA189" s="9"/>
       <c r="AB189" s="9"/>
@@ -15358,7 +15561,9 @@
       <c r="X190" s="18">
         <v>4.3952866080624178</v>
       </c>
-      <c r="Y190" s="9"/>
+      <c r="Y190" s="18">
+        <v>4.4617837952819812</v>
+      </c>
       <c r="Z190" s="9"/>
       <c r="AA190" s="9"/>
       <c r="AB190" s="9"/>
@@ -15504,7 +15709,9 @@
       <c r="X191" s="18">
         <v>8.0493186905248315</v>
       </c>
-      <c r="Y191" s="9"/>
+      <c r="Y191" s="18">
+        <v>8.928332686903742</v>
+      </c>
       <c r="Z191" s="9"/>
       <c r="AA191" s="9"/>
       <c r="AB191" s="9"/>
@@ -15650,7 +15857,9 @@
       <c r="X192" s="18">
         <v>3.2038826466336228</v>
       </c>
-      <c r="Y192" s="9"/>
+      <c r="Y192" s="18">
+        <v>3.1783056408259007</v>
+      </c>
       <c r="Z192" s="9"/>
       <c r="AA192" s="9"/>
       <c r="AB192" s="9"/>
@@ -15796,7 +16005,9 @@
       <c r="X193" s="18">
         <v>1.545052514311358</v>
       </c>
-      <c r="Y193" s="9"/>
+      <c r="Y193" s="18">
+        <v>1.7055682763226463</v>
+      </c>
       <c r="Z193" s="9"/>
       <c r="AA193" s="9"/>
       <c r="AB193" s="9"/>
@@ -15942,7 +16153,9 @@
       <c r="X194" s="18">
         <v>5.4225939775220979</v>
       </c>
-      <c r="Y194" s="9"/>
+      <c r="Y194" s="18">
+        <v>5.49810795044408</v>
+      </c>
       <c r="Z194" s="9"/>
       <c r="AA194" s="9"/>
       <c r="AB194" s="9"/>
@@ -16088,7 +16301,9 @@
       <c r="X195" s="18">
         <v>6.973192000425037</v>
       </c>
-      <c r="Y195" s="9"/>
+      <c r="Y195" s="18">
+        <v>7.8790121722457167</v>
+      </c>
       <c r="Z195" s="9"/>
       <c r="AA195" s="9"/>
       <c r="AB195" s="9"/>
@@ -16234,7 +16449,9 @@
       <c r="X196" s="18">
         <v>14.210447084920839</v>
       </c>
-      <c r="Y196" s="9"/>
+      <c r="Y196" s="18">
+        <v>14.602561617249805</v>
+      </c>
       <c r="Z196" s="9"/>
       <c r="AA196" s="9"/>
       <c r="AB196" s="9"/>
@@ -16478,7 +16695,9 @@
       <c r="X198" s="18">
         <v>100</v>
       </c>
-      <c r="Y198" s="9"/>
+      <c r="Y198" s="18">
+        <v>100</v>
+      </c>
       <c r="Z198" s="9"/>
       <c r="AA198" s="9"/>
       <c r="AB198" s="9"/>
@@ -16576,6 +16795,7 @@
       <c r="V199" s="12"/>
       <c r="W199" s="12"/>
       <c r="X199" s="12"/>
+      <c r="Y199" s="12"/>
     </row>
     <row r="200" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A200" s="13" t="s">
@@ -16771,9 +16991,9 @@
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="23" man="1"/>
-    <brk id="116" max="23" man="1"/>
-    <brk id="144" max="23" man="1"/>
+    <brk id="58" max="24" man="1"/>
+    <brk id="116" max="24" man="1"/>
+    <brk id="144" max="24" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q1 2024 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2024\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2024\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42466AC0-7B75-4DED-A854-D88C81F844C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06820CE3-41CC-45B0-A911-1149853BD3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="975" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -214,13 +214,13 @@
     <t>2022 - 2023</t>
   </si>
   <si>
-    <t>As of January 2024</t>
-  </si>
-  <si>
     <t>Annual 2000 to 2023</t>
   </si>
   <si>
     <t>Annual 2001 to 2023</t>
+  </si>
+  <si>
+    <t>As of April 2024</t>
   </si>
 </sst>
 </file>
@@ -677,50 +677,50 @@
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
-    <col min="2" max="25" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="7.77734375" style="1"/>
+    <col min="1" max="1" width="38.90625" style="1" customWidth="1"/>
+    <col min="2" max="25" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="7.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>30</v>
@@ -749,7 +749,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -826,10 +826,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="11" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -900,10 +900,10 @@
         <v>5631917.6611599475</v>
       </c>
       <c r="X12" s="8">
-        <v>6332133.7395619042</v>
+        <v>6332466.545114967</v>
       </c>
       <c r="Y12" s="8">
-        <v>6846247.7146898005</v>
+        <v>6848907.220050659</v>
       </c>
       <c r="Z12" s="9"/>
       <c r="AA12" s="9"/>
@@ -977,7 +977,7 @@
       <c r="CQ12" s="9"/>
       <c r="CR12" s="9"/>
     </row>
-    <row r="13" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1048,10 +1048,10 @@
         <v>301917.11163271719</v>
       </c>
       <c r="X13" s="8">
-        <v>329167.74690513348</v>
+        <v>328373.32579338714</v>
       </c>
       <c r="Y13" s="8">
-        <v>355136.62934378185</v>
+        <v>354226.30741373129</v>
       </c>
       <c r="Z13" s="9"/>
       <c r="AA13" s="9"/>
@@ -1125,7 +1125,7 @@
       <c r="CQ13" s="9"/>
       <c r="CR13" s="9"/>
     </row>
-    <row r="14" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1196,10 +1196,10 @@
         <v>259081.0383612804</v>
       </c>
       <c r="X14" s="8">
-        <v>279315.48708031955</v>
+        <v>279995.88461607165</v>
       </c>
       <c r="Y14" s="8">
-        <v>263849.95596516988</v>
+        <v>263342.25406077132</v>
       </c>
       <c r="Z14" s="9"/>
       <c r="AA14" s="9"/>
@@ -1273,7 +1273,7 @@
       <c r="CQ14" s="9"/>
       <c r="CR14" s="9"/>
     </row>
-    <row r="15" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1344,10 +1344,10 @@
         <v>1868389.5245533392</v>
       </c>
       <c r="X15" s="8">
-        <v>2086180.117886059</v>
+        <v>2085782.8103059449</v>
       </c>
       <c r="Y15" s="8">
-        <v>2291054.1968541136</v>
+        <v>2288558.2310069762</v>
       </c>
       <c r="Z15" s="9"/>
       <c r="AA15" s="9"/>
@@ -1421,7 +1421,7 @@
       <c r="CQ15" s="9"/>
       <c r="CR15" s="9"/>
     </row>
-    <row r="16" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -1492,10 +1492,10 @@
         <v>414184.46497346624</v>
       </c>
       <c r="X16" s="8">
-        <v>465276.59060639073</v>
+        <v>464534.41911176633</v>
       </c>
       <c r="Y16" s="8">
-        <v>482024.65746953094</v>
+        <v>482848.52588353655</v>
       </c>
       <c r="Z16" s="9"/>
       <c r="AA16" s="9"/>
@@ -1569,7 +1569,7 @@
       <c r="CQ16" s="9"/>
       <c r="CR16" s="9"/>
     </row>
-    <row r="17" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1640,10 +1640,10 @@
         <v>680588.98821395624</v>
       </c>
       <c r="X17" s="8">
-        <v>717176.35769040021</v>
+        <v>717313.01619522378</v>
       </c>
       <c r="Y17" s="8">
-        <v>798368.39141860767</v>
+        <v>798467.37734682765</v>
       </c>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
@@ -1717,7 +1717,7 @@
       <c r="CQ17" s="9"/>
       <c r="CR17" s="9"/>
     </row>
-    <row r="18" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1788,10 +1788,10 @@
         <v>1152839.6629508231</v>
       </c>
       <c r="X18" s="8">
-        <v>1516541.5231672169</v>
+        <v>1518007.0763492808</v>
       </c>
       <c r="Y18" s="8">
-        <v>1804864.973114013</v>
+        <v>1803606.0854710373</v>
       </c>
       <c r="Z18" s="9"/>
       <c r="AA18" s="9"/>
@@ -1865,7 +1865,7 @@
       <c r="CQ18" s="9"/>
       <c r="CR18" s="9"/>
     </row>
-    <row r="19" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1936,10 +1936,10 @@
         <v>437277.79155718104</v>
       </c>
       <c r="X19" s="8">
-        <v>472423.64602658915</v>
+        <v>471914.65554296359</v>
       </c>
       <c r="Y19" s="8">
-        <v>498157.24030570779</v>
+        <v>497855.48647702747</v>
       </c>
       <c r="Z19" s="9"/>
       <c r="AA19" s="9"/>
@@ -2013,7 +2013,7 @@
       <c r="CQ19" s="9"/>
       <c r="CR19" s="9"/>
     </row>
-    <row r="20" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2084,10 +2084,10 @@
         <v>184086.01566947822</v>
       </c>
       <c r="X20" s="8">
-        <v>236550.09149463687</v>
+        <v>236099.86822459626</v>
       </c>
       <c r="Y20" s="8">
-        <v>287219.46670092957</v>
+        <v>286984.02428991569</v>
       </c>
       <c r="Z20" s="9"/>
       <c r="AA20" s="9"/>
@@ -2161,7 +2161,7 @@
       <c r="CQ20" s="9"/>
       <c r="CR20" s="9"/>
     </row>
-    <row r="21" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2232,10 +2232,10 @@
         <v>751571.57558303094</v>
       </c>
       <c r="X21" s="8">
-        <v>833429.42225008144</v>
+        <v>831462.5111797424</v>
       </c>
       <c r="Y21" s="8">
-        <v>923978.21699643123</v>
+        <v>923610.22288231843</v>
       </c>
       <c r="Z21" s="9"/>
       <c r="AA21" s="9"/>
@@ -2309,7 +2309,7 @@
       <c r="CQ21" s="9"/>
       <c r="CR21" s="9"/>
     </row>
-    <row r="22" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2380,10 +2380,10 @@
         <v>868805.98865425971</v>
       </c>
       <c r="X22" s="8">
-        <v>1161512.316140129</v>
+        <v>1163319.6035454657</v>
       </c>
       <c r="Y22" s="8">
-        <v>1478990.4199602341</v>
+        <v>1478999.5195481982</v>
       </c>
       <c r="Z22" s="9"/>
       <c r="AA22" s="9"/>
@@ -2457,7 +2457,7 @@
       <c r="CQ22" s="9"/>
       <c r="CR22" s="9"/>
     </row>
-    <row r="23" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -2528,10 +2528,10 @@
         <v>2057886.6796678836</v>
       </c>
       <c r="X23" s="8">
-        <v>2295052.1911296258</v>
+        <v>2295775.0077454327</v>
       </c>
       <c r="Y23" s="8">
-        <v>2581871.5220405483</v>
+        <v>2580923.9259518366</v>
       </c>
       <c r="Z23" s="9"/>
       <c r="AA23" s="9"/>
@@ -2605,7 +2605,7 @@
       <c r="CQ23" s="9"/>
       <c r="CR23" s="9"/>
     </row>
-    <row r="24" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2703,7 +2703,7 @@
       <c r="CQ24" s="9"/>
       <c r="CR24" s="9"/>
     </row>
-    <row r="25" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
@@ -2774,10 +2774,10 @@
         <v>14608546.502977364</v>
       </c>
       <c r="X25" s="11">
-        <v>16724759.229938485</v>
+        <v>16725044.723724842</v>
       </c>
       <c r="Y25" s="11">
-        <v>18611763.384858873</v>
+        <v>18608329.180382837</v>
       </c>
       <c r="Z25" s="9"/>
       <c r="AA25" s="9"/>
@@ -2851,7 +2851,7 @@
       <c r="CQ25" s="9"/>
       <c r="CR25" s="9"/>
     </row>
-    <row r="26" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -2878,12 +2878,12 @@
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2981,7 +2981,7 @@
       <c r="CQ28" s="9"/>
       <c r="CR28" s="9"/>
     </row>
-    <row r="29" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3079,37 +3079,37 @@
       <c r="CQ29" s="9"/>
       <c r="CR29" s="9"/>
     </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
         <v>30</v>
@@ -3138,7 +3138,7 @@
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
     </row>
-    <row r="39" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>51</v>
       </c>
@@ -3215,10 +3215,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="40" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -3289,10 +3289,10 @@
         <v>5159981.5267388932</v>
       </c>
       <c r="X41" s="8">
-        <v>5455159.0229229797</v>
+        <v>5455458.12541545</v>
       </c>
       <c r="Y41" s="8">
-        <v>5479666.1405735118</v>
+        <v>5481802.1240293887</v>
       </c>
       <c r="Z41" s="9"/>
       <c r="AA41" s="9"/>
@@ -3366,7 +3366,7 @@
       <c r="CQ41" s="9"/>
       <c r="CR41" s="9"/>
     </row>
-    <row r="42" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -3437,10 +3437,10 @@
         <v>210217.82575502741</v>
       </c>
       <c r="X42" s="8">
-        <v>212289.07465789252</v>
+        <v>211802.0002579182</v>
       </c>
       <c r="Y42" s="8">
-        <v>209135.37465100674</v>
+        <v>208588.49027010356</v>
       </c>
       <c r="Z42" s="9"/>
       <c r="AA42" s="9"/>
@@ -3514,7 +3514,7 @@
       <c r="CQ42" s="9"/>
       <c r="CR42" s="9"/>
     </row>
-    <row r="43" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -3585,10 +3585,10 @@
         <v>244485.73965628369</v>
       </c>
       <c r="X43" s="8">
-        <v>256454.83999876378</v>
+        <v>257074.46180447156</v>
       </c>
       <c r="Y43" s="8">
-        <v>232210.01918775839</v>
+        <v>231770.69883863215</v>
       </c>
       <c r="Z43" s="9"/>
       <c r="AA43" s="9"/>
@@ -3662,7 +3662,7 @@
       <c r="CQ43" s="9"/>
       <c r="CR43" s="9"/>
     </row>
-    <row r="44" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -3733,10 +3733,10 @@
         <v>1768543.9657307984</v>
       </c>
       <c r="X44" s="8">
-        <v>1851506.0393151762</v>
+        <v>1851187.4687877942</v>
       </c>
       <c r="Y44" s="8">
-        <v>1939960.9296062016</v>
+        <v>1937827.3684991344</v>
       </c>
       <c r="Z44" s="9"/>
       <c r="AA44" s="9"/>
@@ -3810,7 +3810,7 @@
       <c r="CQ44" s="9"/>
       <c r="CR44" s="9"/>
     </row>
-    <row r="45" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>8</v>
       </c>
@@ -3881,10 +3881,10 @@
         <v>379727.26651260047</v>
       </c>
       <c r="X45" s="8">
-        <v>413086.03240013786</v>
+        <v>412423.56734884565</v>
       </c>
       <c r="Y45" s="8">
-        <v>407341.24639938149</v>
+        <v>408026.98579490924</v>
       </c>
       <c r="Z45" s="9"/>
       <c r="AA45" s="9"/>
@@ -3958,7 +3958,7 @@
       <c r="CQ45" s="9"/>
       <c r="CR45" s="9"/>
     </row>
-    <row r="46" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -4029,10 +4029,10 @@
         <v>624079.48523468187</v>
       </c>
       <c r="X46" s="8">
-        <v>640402.80102581426</v>
+        <v>640500.98494482529</v>
       </c>
       <c r="Y46" s="8">
-        <v>686399.04521566012</v>
+        <v>686485.72470534209</v>
       </c>
       <c r="Z46" s="9"/>
       <c r="AA46" s="9"/>
@@ -4106,7 +4106,7 @@
       <c r="CQ46" s="9"/>
       <c r="CR46" s="9"/>
     </row>
-    <row r="47" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -4177,10 +4177,10 @@
         <v>1006192.5085302058</v>
       </c>
       <c r="X47" s="8">
-        <v>1172803.2083973573</v>
+        <v>1173974.1930444073</v>
       </c>
       <c r="Y47" s="8">
-        <v>1373531.1509577949</v>
+        <v>1372568.9105471093</v>
       </c>
       <c r="Z47" s="9"/>
       <c r="AA47" s="9"/>
@@ -4254,7 +4254,7 @@
       <c r="CQ47" s="9"/>
       <c r="CR47" s="9"/>
     </row>
-    <row r="48" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -4325,10 +4325,10 @@
         <v>434718.13045070309</v>
       </c>
       <c r="X48" s="8">
-        <v>466812.65729031921</v>
+        <v>466322.15893102379</v>
       </c>
       <c r="Y48" s="8">
-        <v>488949.2762005449</v>
+        <v>488689.78713736549</v>
       </c>
       <c r="Z48" s="9"/>
       <c r="AA48" s="9"/>
@@ -4402,7 +4402,7 @@
       <c r="CQ48" s="9"/>
       <c r="CR48" s="9"/>
     </row>
-    <row r="49" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -4473,10 +4473,10 @@
         <v>179288.73530703833</v>
       </c>
       <c r="X49" s="8">
-        <v>225117.50566663369</v>
+        <v>224673.14404452546</v>
       </c>
       <c r="Y49" s="8">
-        <v>262383.94555467163</v>
+        <v>262144.38324165763</v>
       </c>
       <c r="Z49" s="9"/>
       <c r="AA49" s="9"/>
@@ -4550,7 +4550,7 @@
       <c r="CQ49" s="9"/>
       <c r="CR49" s="9"/>
     </row>
-    <row r="50" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -4621,10 +4621,10 @@
         <v>726064.34423630452</v>
       </c>
       <c r="X50" s="8">
-        <v>790083.71505532251</v>
+        <v>788210.95003522548</v>
       </c>
       <c r="Y50" s="8">
-        <v>845826.74123924901</v>
+        <v>845511.5781502364</v>
       </c>
       <c r="Z50" s="9"/>
       <c r="AA50" s="9"/>
@@ -4698,7 +4698,7 @@
       <c r="CQ50" s="9"/>
       <c r="CR50" s="9"/>
     </row>
-    <row r="51" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -4769,10 +4769,10 @@
         <v>793898.30837798945</v>
       </c>
       <c r="X51" s="8">
-        <v>1016009.2133631294</v>
+        <v>1017583.8689245896</v>
       </c>
       <c r="Y51" s="8">
-        <v>1212104.1001562546</v>
+        <v>1212135.6754892948</v>
       </c>
       <c r="Z51" s="9"/>
       <c r="AA51" s="9"/>
@@ -4846,7 +4846,7 @@
       <c r="CQ51" s="9"/>
       <c r="CR51" s="9"/>
     </row>
-    <row r="52" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
@@ -4917,10 +4917,10 @@
         <v>1927919.2276264182</v>
       </c>
       <c r="X52" s="8">
-        <v>2070492.9913601633</v>
+        <v>2071137.2785927998</v>
       </c>
       <c r="Y52" s="8">
-        <v>2246452.2737255702</v>
+        <v>2245719.9209137536</v>
       </c>
       <c r="Z52" s="9"/>
       <c r="AA52" s="9"/>
@@ -4994,7 +4994,7 @@
       <c r="CQ52" s="9"/>
       <c r="CR52" s="9"/>
     </row>
-    <row r="53" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -5092,7 +5092,7 @@
       <c r="CQ53" s="9"/>
       <c r="CR53" s="9"/>
     </row>
-    <row r="54" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>18</v>
       </c>
@@ -5163,10 +5163,10 @@
         <v>13455117.064156944</v>
       </c>
       <c r="X54" s="11">
-        <v>14570217.10145369</v>
+        <v>14570348.202131879</v>
       </c>
       <c r="Y54" s="11">
-        <v>15383960.243467607</v>
+        <v>15381271.647616928</v>
       </c>
       <c r="Z54" s="9"/>
       <c r="AA54" s="9"/>
@@ -5240,7 +5240,7 @@
       <c r="CQ54" s="9"/>
       <c r="CR54" s="9"/>
     </row>
-    <row r="55" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -5267,12 +5267,12 @@
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
     </row>
-    <row r="56" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -5370,7 +5370,7 @@
       <c r="CQ57" s="9"/>
       <c r="CR57" s="9"/>
     </row>
-    <row r="58" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -5468,37 +5468,37 @@
       <c r="CQ58" s="9"/>
       <c r="CR58" s="9"/>
     </row>
-    <row r="59" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="65" spans="1:91" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
         <v>30</v>
@@ -5527,7 +5527,7 @@
       <c r="X67" s="4"/>
       <c r="Y67" s="4"/>
     </row>
-    <row r="68" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>51</v>
       </c>
@@ -5602,10 +5602,10 @@
       </c>
       <c r="Y68" s="17"/>
     </row>
-    <row r="69" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
@@ -5673,10 +5673,10 @@
         <v>8.6155967108178118</v>
       </c>
       <c r="W70" s="18">
-        <v>12.432995660269299</v>
+        <v>12.438904936169365</v>
       </c>
       <c r="X70" s="18">
-        <v>8.1191269210852965</v>
+        <v>8.1554426108115621</v>
       </c>
       <c r="Y70" s="18"/>
       <c r="Z70" s="9"/>
@@ -5746,7 +5746,7 @@
       <c r="CL70" s="9"/>
       <c r="CM70" s="9"/>
     </row>
-    <row r="71" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -5814,10 +5814,10 @@
         <v>1.8816164812712088</v>
       </c>
       <c r="W71" s="18">
-        <v>9.0258664456113138</v>
+        <v>8.7627408786468521</v>
       </c>
       <c r="X71" s="18">
-        <v>7.8892548503947495</v>
+        <v>7.8730455824572232</v>
       </c>
       <c r="Y71" s="18"/>
       <c r="Z71" s="9"/>
@@ -5887,7 +5887,7 @@
       <c r="CL71" s="9"/>
       <c r="CM71" s="9"/>
     </row>
-    <row r="72" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
@@ -5955,10 +5955,10 @@
         <v>15.769594196596287</v>
       </c>
       <c r="W72" s="18">
-        <v>7.8100847700103913</v>
+        <v>8.0727043503763269</v>
       </c>
       <c r="X72" s="18">
-        <v>-5.5369400661633961</v>
+        <v>-5.9478126180803343</v>
       </c>
       <c r="Y72" s="18"/>
       <c r="Z72" s="9"/>
@@ -6028,7 +6028,7 @@
       <c r="CL72" s="9"/>
       <c r="CM72" s="9"/>
     </row>
-    <row r="73" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
@@ -6096,10 +6096,10 @@
         <v>5.9914191239633965</v>
       </c>
       <c r="W73" s="18">
-        <v>11.656594648526792</v>
+        <v>11.635329940343993</v>
       </c>
       <c r="X73" s="18">
-        <v>9.8205364537581374</v>
+        <v>9.7217898095194357</v>
       </c>
       <c r="Y73" s="18"/>
       <c r="Z73" s="9"/>
@@ -6169,7 +6169,7 @@
       <c r="CL73" s="9"/>
       <c r="CM73" s="9"/>
     </row>
-    <row r="74" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -6237,10 +6237,10 @@
         <v>5.8338132278838515</v>
       </c>
       <c r="W74" s="18">
-        <v>12.335596806171267</v>
+        <v>12.156408169853904</v>
       </c>
       <c r="X74" s="18">
-        <v>3.5995937043195312</v>
+        <v>3.9424649753162555</v>
       </c>
       <c r="Y74" s="18"/>
       <c r="Z74" s="9"/>
@@ -6310,7 +6310,7 @@
       <c r="CL74" s="9"/>
       <c r="CM74" s="9"/>
     </row>
-    <row r="75" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -6378,10 +6378,10 @@
         <v>17.728344358323383</v>
       </c>
       <c r="W75" s="18">
-        <v>5.3758391790115212</v>
+        <v>5.3959186259596947</v>
       </c>
       <c r="X75" s="18">
-        <v>11.321069477203466</v>
+        <v>11.313660747725351</v>
       </c>
       <c r="Y75" s="18"/>
       <c r="Z75" s="9"/>
@@ -6451,7 +6451,7 @@
       <c r="CL75" s="9"/>
       <c r="CM75" s="9"/>
     </row>
-    <row r="76" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -6519,10 +6519,10 @@
         <v>9.9178464913791942</v>
       </c>
       <c r="W76" s="18">
-        <v>31.548347259796572</v>
+        <v>31.675472759479021</v>
       </c>
       <c r="X76" s="18">
-        <v>19.011906073277032</v>
+        <v>18.814076269565589</v>
       </c>
       <c r="Y76" s="18"/>
       <c r="Z76" s="9"/>
@@ -6592,7 +6592,7 @@
       <c r="CL76" s="9"/>
       <c r="CM76" s="9"/>
     </row>
-    <row r="77" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -6660,10 +6660,10 @@
         <v>9.3377320653113003</v>
       </c>
       <c r="W77" s="18">
-        <v>8.0374204105474689</v>
+        <v>7.9210206085330555</v>
       </c>
       <c r="X77" s="18">
-        <v>5.4471435745344365</v>
+        <v>5.4969326825032567</v>
       </c>
       <c r="Y77" s="18"/>
       <c r="Z77" s="9"/>
@@ -6733,7 +6733,7 @@
       <c r="CL77" s="9"/>
       <c r="CM77" s="9"/>
     </row>
-    <row r="78" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -6801,10 +6801,10 @@
         <v>2.7650727529354242</v>
       </c>
       <c r="W78" s="18">
-        <v>28.499761719736796</v>
+        <v>28.255189491692619</v>
       </c>
       <c r="X78" s="18">
-        <v>21.420146103575476</v>
+        <v>21.551962924822348</v>
       </c>
       <c r="Y78" s="18"/>
       <c r="Z78" s="9"/>
@@ -6874,7 +6874,7 @@
       <c r="CL78" s="9"/>
       <c r="CM78" s="9"/>
     </row>
-    <row r="79" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
@@ -6942,10 +6942,10 @@
         <v>9.9141472177346515</v>
       </c>
       <c r="W79" s="18">
-        <v>10.891557015517691</v>
+        <v>10.629850594700343</v>
       </c>
       <c r="X79" s="18">
-        <v>10.864602608087367</v>
+        <v>11.082605705437018</v>
       </c>
       <c r="Y79" s="18"/>
       <c r="Z79" s="9"/>
@@ -7015,7 +7015,7 @@
       <c r="CL79" s="9"/>
       <c r="CM79" s="9"/>
     </row>
-    <row r="80" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -7083,10 +7083,10 @@
         <v>8.4921142948448249</v>
       </c>
       <c r="W80" s="18">
-        <v>33.69064340121065</v>
+        <v>33.898663077517909</v>
       </c>
       <c r="X80" s="18">
-        <v>27.333167234518015</v>
+        <v>27.136129662100615</v>
       </c>
       <c r="Y80" s="18"/>
       <c r="Z80" s="9"/>
@@ -7156,7 +7156,7 @@
       <c r="CL80" s="9"/>
       <c r="CM80" s="9"/>
     </row>
-    <row r="81" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -7224,10 +7224,10 @@
         <v>6.8441068856295288</v>
       </c>
       <c r="W81" s="18">
-        <v>11.524711919512384</v>
+        <v>11.559836138107542</v>
       </c>
       <c r="X81" s="18">
-        <v>12.497290127844536</v>
+        <v>12.420595103804828</v>
       </c>
       <c r="Y81" s="18"/>
       <c r="Z81" s="9"/>
@@ -7297,7 +7297,7 @@
       <c r="CL81" s="9"/>
       <c r="CM81" s="9"/>
     </row>
-    <row r="82" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -7390,7 +7390,7 @@
       <c r="CL82" s="9"/>
       <c r="CM82" s="9"/>
     </row>
-    <row r="83" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="s">
         <v>18</v>
       </c>
@@ -7458,10 +7458,10 @@
         <v>8.4035676420612475</v>
       </c>
       <c r="W83" s="18">
-        <v>14.486127874048378</v>
+        <v>14.488082166943258</v>
       </c>
       <c r="X83" s="18">
-        <v>11.282698477013156</v>
+        <v>11.260265594306688</v>
       </c>
       <c r="Y83" s="18"/>
       <c r="Z83" s="9"/>
@@ -7531,7 +7531,7 @@
       <c r="CL83" s="9"/>
       <c r="CM83" s="9"/>
     </row>
-    <row r="84" spans="1:91" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:91" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -7558,12 +7558,12 @@
       <c r="X84" s="12"/>
       <c r="Y84" s="12"/>
     </row>
-    <row r="85" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -7656,7 +7656,7 @@
       <c r="CL86" s="9"/>
       <c r="CM86" s="9"/>
     </row>
-    <row r="87" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -7749,37 +7749,37 @@
       <c r="CL87" s="9"/>
       <c r="CM87" s="9"/>
     </row>
-    <row r="88" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="92" spans="1:91" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="92" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="94" spans="1:91" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4" t="s">
         <v>30</v>
@@ -7808,7 +7808,7 @@
       <c r="X96" s="4"/>
       <c r="Y96" s="4"/>
     </row>
-    <row r="97" spans="1:91" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:91" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>51</v>
       </c>
@@ -7883,10 +7883,10 @@
       </c>
       <c r="Y97" s="17"/>
     </row>
-    <row r="98" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
     </row>
-    <row r="99" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
@@ -7954,10 +7954,10 @@
         <v>3.4377921329759289</v>
       </c>
       <c r="W99" s="18">
-        <v>5.7205145920481471</v>
+        <v>5.7263111727320108</v>
       </c>
       <c r="X99" s="18">
-        <v>0.44924662228086731</v>
+        <v>0.48289250890240965</v>
       </c>
       <c r="Y99" s="18"/>
       <c r="Z99" s="9"/>
@@ -8027,7 +8027,7 @@
       <c r="CL99" s="9"/>
       <c r="CM99" s="9"/>
     </row>
-    <row r="100" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>11</v>
       </c>
@@ -8095,10 +8095,10 @@
         <v>-7.6109984229013321</v>
       </c>
       <c r="W100" s="18">
-        <v>0.98528699715446066</v>
+        <v>0.75358714095771973</v>
       </c>
       <c r="X100" s="18">
-        <v>-1.4855686812748132</v>
+        <v>-1.5172236257926954</v>
       </c>
       <c r="Y100" s="18"/>
       <c r="Z100" s="9"/>
@@ -8168,7 +8168,7 @@
       <c r="CL100" s="9"/>
       <c r="CM100" s="9"/>
     </row>
-    <row r="101" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -8236,10 +8236,10 @@
         <v>13.312004457698535</v>
       </c>
       <c r="W101" s="18">
-        <v>4.8956230982253288</v>
+        <v>5.1490619313363766</v>
       </c>
       <c r="X101" s="18">
-        <v>-9.4538363210935188</v>
+        <v>-9.8429703161589117</v>
       </c>
       <c r="Y101" s="18"/>
       <c r="Z101" s="9"/>
@@ -8309,7 +8309,7 @@
       <c r="CL101" s="9"/>
       <c r="CM101" s="9"/>
     </row>
-    <row r="102" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>9</v>
       </c>
@@ -8377,10 +8377,10 @@
         <v>3.1953987899619278</v>
       </c>
       <c r="W102" s="18">
-        <v>4.6909816884363522</v>
+        <v>4.6729685356081063</v>
       </c>
       <c r="X102" s="18">
-        <v>4.7774562120112023</v>
+        <v>4.6802336971346392</v>
       </c>
       <c r="Y102" s="18"/>
       <c r="Z102" s="9"/>
@@ -8450,7 +8450,7 @@
       <c r="CL102" s="9"/>
       <c r="CM102" s="9"/>
     </row>
-    <row r="103" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
         <v>8</v>
       </c>
@@ -8518,10 +8518,10 @@
         <v>3.3295140773784766</v>
       </c>
       <c r="W103" s="18">
-        <v>8.7849277177019474</v>
+        <v>8.6104695974367615</v>
       </c>
       <c r="X103" s="18">
-        <v>-1.3906996485399645</v>
+        <v>-1.0660354795431886</v>
       </c>
       <c r="Y103" s="18"/>
       <c r="Z103" s="9"/>
@@ -8591,7 +8591,7 @@
       <c r="CL103" s="9"/>
       <c r="CM103" s="9"/>
     </row>
-    <row r="104" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -8659,10 +8659,10 @@
         <v>14.188148530513487</v>
       </c>
       <c r="W104" s="18">
-        <v>2.6155828187484929</v>
+        <v>2.6313154171328392</v>
       </c>
       <c r="X104" s="18">
-        <v>7.1823927247300929</v>
+        <v>7.1794955576029338</v>
       </c>
       <c r="Y104" s="18"/>
       <c r="Z104" s="9"/>
@@ -8732,7 +8732,7 @@
       <c r="CL104" s="9"/>
       <c r="CM104" s="9"/>
     </row>
-    <row r="105" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -8800,10 +8800,10 @@
         <v>0.1313093770090461</v>
       </c>
       <c r="W105" s="18">
-        <v>16.558531141374516</v>
+        <v>16.674908935596065</v>
       </c>
       <c r="X105" s="18">
-        <v>17.11522795326708</v>
+        <v>16.916446603284911</v>
       </c>
       <c r="Y105" s="18"/>
       <c r="Z105" s="9"/>
@@ -8873,7 +8873,7 @@
       <c r="CL105" s="9"/>
       <c r="CM105" s="9"/>
     </row>
-    <row r="106" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -8941,10 +8941,10 @@
         <v>9.0700500752324302</v>
       </c>
       <c r="W106" s="18">
-        <v>7.3828360474272046</v>
+        <v>7.2700046919033809</v>
       </c>
       <c r="X106" s="18">
-        <v>4.7420776974473853</v>
+        <v>4.7966041883182839</v>
       </c>
       <c r="Y106" s="18"/>
       <c r="Z106" s="9"/>
@@ -9014,7 +9014,7 @@
       <c r="CL106" s="9"/>
       <c r="CM106" s="9"/>
     </row>
-    <row r="107" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -9082,10 +9082,10 @@
         <v>2.7899697543418256</v>
       </c>
       <c r="W107" s="18">
-        <v>25.561433227308996</v>
+        <v>25.313586299643816</v>
       </c>
       <c r="X107" s="18">
-        <v>16.554216775670966</v>
+        <v>16.678112266816441</v>
       </c>
       <c r="Y107" s="18"/>
       <c r="Z107" s="9"/>
@@ -9155,7 +9155,7 @@
       <c r="CL107" s="9"/>
       <c r="CM107" s="9"/>
     </row>
-    <row r="108" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
@@ -9223,10 +9223,10 @@
         <v>8.8338029267693656</v>
       </c>
       <c r="W108" s="18">
-        <v>8.8173136895126589</v>
+        <v>8.5593799354365103</v>
       </c>
       <c r="X108" s="18">
-        <v>7.0553316214122077</v>
+        <v>7.2697071910064324</v>
       </c>
       <c r="Y108" s="18"/>
       <c r="Z108" s="9"/>
@@ -9296,7 +9296,7 @@
       <c r="CL108" s="9"/>
       <c r="CM108" s="9"/>
     </row>
-    <row r="109" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>2</v>
       </c>
@@ -9364,10 +9364,10 @@
         <v>4.6201866452733782</v>
       </c>
       <c r="W109" s="18">
-        <v>27.977248803934842</v>
+        <v>28.17559354719009</v>
       </c>
       <c r="X109" s="18">
-        <v>19.300502811783019</v>
+        <v>19.118994758664257</v>
       </c>
       <c r="Y109" s="18"/>
       <c r="Z109" s="9"/>
@@ -9437,7 +9437,7 @@
       <c r="CL109" s="9"/>
       <c r="CM109" s="9"/>
     </row>
-    <row r="110" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>1</v>
       </c>
@@ -9505,10 +9505,10 @@
         <v>4.3287095568396978</v>
       </c>
       <c r="W110" s="18">
-        <v>7.3952145759382546</v>
+        <v>7.4286333635826765</v>
       </c>
       <c r="X110" s="18">
-        <v>8.4984244380278824</v>
+        <v>8.4293129250983867</v>
       </c>
       <c r="Y110" s="18"/>
       <c r="Z110" s="9"/>
@@ -9578,7 +9578,7 @@
       <c r="CL110" s="9"/>
       <c r="CM110" s="9"/>
     </row>
-    <row r="111" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -9671,7 +9671,7 @@
       <c r="CL111" s="9"/>
       <c r="CM111" s="9"/>
     </row>
-    <row r="112" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>18</v>
       </c>
@@ -9739,10 +9739,10 @@
         <v>4.2114869311265863</v>
       </c>
       <c r="W112" s="18">
-        <v>8.2875535900557793</v>
+        <v>8.2885279455932448</v>
       </c>
       <c r="X112" s="18">
-        <v>5.5849760943694378</v>
+        <v>5.5655735486568574</v>
       </c>
       <c r="Y112" s="18"/>
       <c r="Z112" s="9"/>
@@ -9812,7 +9812,7 @@
       <c r="CL112" s="9"/>
       <c r="CM112" s="9"/>
     </row>
-    <row r="113" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
@@ -9839,12 +9839,12 @@
       <c r="X113" s="12"/>
       <c r="Y113" s="12"/>
     </row>
-    <row r="114" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -9938,7 +9938,7 @@
       <c r="CM115" s="9"/>
       <c r="CN115" s="9"/>
     </row>
-    <row r="116" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -10032,32 +10032,32 @@
       <c r="CM116" s="9"/>
       <c r="CN116" s="9"/>
     </row>
-    <row r="117" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="120" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="120" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="122" spans="1:96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="122" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4" t="s">
         <v>30</v>
@@ -10086,7 +10086,7 @@
       <c r="X124" s="4"/>
       <c r="Y124" s="4"/>
     </row>
-    <row r="125" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>51</v>
       </c>
@@ -10163,10 +10163,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="126" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
     </row>
-    <row r="127" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>12</v>
       </c>
@@ -10237,10 +10237,10 @@
         <v>109.14608186047747</v>
       </c>
       <c r="X127" s="18">
-        <v>116.07606144850794</v>
+        <v>116.07579784388373</v>
       </c>
       <c r="Y127" s="18">
-        <v>124.93913933912148</v>
+        <v>124.93897198566486</v>
       </c>
       <c r="Z127" s="9"/>
       <c r="AA127" s="9"/>
@@ -10314,7 +10314,7 @@
       <c r="CQ127" s="9"/>
       <c r="CR127" s="9"/>
     </row>
-    <row r="128" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>11</v>
       </c>
@@ -10385,10 +10385,10 @@
         <v>143.6210799670954</v>
       </c>
       <c r="X128" s="18">
-        <v>155.05637651659322</v>
+        <v>155.03787754294871</v>
       </c>
       <c r="Y128" s="18">
-        <v>169.81184074497858</v>
+        <v>169.82063917095317</v>
       </c>
       <c r="Z128" s="9"/>
       <c r="AA128" s="9"/>
@@ -10462,7 +10462,7 @@
       <c r="CQ128" s="9"/>
       <c r="CR128" s="9"/>
     </row>
-    <row r="129" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -10533,10 +10533,10 @@
         <v>105.96979550852981</v>
       </c>
       <c r="X129" s="18">
-        <v>108.91410241337849</v>
+        <v>108.91625821200159</v>
       </c>
       <c r="Y129" s="18">
-        <v>113.62556916712036</v>
+        <v>113.6218924050104</v>
       </c>
       <c r="Z129" s="9"/>
       <c r="AA129" s="9"/>
@@ -10610,7 +10610,7 @@
       <c r="CQ129" s="9"/>
       <c r="CR129" s="9"/>
     </row>
-    <row r="130" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>9</v>
       </c>
@@ -10681,10 +10681,10 @@
         <v>105.64563622715949</v>
       </c>
       <c r="X130" s="18">
-        <v>112.67476711324595</v>
+        <v>112.67269498489907</v>
       </c>
       <c r="Y130" s="18">
-        <v>118.09795557682605</v>
+        <v>118.09917994808208</v>
       </c>
       <c r="Z130" s="9"/>
       <c r="AA130" s="9"/>
@@ -10758,7 +10758,7 @@
       <c r="CQ130" s="9"/>
       <c r="CR130" s="9"/>
     </row>
-    <row r="131" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>8</v>
       </c>
@@ -10829,10 +10829,10 @@
         <v>109.07419653513935</v>
       </c>
       <c r="X131" s="18">
-        <v>112.63430716914151</v>
+        <v>112.63527496692328</v>
       </c>
       <c r="Y131" s="18">
-        <v>118.33436012932641</v>
+        <v>118.33739990085745</v>
       </c>
       <c r="Z131" s="9"/>
       <c r="AA131" s="9"/>
@@ -10906,7 +10906,7 @@
       <c r="CQ131" s="9"/>
       <c r="CR131" s="9"/>
     </row>
-    <row r="132" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -10977,10 +10977,10 @@
         <v>109.05485668352392</v>
       </c>
       <c r="X132" s="18">
-        <v>111.98832305880113</v>
+        <v>111.99249229211026</v>
       </c>
       <c r="Y132" s="18">
-        <v>116.31257312832768</v>
+        <v>116.31230608466782</v>
       </c>
       <c r="Z132" s="9"/>
       <c r="AA132" s="9"/>
@@ -11054,7 +11054,7 @@
       <c r="CQ132" s="9"/>
       <c r="CR132" s="9"/>
     </row>
-    <row r="133" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>6</v>
       </c>
@@ -11125,10 +11125,10 @@
         <v>114.57446295588424</v>
       </c>
       <c r="X133" s="18">
-        <v>129.30912128383244</v>
+        <v>129.30497836691885</v>
       </c>
       <c r="Y133" s="18">
-        <v>131.40327919431888</v>
+        <v>131.40368192895434</v>
       </c>
       <c r="Z133" s="9"/>
       <c r="AA133" s="9"/>
@@ -11202,7 +11202,7 @@
       <c r="CQ133" s="9"/>
       <c r="CR133" s="9"/>
     </row>
-    <row r="134" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -11273,10 +11273,10 @@
         <v>100.58880937489867</v>
       </c>
       <c r="X134" s="18">
-        <v>101.20197870572743</v>
+        <v>101.19927747477404</v>
       </c>
       <c r="Y134" s="18">
-        <v>101.88321458960216</v>
+        <v>101.87556596861837</v>
       </c>
       <c r="Z134" s="9"/>
       <c r="AA134" s="9"/>
@@ -11350,7 +11350,7 @@
       <c r="CQ134" s="9"/>
       <c r="CR134" s="9"/>
     </row>
-    <row r="135" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>4</v>
       </c>
@@ -11421,10 +11421,10 @@
         <v>102.67572882045511</v>
       </c>
       <c r="X135" s="18">
-        <v>105.07849702498622</v>
+        <v>105.08593237908588</v>
       </c>
       <c r="Y135" s="18">
-        <v>109.46533565297084</v>
+        <v>109.47555722579021</v>
       </c>
       <c r="Z135" s="9"/>
       <c r="AA135" s="9"/>
@@ -11498,7 +11498,7 @@
       <c r="CQ135" s="9"/>
       <c r="CR135" s="9"/>
     </row>
-    <row r="136" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -11569,10 +11569,10 @@
         <v>103.5130813886138</v>
       </c>
       <c r="X136" s="18">
-        <v>105.48621701331027</v>
+        <v>105.48730782572659</v>
       </c>
       <c r="Y136" s="18">
-        <v>109.23965535100959</v>
+        <v>109.23685100834952</v>
       </c>
       <c r="Z136" s="9"/>
       <c r="AA136" s="9"/>
@@ -11646,7 +11646,7 @@
       <c r="CQ136" s="9"/>
       <c r="CR136" s="9"/>
     </row>
-    <row r="137" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>2</v>
       </c>
@@ -11717,10 +11717,10 @@
         <v>109.4354251024056</v>
       </c>
       <c r="X137" s="18">
-        <v>114.32104166608532</v>
+        <v>114.32174183096021</v>
       </c>
       <c r="Y137" s="18">
-        <v>122.01843222620687</v>
+        <v>122.01600443375946</v>
       </c>
       <c r="Z137" s="9"/>
       <c r="AA137" s="9"/>
@@ -11794,7 +11794,7 @@
       <c r="CQ137" s="9"/>
       <c r="CR137" s="9"/>
     </row>
-    <row r="138" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -11865,10 +11865,10 @@
         <v>106.74133284107947</v>
       </c>
       <c r="X138" s="18">
-        <v>110.84568751048722</v>
+        <v>110.84610525214723</v>
       </c>
       <c r="Y138" s="18">
-        <v>114.93106496131836</v>
+        <v>114.92634953791089</v>
       </c>
       <c r="Z138" s="9"/>
       <c r="AA138" s="9"/>
@@ -11942,7 +11942,7 @@
       <c r="CQ138" s="9"/>
       <c r="CR138" s="9"/>
     </row>
-    <row r="139" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -12040,7 +12040,7 @@
       <c r="CQ139" s="9"/>
       <c r="CR139" s="9"/>
     </row>
-    <row r="140" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="s">
         <v>18</v>
       </c>
@@ -12111,10 +12111,10 @@
         <v>108.5724221745572</v>
       </c>
       <c r="X140" s="18">
-        <v>114.78730284856107</v>
+        <v>114.78822943488541</v>
       </c>
       <c r="Y140" s="18">
-        <v>120.98161390375321</v>
+        <v>120.98043391143077</v>
       </c>
       <c r="Z140" s="9"/>
       <c r="AA140" s="9"/>
@@ -12188,7 +12188,7 @@
       <c r="CQ140" s="9"/>
       <c r="CR140" s="9"/>
     </row>
-    <row r="141" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -12215,42 +12215,42 @@
       <c r="X141" s="12"/>
       <c r="Y141" s="12"/>
     </row>
-    <row r="142" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="149" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="149" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="151" spans="1:96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="151" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4" t="s">
         <v>30</v>
@@ -12279,7 +12279,7 @@
       <c r="X153" s="4"/>
       <c r="Y153" s="4"/>
     </row>
-    <row r="154" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>51</v>
       </c>
@@ -12356,10 +12356,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="155" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
     </row>
-    <row r="156" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>12</v>
       </c>
@@ -12430,10 +12430,10 @@
         <v>38.552210926748309</v>
       </c>
       <c r="X156" s="18">
-        <v>37.860836455133793</v>
+        <v>37.86218004028548</v>
       </c>
       <c r="Y156" s="18">
-        <v>36.78451940915707</v>
+        <v>36.805600081875561</v>
       </c>
       <c r="Z156" s="9"/>
       <c r="AA156" s="9"/>
@@ -12507,7 +12507,7 @@
       <c r="CQ156" s="9"/>
       <c r="CR156" s="9"/>
     </row>
-    <row r="157" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
@@ -12578,10 +12578,10 @@
         <v>2.0667156145286842</v>
       </c>
       <c r="X157" s="18">
-        <v>1.9681464012701617</v>
+        <v>1.9633629160200832</v>
       </c>
       <c r="Y157" s="18">
-        <v>1.9081299391152491</v>
+        <v>1.9035900750678985</v>
       </c>
       <c r="Z157" s="9"/>
       <c r="AA157" s="9"/>
@@ -12655,7 +12655,7 @@
       <c r="CQ157" s="9"/>
       <c r="CR157" s="9"/>
     </row>
-    <row r="158" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>10</v>
       </c>
@@ -12726,10 +12726,10 @@
         <v>1.7734895001941304</v>
       </c>
       <c r="X158" s="18">
-        <v>1.6700717973884214</v>
+        <v>1.6741114253577531</v>
       </c>
       <c r="Y158" s="18">
-        <v>1.4176515707255246</v>
+        <v>1.415184842808942</v>
       </c>
       <c r="Z158" s="9"/>
       <c r="AA158" s="9"/>
@@ -12803,7 +12803,7 @@
       <c r="CQ158" s="9"/>
       <c r="CR158" s="9"/>
     </row>
-    <row r="159" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>9</v>
       </c>
@@ -12874,10 +12874,10 @@
         <v>12.789701728180441</v>
       </c>
       <c r="X159" s="18">
-        <v>12.47360329200824</v>
+        <v>12.47101484486446</v>
       </c>
       <c r="Y159" s="18">
-        <v>12.309710528116549</v>
+        <v>12.298569145152518</v>
       </c>
       <c r="Z159" s="9"/>
       <c r="AA159" s="9"/>
@@ -12951,7 +12951,7 @@
       <c r="CQ159" s="9"/>
       <c r="CR159" s="9"/>
     </row>
-    <row r="160" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="10" t="s">
         <v>8</v>
       </c>
@@ -13022,10 +13022,10 @@
         <v>2.8352202246065437</v>
       </c>
       <c r="X160" s="18">
-        <v>2.7819628624220383</v>
+        <v>2.7774778889100018</v>
       </c>
       <c r="Y160" s="18">
-        <v>2.5898924647928303</v>
+        <v>2.5947978520960513</v>
       </c>
       <c r="Z160" s="9"/>
       <c r="AA160" s="9"/>
@@ -13099,7 +13099,7 @@
       <c r="CQ160" s="9"/>
       <c r="CR160" s="9"/>
     </row>
-    <row r="161" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>7</v>
       </c>
@@ -13170,10 +13170,10 @@
         <v>4.6588412343092838</v>
       </c>
       <c r="X161" s="18">
-        <v>4.2881117021200792</v>
+        <v>4.2888555937772743</v>
       </c>
       <c r="Y161" s="18">
-        <v>4.2895902710008667</v>
+        <v>4.2909138676920184</v>
       </c>
       <c r="Z161" s="9"/>
       <c r="AA161" s="9"/>
@@ -13247,7 +13247,7 @@
       <c r="CQ161" s="9"/>
       <c r="CR161" s="9"/>
     </row>
-    <row r="162" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>6</v>
       </c>
@@ -13318,10 +13318,10 @@
         <v>7.891542548164276</v>
       </c>
       <c r="X162" s="18">
-        <v>9.067643380195884</v>
+        <v>9.0762512233880877</v>
       </c>
       <c r="Y162" s="18">
-        <v>9.6974420735560987</v>
+        <v>9.6924665722940055</v>
       </c>
       <c r="Z162" s="9"/>
       <c r="AA162" s="9"/>
@@ -13395,7 +13395,7 @@
       <c r="CQ162" s="9"/>
       <c r="CR162" s="9"/>
     </row>
-    <row r="163" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -13466,10 +13466,10 @@
         <v>2.9933011574290407</v>
       </c>
       <c r="X163" s="18">
-        <v>2.824696245437829</v>
+        <v>2.8216047450895143</v>
       </c>
       <c r="Y163" s="18">
-        <v>2.6765719615314416</v>
+        <v>2.6754443220075546</v>
       </c>
       <c r="Z163" s="9"/>
       <c r="AA163" s="9"/>
@@ -13543,7 +13543,7 @@
       <c r="CQ163" s="9"/>
       <c r="CR163" s="9"/>
     </row>
-    <row r="164" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>4</v>
       </c>
@@ -13614,10 +13614,10 @@
         <v>1.2601254726605395</v>
       </c>
       <c r="X164" s="18">
-        <v>1.4143706838613002</v>
+        <v>1.4116546300751198</v>
       </c>
       <c r="Y164" s="18">
-        <v>1.5432146904177262</v>
+        <v>1.5422342409573144</v>
       </c>
       <c r="Z164" s="9"/>
       <c r="AA164" s="9"/>
@@ -13691,7 +13691,7 @@
       <c r="CQ164" s="9"/>
       <c r="CR164" s="9"/>
     </row>
-    <row r="165" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>3</v>
       </c>
@@ -13762,10 +13762,10 @@
         <v>5.144738906296074</v>
       </c>
       <c r="X165" s="18">
-        <v>4.9832072963907583</v>
+        <v>4.971361959949169</v>
       </c>
       <c r="Y165" s="18">
-        <v>4.9644850833860819</v>
+        <v>4.9634237116570432</v>
       </c>
       <c r="Z165" s="9"/>
       <c r="AA165" s="9"/>
@@ -13839,7 +13839,7 @@
       <c r="CQ165" s="9"/>
       <c r="CR165" s="9"/>
     </row>
-    <row r="166" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -13910,10 +13910,10 @@
         <v>5.9472445700000929</v>
       </c>
       <c r="X166" s="18">
-        <v>6.9448671886465254</v>
+        <v>6.955554515769224</v>
       </c>
       <c r="Y166" s="18">
-        <v>7.9465356902367947</v>
+        <v>7.9480511399560818</v>
       </c>
       <c r="Z166" s="9"/>
       <c r="AA166" s="9"/>
@@ -13987,7 +13987,7 @@
       <c r="CQ166" s="9"/>
       <c r="CR166" s="9"/>
     </row>
-    <row r="167" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
@@ -14058,10 +14058,10 @@
         <v>14.086868116882581</v>
       </c>
       <c r="X167" s="18">
-        <v>13.722482695124977</v>
+        <v>13.726570216513833</v>
       </c>
       <c r="Y167" s="18">
-        <v>13.872256317963746</v>
+        <v>13.869724148435008</v>
       </c>
       <c r="Z167" s="9"/>
       <c r="AA167" s="9"/>
@@ -14135,7 +14135,7 @@
       <c r="CQ167" s="9"/>
       <c r="CR167" s="9"/>
     </row>
-    <row r="168" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
@@ -14233,7 +14233,7 @@
       <c r="CQ168" s="9"/>
       <c r="CR168" s="9"/>
     </row>
-    <row r="169" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="10" t="s">
         <v>18</v>
       </c>
@@ -14381,7 +14381,7 @@
       <c r="CQ169" s="9"/>
       <c r="CR169" s="9"/>
     </row>
-    <row r="170" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -14408,12 +14408,12 @@
       <c r="X170" s="12"/>
       <c r="Y170" s="12"/>
     </row>
-    <row r="171" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -14511,7 +14511,7 @@
       <c r="CQ172" s="9"/>
       <c r="CR172" s="9"/>
     </row>
-    <row r="173" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -14609,37 +14609,37 @@
       <c r="CQ173" s="9"/>
       <c r="CR173" s="9"/>
     </row>
-    <row r="174" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="178" spans="1:96" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="178" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="180" spans="1:96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="180" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="4" t="s">
         <v>30</v>
@@ -14668,7 +14668,7 @@
       <c r="X182" s="4"/>
       <c r="Y182" s="4"/>
     </row>
-    <row r="183" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>51</v>
       </c>
@@ -14745,10 +14745,10 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="184" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
     </row>
-    <row r="185" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>12</v>
       </c>
@@ -14819,10 +14819,10 @@
         <v>38.349584787222376</v>
       </c>
       <c r="X185" s="18">
-        <v>37.440478648590016</v>
+        <v>37.442194584047265</v>
       </c>
       <c r="Y185" s="18">
-        <v>35.619346734208492</v>
+        <v>35.639459789910823</v>
       </c>
       <c r="Z185" s="9"/>
       <c r="AA185" s="9"/>
@@ -14896,7 +14896,7 @@
       <c r="CQ185" s="9"/>
       <c r="CR185" s="9"/>
     </row>
-    <row r="186" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>11</v>
       </c>
@@ -14967,10 +14967,10 @@
         <v>1.562363409791701</v>
       </c>
       <c r="X186" s="18">
-        <v>1.4570069421732375</v>
+        <v>1.4536509170517156</v>
       </c>
       <c r="Y186" s="18">
-        <v>1.3594378257692818</v>
+        <v>1.3561199298006084</v>
       </c>
       <c r="Z186" s="9"/>
       <c r="AA186" s="9"/>
@@ -15044,7 +15044,7 @@
       <c r="CQ186" s="9"/>
       <c r="CR186" s="9"/>
     </row>
-    <row r="187" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>10</v>
       </c>
@@ -15115,10 +15115,10 @@
         <v>1.8170465443780399</v>
       </c>
       <c r="X187" s="18">
-        <v>1.7601305334920299</v>
+        <v>1.7643673180498003</v>
       </c>
       <c r="Y187" s="18">
-        <v>1.5094294025256614</v>
+        <v>1.5068370427911995</v>
       </c>
       <c r="Z187" s="9"/>
       <c r="AA187" s="9"/>
@@ -15192,7 +15192,7 @@
       <c r="CQ187" s="9"/>
       <c r="CR187" s="9"/>
     </row>
-    <row r="188" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>9</v>
       </c>
@@ -15263,10 +15263,10 @@
         <v>13.144025111769697</v>
       </c>
       <c r="X188" s="18">
-        <v>12.707470495621159</v>
+        <v>12.705169726259086</v>
       </c>
       <c r="Y188" s="18">
-        <v>12.610283040935153</v>
+        <v>12.598616115068539</v>
       </c>
       <c r="Z188" s="9"/>
       <c r="AA188" s="9"/>
@@ -15340,7 +15340,7 @@
       <c r="CQ188" s="9"/>
       <c r="CR188" s="9"/>
     </row>
-    <row r="189" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="10" t="s">
         <v>8</v>
       </c>
@@ -15411,10 +15411,10 @@
         <v>2.8221773523186586</v>
       </c>
       <c r="X189" s="18">
-        <v>2.8351398577233535</v>
+        <v>2.8305676818931573</v>
       </c>
       <c r="Y189" s="18">
-        <v>2.6478308572875324</v>
+        <v>2.6527519644848492</v>
       </c>
       <c r="Z189" s="9"/>
       <c r="AA189" s="9"/>
@@ -15488,7 +15488,7 @@
       <c r="CQ189" s="9"/>
       <c r="CR189" s="9"/>
     </row>
-    <row r="190" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>7</v>
       </c>
@@ -15559,10 +15559,10 @@
         <v>4.6382315535341254</v>
       </c>
       <c r="X190" s="18">
-        <v>4.3952866080624178</v>
+        <v>4.3959209214444828</v>
       </c>
       <c r="Y190" s="18">
-        <v>4.4617837952819812</v>
+        <v>4.4631272396239199</v>
       </c>
       <c r="Z190" s="9"/>
       <c r="AA190" s="9"/>
@@ -15636,7 +15636,7 @@
       <c r="CQ190" s="9"/>
       <c r="CR190" s="9"/>
     </row>
-    <row r="191" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>6</v>
       </c>
@@ -15707,10 +15707,10 @@
         <v>7.4781401286399793</v>
       </c>
       <c r="X191" s="18">
-        <v>8.0493186905248315</v>
+        <v>8.0572830296027913</v>
       </c>
       <c r="Y191" s="18">
-        <v>8.928332686903742</v>
+        <v>8.9236374078327003</v>
       </c>
       <c r="Z191" s="9"/>
       <c r="AA191" s="9"/>
@@ -15784,7 +15784,7 @@
       <c r="CQ191" s="9"/>
       <c r="CR191" s="9"/>
     </row>
-    <row r="192" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>5</v>
       </c>
@@ -15855,10 +15855,10 @@
         <v>3.23087586958829</v>
       </c>
       <c r="X192" s="18">
-        <v>3.2038826466336228</v>
+        <v>3.2004874040195781</v>
       </c>
       <c r="Y192" s="18">
-        <v>3.1783056408259007</v>
+        <v>3.1771741526525852</v>
       </c>
       <c r="Z192" s="9"/>
       <c r="AA192" s="9"/>
@@ -15932,7 +15932,7 @@
       <c r="CQ192" s="9"/>
       <c r="CR192" s="9"/>
     </row>
-    <row r="193" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>4</v>
       </c>
@@ -16003,10 +16003,10 @@
         <v>1.3324948006929289</v>
       </c>
       <c r="X193" s="18">
-        <v>1.545052514311358</v>
+        <v>1.5419888456176505</v>
       </c>
       <c r="Y193" s="18">
-        <v>1.7055682763226463</v>
+        <v>1.7043089105202334</v>
       </c>
       <c r="Z193" s="9"/>
       <c r="AA193" s="9"/>
@@ -16080,7 +16080,7 @@
       <c r="CQ193" s="9"/>
       <c r="CR193" s="9"/>
     </row>
-    <row r="194" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
@@ -16151,10 +16151,10 @@
         <v>5.3961949255013595</v>
       </c>
       <c r="X194" s="18">
-        <v>5.4225939775220979</v>
+        <v>5.409691924314461</v>
       </c>
       <c r="Y194" s="18">
-        <v>5.49810795044408</v>
+        <v>5.4970199962708177</v>
       </c>
       <c r="Z194" s="9"/>
       <c r="AA194" s="9"/>
@@ -16228,7 +16228,7 @@
       <c r="CQ194" s="9"/>
       <c r="CR194" s="9"/>
     </row>
-    <row r="195" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>2</v>
       </c>
@@ -16299,10 +16299,10 @@
         <v>5.9003448620514298</v>
       </c>
       <c r="X195" s="18">
-        <v>6.973192000425037</v>
+        <v>6.983936518248071</v>
       </c>
       <c r="Y195" s="18">
-        <v>7.8790121722457167</v>
+        <v>7.8805946820209432</v>
       </c>
       <c r="Z195" s="9"/>
       <c r="AA195" s="9"/>
@@ -16376,7 +16376,7 @@
       <c r="CQ195" s="9"/>
       <c r="CR195" s="9"/>
     </row>
-    <row r="196" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>1</v>
       </c>
@@ -16447,10 +16447,10 @@
         <v>14.32852065451142</v>
       </c>
       <c r="X196" s="18">
-        <v>14.210447084920839</v>
+        <v>14.21474112945193</v>
       </c>
       <c r="Y196" s="18">
-        <v>14.602561617249805</v>
+        <v>14.600352769022779</v>
       </c>
       <c r="Z196" s="9"/>
       <c r="AA196" s="9"/>
@@ -16524,7 +16524,7 @@
       <c r="CQ196" s="9"/>
       <c r="CR196" s="9"/>
     </row>
-    <row r="197" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -16622,7 +16622,7 @@
       <c r="CQ197" s="9"/>
       <c r="CR197" s="9"/>
     </row>
-    <row r="198" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
         <v>18</v>
       </c>
@@ -16770,7 +16770,7 @@
       <c r="CQ198" s="9"/>
       <c r="CR198" s="9"/>
     </row>
-    <row r="199" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
@@ -16797,12 +16797,12 @@
       <c r="X199" s="12"/>
       <c r="Y199" s="12"/>
     </row>
-    <row r="200" spans="1:96" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:96" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="9"/>
@@ -16894,7 +16894,7 @@
       <c r="CL201" s="9"/>
       <c r="CM201" s="9"/>
     </row>
-    <row r="202" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="9"/>

</xml_diff>

<commit_message>
Q4 2024 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2024\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2025\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06820CE3-41CC-45B0-A911-1149853BD3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE1E9A1-5069-46D1-BBFE-011A5D2D33BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="PCE_Per_Anl">#REF!</definedName>
     <definedName name="PCE_Per_Con_Qrt">[1]HFCE!#REF!</definedName>
     <definedName name="PCE_Per_Cur_Qrt">[1]HFCE!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$Y$202</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">HFCE!$A$1:$Z$202</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="60">
   <si>
     <t>Source: Philippine Statistics Authority</t>
   </si>
@@ -214,13 +214,16 @@
     <t>2022 - 2023</t>
   </si>
   <si>
-    <t>Annual 2000 to 2023</t>
+    <t>2023 - 2024</t>
   </si>
   <si>
-    <t>Annual 2001 to 2023</t>
+    <t>Annual 2000 to 2024</t>
   </si>
   <si>
-    <t>As of April 2024</t>
+    <t>Annual 2001 to 2024</t>
+  </si>
+  <si>
+    <t>As of January 2025</t>
   </si>
 </sst>
 </file>
@@ -683,44 +686,44 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.81640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.90625" style="1" customWidth="1"/>
-    <col min="2" max="25" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="7.81640625" style="1"/>
+    <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
+    <col min="2" max="26" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:96" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>30</v>
@@ -748,8 +751,9 @@
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
-    </row>
-    <row r="10" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z9" s="4"/>
+    </row>
+    <row r="10" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
@@ -825,11 +829,14 @@
       <c r="Y10" s="6">
         <v>2023</v>
       </c>
-    </row>
-    <row r="11" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="6">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -905,7 +912,9 @@
       <c r="Y12" s="8">
         <v>6848907.220050659</v>
       </c>
-      <c r="Z12" s="9"/>
+      <c r="Z12" s="8">
+        <v>7244409.9970068187</v>
+      </c>
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
       <c r="AC12" s="9"/>
@@ -977,7 +986,7 @@
       <c r="CQ12" s="9"/>
       <c r="CR12" s="9"/>
     </row>
-    <row r="13" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1053,7 +1062,9 @@
       <c r="Y13" s="8">
         <v>354226.30741373129</v>
       </c>
-      <c r="Z13" s="9"/>
+      <c r="Z13" s="8">
+        <v>379158.27882896067</v>
+      </c>
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
       <c r="AC13" s="9"/>
@@ -1125,7 +1136,7 @@
       <c r="CQ13" s="9"/>
       <c r="CR13" s="9"/>
     </row>
-    <row r="14" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1201,7 +1212,9 @@
       <c r="Y14" s="8">
         <v>263342.25406077132</v>
       </c>
-      <c r="Z14" s="9"/>
+      <c r="Z14" s="8">
+        <v>275115.37439118931</v>
+      </c>
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
       <c r="AC14" s="9"/>
@@ -1273,7 +1286,7 @@
       <c r="CQ14" s="9"/>
       <c r="CR14" s="9"/>
     </row>
-    <row r="15" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1349,7 +1362,9 @@
       <c r="Y15" s="8">
         <v>2288558.2310069762</v>
       </c>
-      <c r="Z15" s="9"/>
+      <c r="Z15" s="8">
+        <v>2446767.2169441613</v>
+      </c>
       <c r="AA15" s="9"/>
       <c r="AB15" s="9"/>
       <c r="AC15" s="9"/>
@@ -1421,7 +1436,7 @@
       <c r="CQ15" s="9"/>
       <c r="CR15" s="9"/>
     </row>
-    <row r="16" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>8</v>
       </c>
@@ -1497,7 +1512,9 @@
       <c r="Y16" s="8">
         <v>482848.52588353655</v>
       </c>
-      <c r="Z16" s="9"/>
+      <c r="Z16" s="8">
+        <v>513111.64037570212</v>
+      </c>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
       <c r="AC16" s="9"/>
@@ -1569,7 +1586,7 @@
       <c r="CQ16" s="9"/>
       <c r="CR16" s="9"/>
     </row>
-    <row r="17" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
@@ -1645,7 +1662,9 @@
       <c r="Y17" s="8">
         <v>798467.37734682765</v>
       </c>
-      <c r="Z17" s="9"/>
+      <c r="Z17" s="8">
+        <v>902500.56339444569</v>
+      </c>
       <c r="AA17" s="9"/>
       <c r="AB17" s="9"/>
       <c r="AC17" s="9"/>
@@ -1717,7 +1736,7 @@
       <c r="CQ17" s="9"/>
       <c r="CR17" s="9"/>
     </row>
-    <row r="18" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1793,7 +1812,9 @@
       <c r="Y18" s="8">
         <v>1803606.0854710373</v>
       </c>
-      <c r="Z18" s="9"/>
+      <c r="Z18" s="8">
+        <v>1981139.30968123</v>
+      </c>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
       <c r="AC18" s="9"/>
@@ -1865,7 +1886,7 @@
       <c r="CQ18" s="9"/>
       <c r="CR18" s="9"/>
     </row>
-    <row r="19" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -1941,7 +1962,9 @@
       <c r="Y19" s="8">
         <v>497855.48647702747</v>
       </c>
-      <c r="Z19" s="9"/>
+      <c r="Z19" s="8">
+        <v>523995.41740346444</v>
+      </c>
       <c r="AA19" s="9"/>
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
@@ -2013,7 +2036,7 @@
       <c r="CQ19" s="9"/>
       <c r="CR19" s="9"/>
     </row>
-    <row r="20" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2112,9 @@
       <c r="Y20" s="8">
         <v>286984.02428991569</v>
       </c>
-      <c r="Z20" s="9"/>
+      <c r="Z20" s="8">
+        <v>325005.69285789115</v>
+      </c>
       <c r="AA20" s="9"/>
       <c r="AB20" s="9"/>
       <c r="AC20" s="9"/>
@@ -2161,7 +2186,7 @@
       <c r="CQ20" s="9"/>
       <c r="CR20" s="9"/>
     </row>
-    <row r="21" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
@@ -2237,7 +2262,9 @@
       <c r="Y21" s="8">
         <v>923610.22288231843</v>
       </c>
-      <c r="Z21" s="9"/>
+      <c r="Z21" s="8">
+        <v>992910.75619914383</v>
+      </c>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9"/>
       <c r="AC21" s="9"/>
@@ -2309,7 +2336,7 @@
       <c r="CQ21" s="9"/>
       <c r="CR21" s="9"/>
     </row>
-    <row r="22" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2385,7 +2412,9 @@
       <c r="Y22" s="8">
         <v>1478999.5195481982</v>
       </c>
-      <c r="Z22" s="9"/>
+      <c r="Z22" s="8">
+        <v>1692348.4181696777</v>
+      </c>
       <c r="AA22" s="9"/>
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
@@ -2457,7 +2486,7 @@
       <c r="CQ22" s="9"/>
       <c r="CR22" s="9"/>
     </row>
-    <row r="23" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -2533,7 +2562,9 @@
       <c r="Y23" s="8">
         <v>2580923.9259518366</v>
       </c>
-      <c r="Z23" s="9"/>
+      <c r="Z23" s="8">
+        <v>2850858.7868131101</v>
+      </c>
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
@@ -2605,7 +2636,7 @@
       <c r="CQ23" s="9"/>
       <c r="CR23" s="9"/>
     </row>
-    <row r="24" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2703,7 +2734,7 @@
       <c r="CQ24" s="9"/>
       <c r="CR24" s="9"/>
     </row>
-    <row r="25" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>18</v>
       </c>
@@ -2779,7 +2810,9 @@
       <c r="Y25" s="11">
         <v>18608329.180382837</v>
       </c>
-      <c r="Z25" s="9"/>
+      <c r="Z25" s="11">
+        <v>20127321.452065796</v>
+      </c>
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
       <c r="AC25" s="9"/>
@@ -2851,7 +2884,7 @@
       <c r="CQ25" s="9"/>
       <c r="CR25" s="9"/>
     </row>
-    <row r="26" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -2877,13 +2910,14 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
-    </row>
-    <row r="27" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z26" s="12"/>
+    </row>
+    <row r="27" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28" s="14"/>
       <c r="C28" s="14"/>
@@ -2909,7 +2943,7 @@
       <c r="W28" s="14"/>
       <c r="X28" s="14"/>
       <c r="Y28" s="14"/>
-      <c r="Z28" s="9"/>
+      <c r="Z28" s="14"/>
       <c r="AA28" s="9"/>
       <c r="AB28" s="9"/>
       <c r="AC28" s="9"/>
@@ -2981,7 +3015,7 @@
       <c r="CQ28" s="9"/>
       <c r="CR28" s="9"/>
     </row>
-    <row r="29" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3007,7 +3041,7 @@
       <c r="W29" s="15"/>
       <c r="X29" s="15"/>
       <c r="Y29" s="15"/>
-      <c r="Z29" s="9"/>
+      <c r="Z29" s="15"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9"/>
       <c r="AC29" s="9"/>
@@ -3079,37 +3113,37 @@
       <c r="CQ29" s="9"/>
       <c r="CR29" s="9"/>
     </row>
-    <row r="30" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:96" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
         <v>30</v>
@@ -3137,8 +3171,9 @@
       <c r="W38" s="4"/>
       <c r="X38" s="4"/>
       <c r="Y38" s="4"/>
-    </row>
-    <row r="39" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z38" s="4"/>
+    </row>
+    <row r="39" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>51</v>
       </c>
@@ -3214,11 +3249,14 @@
       <c r="Y39" s="17">
         <v>2023</v>
       </c>
-    </row>
-    <row r="40" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z39" s="17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="40" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>12</v>
       </c>
@@ -3294,7 +3332,9 @@
       <c r="Y41" s="8">
         <v>5481802.1240293887</v>
       </c>
-      <c r="Z41" s="9"/>
+      <c r="Z41" s="8">
+        <v>5555837.2035099892</v>
+      </c>
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
       <c r="AC41" s="9"/>
@@ -3366,7 +3406,7 @@
       <c r="CQ41" s="9"/>
       <c r="CR41" s="9"/>
     </row>
-    <row r="42" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
@@ -3442,7 +3482,9 @@
       <c r="Y42" s="8">
         <v>208588.49027010356</v>
       </c>
-      <c r="Z42" s="9"/>
+      <c r="Z42" s="8">
+        <v>213677.10598273925</v>
+      </c>
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
       <c r="AC42" s="9"/>
@@ -3514,7 +3556,7 @@
       <c r="CQ42" s="9"/>
       <c r="CR42" s="9"/>
     </row>
-    <row r="43" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
@@ -3590,7 +3632,9 @@
       <c r="Y43" s="8">
         <v>231770.69883863215</v>
       </c>
-      <c r="Z43" s="9"/>
+      <c r="Z43" s="8">
+        <v>235156.8803390268</v>
+      </c>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
       <c r="AC43" s="9"/>
@@ -3662,7 +3706,7 @@
       <c r="CQ43" s="9"/>
       <c r="CR43" s="9"/>
     </row>
-    <row r="44" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -3738,7 +3782,9 @@
       <c r="Y44" s="8">
         <v>1937827.3684991344</v>
       </c>
-      <c r="Z44" s="9"/>
+      <c r="Z44" s="8">
+        <v>2038956.7803173</v>
+      </c>
       <c r="AA44" s="9"/>
       <c r="AB44" s="9"/>
       <c r="AC44" s="9"/>
@@ -3810,7 +3856,7 @@
       <c r="CQ44" s="9"/>
       <c r="CR44" s="9"/>
     </row>
-    <row r="45" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>8</v>
       </c>
@@ -3886,7 +3932,9 @@
       <c r="Y45" s="8">
         <v>408026.98579490924</v>
       </c>
-      <c r="Z45" s="9"/>
+      <c r="Z45" s="8">
+        <v>421407.05871969997</v>
+      </c>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
       <c r="AC45" s="9"/>
@@ -3958,7 +4006,7 @@
       <c r="CQ45" s="9"/>
       <c r="CR45" s="9"/>
     </row>
-    <row r="46" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
@@ -4034,7 +4082,9 @@
       <c r="Y46" s="8">
         <v>686485.72470534209</v>
       </c>
-      <c r="Z46" s="9"/>
+      <c r="Z46" s="8">
+        <v>754543.91240541195</v>
+      </c>
       <c r="AA46" s="9"/>
       <c r="AB46" s="9"/>
       <c r="AC46" s="9"/>
@@ -4106,7 +4156,7 @@
       <c r="CQ46" s="9"/>
       <c r="CR46" s="9"/>
     </row>
-    <row r="47" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -4182,7 +4232,9 @@
       <c r="Y47" s="8">
         <v>1372568.9105471093</v>
       </c>
-      <c r="Z47" s="9"/>
+      <c r="Z47" s="8">
+        <v>1496814.6225923188</v>
+      </c>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9"/>
       <c r="AC47" s="9"/>
@@ -4254,7 +4306,7 @@
       <c r="CQ47" s="9"/>
       <c r="CR47" s="9"/>
     </row>
-    <row r="48" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -4330,7 +4382,9 @@
       <c r="Y48" s="8">
         <v>488689.78713736549</v>
       </c>
-      <c r="Z48" s="9"/>
+      <c r="Z48" s="8">
+        <v>512296.92688009219</v>
+      </c>
       <c r="AA48" s="9"/>
       <c r="AB48" s="9"/>
       <c r="AC48" s="9"/>
@@ -4402,7 +4456,7 @@
       <c r="CQ48" s="9"/>
       <c r="CR48" s="9"/>
     </row>
-    <row r="49" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -4478,7 +4532,9 @@
       <c r="Y49" s="8">
         <v>262144.38324165763</v>
       </c>
-      <c r="Z49" s="9"/>
+      <c r="Z49" s="8">
+        <v>287587.05246756552</v>
+      </c>
       <c r="AA49" s="9"/>
       <c r="AB49" s="9"/>
       <c r="AC49" s="9"/>
@@ -4550,7 +4606,7 @@
       <c r="CQ49" s="9"/>
       <c r="CR49" s="9"/>
     </row>
-    <row r="50" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -4626,7 +4682,9 @@
       <c r="Y50" s="8">
         <v>845511.5781502364</v>
       </c>
-      <c r="Z50" s="9"/>
+      <c r="Z50" s="8">
+        <v>871432.28579732252</v>
+      </c>
       <c r="AA50" s="9"/>
       <c r="AB50" s="9"/>
       <c r="AC50" s="9"/>
@@ -4698,7 +4756,7 @@
       <c r="CQ50" s="9"/>
       <c r="CR50" s="9"/>
     </row>
-    <row r="51" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>2</v>
       </c>
@@ -4774,7 +4832,9 @@
       <c r="Y51" s="8">
         <v>1212135.6754892948</v>
       </c>
-      <c r="Z51" s="9"/>
+      <c r="Z51" s="8">
+        <v>1324563.1824380772</v>
+      </c>
       <c r="AA51" s="9"/>
       <c r="AB51" s="9"/>
       <c r="AC51" s="9"/>
@@ -4846,7 +4906,7 @@
       <c r="CQ51" s="9"/>
       <c r="CR51" s="9"/>
     </row>
-    <row r="52" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
@@ -4922,7 +4982,9 @@
       <c r="Y52" s="8">
         <v>2245719.9209137536</v>
       </c>
-      <c r="Z52" s="9"/>
+      <c r="Z52" s="8">
+        <v>2403894.1661086208</v>
+      </c>
       <c r="AA52" s="9"/>
       <c r="AB52" s="9"/>
       <c r="AC52" s="9"/>
@@ -4994,7 +5056,7 @@
       <c r="CQ52" s="9"/>
       <c r="CR52" s="9"/>
     </row>
-    <row r="53" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -5092,7 +5154,7 @@
       <c r="CQ53" s="9"/>
       <c r="CR53" s="9"/>
     </row>
-    <row r="54" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
         <v>18</v>
       </c>
@@ -5168,7 +5230,9 @@
       <c r="Y54" s="11">
         <v>15381271.647616928</v>
       </c>
-      <c r="Z54" s="9"/>
+      <c r="Z54" s="11">
+        <v>16116167.177558165</v>
+      </c>
       <c r="AA54" s="9"/>
       <c r="AB54" s="9"/>
       <c r="AC54" s="9"/>
@@ -5240,7 +5304,7 @@
       <c r="CQ54" s="9"/>
       <c r="CR54" s="9"/>
     </row>
-    <row r="55" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="12"/>
       <c r="B55" s="12"/>
       <c r="C55" s="12"/>
@@ -5266,13 +5330,14 @@
       <c r="W55" s="12"/>
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
-    </row>
-    <row r="56" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z55" s="12"/>
+    </row>
+    <row r="56" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -5370,7 +5435,7 @@
       <c r="CQ57" s="9"/>
       <c r="CR57" s="9"/>
     </row>
-    <row r="58" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
@@ -5396,7 +5461,7 @@
       <c r="W58" s="16"/>
       <c r="X58" s="16"/>
       <c r="Y58" s="16"/>
-      <c r="Z58" s="9"/>
+      <c r="Z58" s="16"/>
       <c r="AA58" s="9"/>
       <c r="AB58" s="9"/>
       <c r="AC58" s="9"/>
@@ -5468,37 +5533,37 @@
       <c r="CQ58" s="9"/>
       <c r="CR58" s="9"/>
     </row>
-    <row r="59" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="1:91" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
         <v>30</v>
@@ -5526,8 +5591,9 @@
       <c r="W67" s="4"/>
       <c r="X67" s="4"/>
       <c r="Y67" s="4"/>
-    </row>
-    <row r="68" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="Z67" s="4"/>
+    </row>
+    <row r="68" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>51</v>
       </c>
@@ -5600,12 +5666,15 @@
       <c r="X68" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="Y68" s="17"/>
-    </row>
-    <row r="69" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y68" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z68" s="17"/>
+    </row>
+    <row r="69" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
     </row>
-    <row r="70" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
@@ -5678,8 +5747,10 @@
       <c r="X70" s="18">
         <v>8.1554426108115621</v>
       </c>
-      <c r="Y70" s="18"/>
-      <c r="Z70" s="9"/>
+      <c r="Y70" s="18">
+        <v>5.774684402181677</v>
+      </c>
+      <c r="Z70" s="18"/>
       <c r="AA70" s="9"/>
       <c r="AB70" s="9"/>
       <c r="AC70" s="9"/>
@@ -5746,7 +5817,7 @@
       <c r="CL70" s="9"/>
       <c r="CM70" s="9"/>
     </row>
-    <row r="71" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
@@ -5819,8 +5890,10 @@
       <c r="X71" s="18">
         <v>7.8730455824572232</v>
       </c>
-      <c r="Y71" s="18"/>
-      <c r="Z71" s="9"/>
+      <c r="Y71" s="18">
+        <v>7.0384302050466232</v>
+      </c>
+      <c r="Z71" s="18"/>
       <c r="AA71" s="9"/>
       <c r="AB71" s="9"/>
       <c r="AC71" s="9"/>
@@ -5887,7 +5960,7 @@
       <c r="CL71" s="9"/>
       <c r="CM71" s="9"/>
     </row>
-    <row r="72" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
@@ -5960,8 +6033,10 @@
       <c r="X72" s="18">
         <v>-5.9478126180803343</v>
       </c>
-      <c r="Y72" s="18"/>
-      <c r="Z72" s="9"/>
+      <c r="Y72" s="18">
+        <v>4.4706537400948605</v>
+      </c>
+      <c r="Z72" s="18"/>
       <c r="AA72" s="9"/>
       <c r="AB72" s="9"/>
       <c r="AC72" s="9"/>
@@ -6028,7 +6103,7 @@
       <c r="CL72" s="9"/>
       <c r="CM72" s="9"/>
     </row>
-    <row r="73" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
@@ -6101,8 +6176,10 @@
       <c r="X73" s="18">
         <v>9.7217898095194357</v>
       </c>
-      <c r="Y73" s="18"/>
-      <c r="Z73" s="9"/>
+      <c r="Y73" s="18">
+        <v>6.9130417480167239</v>
+      </c>
+      <c r="Z73" s="18"/>
       <c r="AA73" s="9"/>
       <c r="AB73" s="9"/>
       <c r="AC73" s="9"/>
@@ -6169,7 +6246,7 @@
       <c r="CL73" s="9"/>
       <c r="CM73" s="9"/>
     </row>
-    <row r="74" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
         <v>8</v>
       </c>
@@ -6242,8 +6319,10 @@
       <c r="X74" s="18">
         <v>3.9424649753162555</v>
       </c>
-      <c r="Y74" s="18"/>
-      <c r="Z74" s="9"/>
+      <c r="Y74" s="18">
+        <v>6.2676207692233987</v>
+      </c>
+      <c r="Z74" s="18"/>
       <c r="AA74" s="9"/>
       <c r="AB74" s="9"/>
       <c r="AC74" s="9"/>
@@ -6310,7 +6389,7 @@
       <c r="CL74" s="9"/>
       <c r="CM74" s="9"/>
     </row>
-    <row r="75" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>7</v>
       </c>
@@ -6383,8 +6462,10 @@
       <c r="X75" s="18">
         <v>11.313660747725351</v>
       </c>
-      <c r="Y75" s="18"/>
-      <c r="Z75" s="9"/>
+      <c r="Y75" s="18">
+        <v>13.029109140726931</v>
+      </c>
+      <c r="Z75" s="18"/>
       <c r="AA75" s="9"/>
       <c r="AB75" s="9"/>
       <c r="AC75" s="9"/>
@@ -6451,7 +6532,7 @@
       <c r="CL75" s="9"/>
       <c r="CM75" s="9"/>
     </row>
-    <row r="76" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
@@ -6524,8 +6605,10 @@
       <c r="X76" s="18">
         <v>18.814076269565589</v>
       </c>
-      <c r="Y76" s="18"/>
-      <c r="Z76" s="9"/>
+      <c r="Y76" s="18">
+        <v>9.8432371480842136</v>
+      </c>
+      <c r="Z76" s="18"/>
       <c r="AA76" s="9"/>
       <c r="AB76" s="9"/>
       <c r="AC76" s="9"/>
@@ -6592,7 +6675,7 @@
       <c r="CL76" s="9"/>
       <c r="CM76" s="9"/>
     </row>
-    <row r="77" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
@@ -6665,8 +6748,10 @@
       <c r="X77" s="18">
         <v>5.4969326825032567</v>
       </c>
-      <c r="Y77" s="18"/>
-      <c r="Z77" s="9"/>
+      <c r="Y77" s="18">
+        <v>5.2505057464387477</v>
+      </c>
+      <c r="Z77" s="18"/>
       <c r="AA77" s="9"/>
       <c r="AB77" s="9"/>
       <c r="AC77" s="9"/>
@@ -6733,7 +6818,7 @@
       <c r="CL77" s="9"/>
       <c r="CM77" s="9"/>
     </row>
-    <row r="78" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -6806,8 +6891,10 @@
       <c r="X78" s="18">
         <v>21.551962924822348</v>
       </c>
-      <c r="Y78" s="18"/>
-      <c r="Z78" s="9"/>
+      <c r="Y78" s="18">
+        <v>13.24870562466063</v>
+      </c>
+      <c r="Z78" s="18"/>
       <c r="AA78" s="9"/>
       <c r="AB78" s="9"/>
       <c r="AC78" s="9"/>
@@ -6874,7 +6961,7 @@
       <c r="CL78" s="9"/>
       <c r="CM78" s="9"/>
     </row>
-    <row r="79" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>3</v>
       </c>
@@ -6947,8 +7034,10 @@
       <c r="X79" s="18">
         <v>11.082605705437018</v>
       </c>
-      <c r="Y79" s="18"/>
-      <c r="Z79" s="9"/>
+      <c r="Y79" s="18">
+        <v>7.5032228530947549</v>
+      </c>
+      <c r="Z79" s="18"/>
       <c r="AA79" s="9"/>
       <c r="AB79" s="9"/>
       <c r="AC79" s="9"/>
@@ -7015,7 +7104,7 @@
       <c r="CL79" s="9"/>
       <c r="CM79" s="9"/>
     </row>
-    <row r="80" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
@@ -7088,8 +7177,10 @@
       <c r="X80" s="18">
         <v>27.136129662100615</v>
       </c>
-      <c r="Y80" s="18"/>
-      <c r="Z80" s="9"/>
+      <c r="Y80" s="18">
+        <v>14.425217574556953</v>
+      </c>
+      <c r="Z80" s="18"/>
       <c r="AA80" s="9"/>
       <c r="AB80" s="9"/>
       <c r="AC80" s="9"/>
@@ -7156,7 +7247,7 @@
       <c r="CL80" s="9"/>
       <c r="CM80" s="9"/>
     </row>
-    <row r="81" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>1</v>
       </c>
@@ -7229,8 +7320,10 @@
       <c r="X81" s="18">
         <v>12.420595103804828</v>
       </c>
-      <c r="Y81" s="18"/>
-      <c r="Z81" s="9"/>
+      <c r="Y81" s="18">
+        <v>10.458846080157997</v>
+      </c>
+      <c r="Z81" s="18"/>
       <c r="AA81" s="9"/>
       <c r="AB81" s="9"/>
       <c r="AC81" s="9"/>
@@ -7297,7 +7390,7 @@
       <c r="CL81" s="9"/>
       <c r="CM81" s="9"/>
     </row>
-    <row r="82" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -7390,7 +7483,7 @@
       <c r="CL82" s="9"/>
       <c r="CM82" s="9"/>
     </row>
-    <row r="83" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
         <v>18</v>
       </c>
@@ -7463,8 +7556,10 @@
       <c r="X83" s="18">
         <v>11.260265594306688</v>
       </c>
-      <c r="Y83" s="18"/>
-      <c r="Z83" s="9"/>
+      <c r="Y83" s="18">
+        <v>8.1629696946908155</v>
+      </c>
+      <c r="Z83" s="18"/>
       <c r="AA83" s="9"/>
       <c r="AB83" s="9"/>
       <c r="AC83" s="9"/>
@@ -7531,7 +7626,7 @@
       <c r="CL83" s="9"/>
       <c r="CM83" s="9"/>
     </row>
-    <row r="84" spans="1:91" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:91" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="12"/>
@@ -7557,13 +7652,14 @@
       <c r="W84" s="12"/>
       <c r="X84" s="12"/>
       <c r="Y84" s="12"/>
-    </row>
-    <row r="85" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="Z84" s="12"/>
+    </row>
+    <row r="85" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -7656,7 +7752,7 @@
       <c r="CL86" s="9"/>
       <c r="CM86" s="9"/>
     </row>
-    <row r="87" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -7749,37 +7845,37 @@
       <c r="CL87" s="9"/>
       <c r="CM87" s="9"/>
     </row>
-    <row r="88" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="92" spans="1:91" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="92" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:91" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:91" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
       <c r="B96" s="4" t="s">
         <v>30</v>
@@ -7807,8 +7903,9 @@
       <c r="W96" s="4"/>
       <c r="X96" s="4"/>
       <c r="Y96" s="4"/>
-    </row>
-    <row r="97" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="Z96" s="4"/>
+    </row>
+    <row r="97" spans="1:91" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>51</v>
       </c>
@@ -7881,12 +7978,15 @@
       <c r="X97" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="Y97" s="17"/>
-    </row>
-    <row r="98" spans="1:91" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y97" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z97" s="17"/>
+    </row>
+    <row r="98" spans="1:91" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
     </row>
-    <row r="99" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>12</v>
       </c>
@@ -7959,8 +8059,10 @@
       <c r="X99" s="18">
         <v>0.48289250890240965</v>
       </c>
-      <c r="Y99" s="18"/>
-      <c r="Z99" s="9"/>
+      <c r="Y99" s="18">
+        <v>1.3505609616237138</v>
+      </c>
+      <c r="Z99" s="18"/>
       <c r="AA99" s="9"/>
       <c r="AB99" s="9"/>
       <c r="AC99" s="9"/>
@@ -8027,7 +8129,7 @@
       <c r="CL99" s="9"/>
       <c r="CM99" s="9"/>
     </row>
-    <row r="100" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>11</v>
       </c>
@@ -8100,8 +8202,10 @@
       <c r="X100" s="18">
         <v>-1.5172236257926954</v>
       </c>
-      <c r="Y100" s="18"/>
-      <c r="Z100" s="9"/>
+      <c r="Y100" s="18">
+        <v>2.4395476979800748</v>
+      </c>
+      <c r="Z100" s="18"/>
       <c r="AA100" s="9"/>
       <c r="AB100" s="9"/>
       <c r="AC100" s="9"/>
@@ -8168,7 +8272,7 @@
       <c r="CL100" s="9"/>
       <c r="CM100" s="9"/>
     </row>
-    <row r="101" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>10</v>
       </c>
@@ -8241,8 +8345,10 @@
       <c r="X101" s="18">
         <v>-9.8429703161589117</v>
       </c>
-      <c r="Y101" s="18"/>
-      <c r="Z101" s="9"/>
+      <c r="Y101" s="18">
+        <v>1.4610050007884041</v>
+      </c>
+      <c r="Z101" s="18"/>
       <c r="AA101" s="9"/>
       <c r="AB101" s="9"/>
       <c r="AC101" s="9"/>
@@ -8309,7 +8415,7 @@
       <c r="CL101" s="9"/>
       <c r="CM101" s="9"/>
     </row>
-    <row r="102" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>9</v>
       </c>
@@ -8382,8 +8488,10 @@
       <c r="X102" s="18">
         <v>4.6802336971346392</v>
       </c>
-      <c r="Y102" s="18"/>
-      <c r="Z102" s="9"/>
+      <c r="Y102" s="18">
+        <v>5.2187007708788542</v>
+      </c>
+      <c r="Z102" s="18"/>
       <c r="AA102" s="9"/>
       <c r="AB102" s="9"/>
       <c r="AC102" s="9"/>
@@ -8450,7 +8558,7 @@
       <c r="CL102" s="9"/>
       <c r="CM102" s="9"/>
     </row>
-    <row r="103" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:91" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
         <v>8</v>
       </c>
@@ -8523,8 +8631,10 @@
       <c r="X103" s="18">
         <v>-1.0660354795431886</v>
       </c>
-      <c r="Y103" s="18"/>
-      <c r="Z103" s="9"/>
+      <c r="Y103" s="18">
+        <v>3.279212745873636</v>
+      </c>
+      <c r="Z103" s="18"/>
       <c r="AA103" s="9"/>
       <c r="AB103" s="9"/>
       <c r="AC103" s="9"/>
@@ -8591,7 +8701,7 @@
       <c r="CL103" s="9"/>
       <c r="CM103" s="9"/>
     </row>
-    <row r="104" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>7</v>
       </c>
@@ -8664,8 +8774,10 @@
       <c r="X104" s="18">
         <v>7.1794955576029338</v>
       </c>
-      <c r="Y104" s="18"/>
-      <c r="Z104" s="9"/>
+      <c r="Y104" s="18">
+        <v>9.9139989734356391</v>
+      </c>
+      <c r="Z104" s="18"/>
       <c r="AA104" s="9"/>
       <c r="AB104" s="9"/>
       <c r="AC104" s="9"/>
@@ -8732,7 +8844,7 @@
       <c r="CL104" s="9"/>
       <c r="CM104" s="9"/>
     </row>
-    <row r="105" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>6</v>
       </c>
@@ -8805,8 +8917,10 @@
       <c r="X105" s="18">
         <v>16.916446603284911</v>
       </c>
-      <c r="Y105" s="18"/>
-      <c r="Z105" s="9"/>
+      <c r="Y105" s="18">
+        <v>9.052056409735016</v>
+      </c>
+      <c r="Z105" s="18"/>
       <c r="AA105" s="9"/>
       <c r="AB105" s="9"/>
       <c r="AC105" s="9"/>
@@ -8873,7 +8987,7 @@
       <c r="CL105" s="9"/>
       <c r="CM105" s="9"/>
     </row>
-    <row r="106" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>5</v>
       </c>
@@ -8946,8 +9060,10 @@
       <c r="X106" s="18">
         <v>4.7966041883182839</v>
       </c>
-      <c r="Y106" s="18"/>
-      <c r="Z106" s="9"/>
+      <c r="Y106" s="18">
+        <v>4.8307004492588135</v>
+      </c>
+      <c r="Z106" s="18"/>
       <c r="AA106" s="9"/>
       <c r="AB106" s="9"/>
       <c r="AC106" s="9"/>
@@ -9014,7 +9130,7 @@
       <c r="CL106" s="9"/>
       <c r="CM106" s="9"/>
     </row>
-    <row r="107" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>4</v>
       </c>
@@ -9087,8 +9203,10 @@
       <c r="X107" s="18">
         <v>16.678112266816441</v>
       </c>
-      <c r="Y107" s="18"/>
-      <c r="Z107" s="9"/>
+      <c r="Y107" s="18">
+        <v>9.7055938835254807</v>
+      </c>
+      <c r="Z107" s="18"/>
       <c r="AA107" s="9"/>
       <c r="AB107" s="9"/>
       <c r="AC107" s="9"/>
@@ -9155,7 +9273,7 @@
       <c r="CL107" s="9"/>
       <c r="CM107" s="9"/>
     </row>
-    <row r="108" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>3</v>
       </c>
@@ -9228,8 +9346,10 @@
       <c r="X108" s="18">
         <v>7.2697071910064324</v>
       </c>
-      <c r="Y108" s="18"/>
-      <c r="Z108" s="9"/>
+      <c r="Y108" s="18">
+        <v>3.0656833468553941</v>
+      </c>
+      <c r="Z108" s="18"/>
       <c r="AA108" s="9"/>
       <c r="AB108" s="9"/>
       <c r="AC108" s="9"/>
@@ -9296,7 +9416,7 @@
       <c r="CL108" s="9"/>
       <c r="CM108" s="9"/>
     </row>
-    <row r="109" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>2</v>
       </c>
@@ -9369,8 +9489,10 @@
       <c r="X109" s="18">
         <v>19.118994758664257</v>
       </c>
-      <c r="Y109" s="18"/>
-      <c r="Z109" s="9"/>
+      <c r="Y109" s="18">
+        <v>9.275158649496845</v>
+      </c>
+      <c r="Z109" s="18"/>
       <c r="AA109" s="9"/>
       <c r="AB109" s="9"/>
       <c r="AC109" s="9"/>
@@ -9437,7 +9559,7 @@
       <c r="CL109" s="9"/>
       <c r="CM109" s="9"/>
     </row>
-    <row r="110" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>1</v>
       </c>
@@ -9510,8 +9632,10 @@
       <c r="X110" s="18">
         <v>8.4293129250983867</v>
       </c>
-      <c r="Y110" s="18"/>
-      <c r="Z110" s="9"/>
+      <c r="Y110" s="18">
+        <v>7.0433647456138857</v>
+      </c>
+      <c r="Z110" s="18"/>
       <c r="AA110" s="9"/>
       <c r="AB110" s="9"/>
       <c r="AC110" s="9"/>
@@ -9578,7 +9702,7 @@
       <c r="CL110" s="9"/>
       <c r="CM110" s="9"/>
     </row>
-    <row r="111" spans="1:91" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:91" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -9671,7 +9795,7 @@
       <c r="CL111" s="9"/>
       <c r="CM111" s="9"/>
     </row>
-    <row r="112" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:91" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
         <v>18</v>
       </c>
@@ -9744,8 +9868,10 @@
       <c r="X112" s="18">
         <v>5.5655735486568574</v>
       </c>
-      <c r="Y112" s="18"/>
-      <c r="Z112" s="9"/>
+      <c r="Y112" s="18">
+        <v>4.7778593784545649</v>
+      </c>
+      <c r="Z112" s="18"/>
       <c r="AA112" s="9"/>
       <c r="AB112" s="9"/>
       <c r="AC112" s="9"/>
@@ -9812,7 +9938,7 @@
       <c r="CL112" s="9"/>
       <c r="CM112" s="9"/>
     </row>
-    <row r="113" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="12"/>
       <c r="B113" s="12"/>
       <c r="C113" s="12"/>
@@ -9838,13 +9964,14 @@
       <c r="W113" s="12"/>
       <c r="X113" s="12"/>
       <c r="Y113" s="12"/>
-    </row>
-    <row r="114" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z113" s="12"/>
+    </row>
+    <row r="114" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A114" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -9938,7 +10065,7 @@
       <c r="CM115" s="9"/>
       <c r="CN115" s="9"/>
     </row>
-    <row r="116" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -10032,32 +10159,32 @@
       <c r="CM116" s="9"/>
       <c r="CN116" s="9"/>
     </row>
-    <row r="117" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="120" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="120" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="122" spans="1:96" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="122" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
       <c r="B124" s="4" t="s">
         <v>30</v>
@@ -10085,8 +10212,9 @@
       <c r="W124" s="4"/>
       <c r="X124" s="4"/>
       <c r="Y124" s="4"/>
-    </row>
-    <row r="125" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z124" s="4"/>
+    </row>
+    <row r="125" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
         <v>51</v>
       </c>
@@ -10162,11 +10290,14 @@
       <c r="Y125" s="17">
         <v>2023</v>
       </c>
-    </row>
-    <row r="126" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z125" s="17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="126" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="7"/>
     </row>
-    <row r="127" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>12</v>
       </c>
@@ -10242,7 +10373,9 @@
       <c r="Y127" s="18">
         <v>124.93897198566486</v>
       </c>
-      <c r="Z127" s="9"/>
+      <c r="Z127" s="18">
+        <v>130.39276947189967</v>
+      </c>
       <c r="AA127" s="9"/>
       <c r="AB127" s="9"/>
       <c r="AC127" s="9"/>
@@ -10314,7 +10447,7 @@
       <c r="CQ127" s="9"/>
       <c r="CR127" s="9"/>
     </row>
-    <row r="128" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>11</v>
       </c>
@@ -10390,7 +10523,9 @@
       <c r="Y128" s="18">
         <v>169.82063917095317</v>
       </c>
-      <c r="Z128" s="9"/>
+      <c r="Z128" s="18">
+        <v>177.44450304357312</v>
+      </c>
       <c r="AA128" s="9"/>
       <c r="AB128" s="9"/>
       <c r="AC128" s="9"/>
@@ -10462,7 +10597,7 @@
       <c r="CQ128" s="9"/>
       <c r="CR128" s="9"/>
     </row>
-    <row r="129" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>10</v>
       </c>
@@ -10538,7 +10673,9 @@
       <c r="Y129" s="18">
         <v>113.6218924050104</v>
       </c>
-      <c r="Z129" s="9"/>
+      <c r="Z129" s="18">
+        <v>116.99227085958708</v>
+      </c>
       <c r="AA129" s="9"/>
       <c r="AB129" s="9"/>
       <c r="AC129" s="9"/>
@@ -10610,7 +10747,7 @@
       <c r="CQ129" s="9"/>
       <c r="CR129" s="9"/>
     </row>
-    <row r="130" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>9</v>
       </c>
@@ -10686,7 +10823,9 @@
       <c r="Y130" s="18">
         <v>118.09917994808208</v>
       </c>
-      <c r="Z130" s="9"/>
+      <c r="Z130" s="18">
+        <v>120.00093580028697</v>
+      </c>
       <c r="AA130" s="9"/>
       <c r="AB130" s="9"/>
       <c r="AC130" s="9"/>
@@ -10758,7 +10897,7 @@
       <c r="CQ130" s="9"/>
       <c r="CR130" s="9"/>
     </row>
-    <row r="131" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
         <v>8</v>
       </c>
@@ -10834,7 +10973,9 @@
       <c r="Y131" s="18">
         <v>118.33739990085745</v>
       </c>
-      <c r="Z131" s="9"/>
+      <c r="Z131" s="18">
+        <v>121.76152006912623</v>
+      </c>
       <c r="AA131" s="9"/>
       <c r="AB131" s="9"/>
       <c r="AC131" s="9"/>
@@ -10906,7 +11047,7 @@
       <c r="CQ131" s="9"/>
       <c r="CR131" s="9"/>
     </row>
-    <row r="132" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>7</v>
       </c>
@@ -10982,7 +11123,9 @@
       <c r="Y132" s="18">
         <v>116.31230608466782</v>
       </c>
-      <c r="Z132" s="9"/>
+      <c r="Z132" s="18">
+        <v>119.60875285804937</v>
+      </c>
       <c r="AA132" s="9"/>
       <c r="AB132" s="9"/>
       <c r="AC132" s="9"/>
@@ -11054,7 +11197,7 @@
       <c r="CQ132" s="9"/>
       <c r="CR132" s="9"/>
     </row>
-    <row r="133" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>6</v>
       </c>
@@ -11130,7 +11273,9 @@
       <c r="Y133" s="18">
         <v>131.40368192895434</v>
       </c>
-      <c r="Z133" s="9"/>
+      <c r="Z133" s="18">
+        <v>132.35702536431091</v>
+      </c>
       <c r="AA133" s="9"/>
       <c r="AB133" s="9"/>
       <c r="AC133" s="9"/>
@@ -11202,7 +11347,7 @@
       <c r="CQ133" s="9"/>
       <c r="CR133" s="9"/>
     </row>
-    <row r="134" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>5</v>
       </c>
@@ -11278,7 +11423,9 @@
       <c r="Y134" s="18">
         <v>101.87556596861837</v>
       </c>
-      <c r="Z134" s="9"/>
+      <c r="Z134" s="18">
+        <v>102.28353712652864</v>
+      </c>
       <c r="AA134" s="9"/>
       <c r="AB134" s="9"/>
       <c r="AC134" s="9"/>
@@ -11350,7 +11497,7 @@
       <c r="CQ134" s="9"/>
       <c r="CR134" s="9"/>
     </row>
-    <row r="135" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>4</v>
       </c>
@@ -11426,7 +11573,9 @@
       <c r="Y135" s="18">
         <v>109.47555722579021</v>
       </c>
-      <c r="Z135" s="9"/>
+      <c r="Z135" s="18">
+        <v>113.01123957746523</v>
+      </c>
       <c r="AA135" s="9"/>
       <c r="AB135" s="9"/>
       <c r="AC135" s="9"/>
@@ -11498,7 +11647,7 @@
       <c r="CQ135" s="9"/>
       <c r="CR135" s="9"/>
     </row>
-    <row r="136" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>3</v>
       </c>
@@ -11574,7 +11723,9 @@
       <c r="Y136" s="18">
         <v>109.23685100834952</v>
       </c>
-      <c r="Z136" s="9"/>
+      <c r="Z136" s="18">
+        <v>113.94009292307476</v>
+      </c>
       <c r="AA136" s="9"/>
       <c r="AB136" s="9"/>
       <c r="AC136" s="9"/>
@@ -11646,7 +11797,7 @@
       <c r="CQ136" s="9"/>
       <c r="CR136" s="9"/>
     </row>
-    <row r="137" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>2</v>
       </c>
@@ -11722,7 +11873,9 @@
       <c r="Y137" s="18">
         <v>122.01600443375946</v>
       </c>
-      <c r="Z137" s="9"/>
+      <c r="Z137" s="18">
+        <v>127.76653017447089</v>
+      </c>
       <c r="AA137" s="9"/>
       <c r="AB137" s="9"/>
       <c r="AC137" s="9"/>
@@ -11794,7 +11947,7 @@
       <c r="CQ137" s="9"/>
       <c r="CR137" s="9"/>
     </row>
-    <row r="138" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1</v>
       </c>
@@ -11870,7 +12023,9 @@
       <c r="Y138" s="18">
         <v>114.92634953791089</v>
       </c>
-      <c r="Z138" s="9"/>
+      <c r="Z138" s="18">
+        <v>118.59335685430892</v>
+      </c>
       <c r="AA138" s="9"/>
       <c r="AB138" s="9"/>
       <c r="AC138" s="9"/>
@@ -11942,7 +12097,7 @@
       <c r="CQ138" s="9"/>
       <c r="CR138" s="9"/>
     </row>
-    <row r="139" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
@@ -12040,7 +12195,7 @@
       <c r="CQ139" s="9"/>
       <c r="CR139" s="9"/>
     </row>
-    <row r="140" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="10" t="s">
         <v>18</v>
       </c>
@@ -12116,7 +12271,9 @@
       <c r="Y140" s="18">
         <v>120.98043391143077</v>
       </c>
-      <c r="Z140" s="9"/>
+      <c r="Z140" s="18">
+        <v>124.88900884630422</v>
+      </c>
       <c r="AA140" s="9"/>
       <c r="AB140" s="9"/>
       <c r="AC140" s="9"/>
@@ -12188,7 +12345,7 @@
       <c r="CQ140" s="9"/>
       <c r="CR140" s="9"/>
     </row>
-    <row r="141" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="12"/>
       <c r="B141" s="12"/>
       <c r="C141" s="12"/>
@@ -12214,43 +12371,44 @@
       <c r="W141" s="12"/>
       <c r="X141" s="12"/>
       <c r="Y141" s="12"/>
-    </row>
-    <row r="142" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z141" s="12"/>
+    </row>
+    <row r="142" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A142" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="146" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="147" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="149" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="149" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="151" spans="1:96" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="151" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="153" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A153" s="3"/>
       <c r="B153" s="4" t="s">
         <v>30</v>
@@ -12278,8 +12436,9 @@
       <c r="W153" s="4"/>
       <c r="X153" s="4"/>
       <c r="Y153" s="4"/>
-    </row>
-    <row r="154" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z153" s="4"/>
+    </row>
+    <row r="154" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>51</v>
       </c>
@@ -12355,11 +12514,14 @@
       <c r="Y154" s="17">
         <v>2023</v>
       </c>
-    </row>
-    <row r="155" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z154" s="17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="155" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="7"/>
     </row>
-    <row r="156" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>12</v>
       </c>
@@ -12435,7 +12597,9 @@
       <c r="Y156" s="18">
         <v>36.805600081875561</v>
       </c>
-      <c r="Z156" s="9"/>
+      <c r="Z156" s="18">
+        <v>35.992916465609873</v>
+      </c>
       <c r="AA156" s="9"/>
       <c r="AB156" s="9"/>
       <c r="AC156" s="9"/>
@@ -12507,7 +12671,7 @@
       <c r="CQ156" s="9"/>
       <c r="CR156" s="9"/>
     </row>
-    <row r="157" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
@@ -12583,7 +12747,9 @@
       <c r="Y157" s="18">
         <v>1.9035900750678985</v>
       </c>
-      <c r="Z157" s="9"/>
+      <c r="Z157" s="18">
+        <v>1.8837989929854537</v>
+      </c>
       <c r="AA157" s="9"/>
       <c r="AB157" s="9"/>
       <c r="AC157" s="9"/>
@@ -12655,7 +12821,7 @@
       <c r="CQ157" s="9"/>
       <c r="CR157" s="9"/>
     </row>
-    <row r="158" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>10</v>
       </c>
@@ -12731,7 +12897,9 @@
       <c r="Y158" s="18">
         <v>1.415184842808942</v>
       </c>
-      <c r="Z158" s="9"/>
+      <c r="Z158" s="18">
+        <v>1.3668752449072277</v>
+      </c>
       <c r="AA158" s="9"/>
       <c r="AB158" s="9"/>
       <c r="AC158" s="9"/>
@@ -12803,7 +12971,7 @@
       <c r="CQ158" s="9"/>
       <c r="CR158" s="9"/>
     </row>
-    <row r="159" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>9</v>
       </c>
@@ -12879,7 +13047,9 @@
       <c r="Y159" s="18">
         <v>12.298569145152518</v>
       </c>
-      <c r="Z159" s="9"/>
+      <c r="Z159" s="18">
+        <v>12.15644725887276</v>
+      </c>
       <c r="AA159" s="9"/>
       <c r="AB159" s="9"/>
       <c r="AC159" s="9"/>
@@ -12951,7 +13121,7 @@
       <c r="CQ159" s="9"/>
       <c r="CR159" s="9"/>
     </row>
-    <row r="160" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="10" t="s">
         <v>8</v>
       </c>
@@ -13027,7 +13197,9 @@
       <c r="Y160" s="18">
         <v>2.5947978520960513</v>
       </c>
-      <c r="Z160" s="9"/>
+      <c r="Z160" s="18">
+        <v>2.549328988448377</v>
+      </c>
       <c r="AA160" s="9"/>
       <c r="AB160" s="9"/>
       <c r="AC160" s="9"/>
@@ -13099,7 +13271,7 @@
       <c r="CQ160" s="9"/>
       <c r="CR160" s="9"/>
     </row>
-    <row r="161" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>7</v>
       </c>
@@ -13175,7 +13347,9 @@
       <c r="Y161" s="18">
         <v>4.2909138676920184</v>
       </c>
-      <c r="Z161" s="9"/>
+      <c r="Z161" s="18">
+        <v>4.4839576172308622</v>
+      </c>
       <c r="AA161" s="9"/>
       <c r="AB161" s="9"/>
       <c r="AC161" s="9"/>
@@ -13247,7 +13421,7 @@
       <c r="CQ161" s="9"/>
       <c r="CR161" s="9"/>
     </row>
-    <row r="162" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>6</v>
       </c>
@@ -13323,7 +13497,9 @@
       <c r="Y162" s="18">
         <v>9.6924665722940055</v>
       </c>
-      <c r="Z162" s="9"/>
+      <c r="Z162" s="18">
+        <v>9.8430350724979014</v>
+      </c>
       <c r="AA162" s="9"/>
       <c r="AB162" s="9"/>
       <c r="AC162" s="9"/>
@@ -13395,7 +13571,7 @@
       <c r="CQ162" s="9"/>
       <c r="CR162" s="9"/>
     </row>
-    <row r="163" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>5</v>
       </c>
@@ -13471,7 +13647,9 @@
       <c r="Y163" s="18">
         <v>2.6754443220075546</v>
       </c>
-      <c r="Z163" s="9"/>
+      <c r="Z163" s="18">
+        <v>2.603403630489955</v>
+      </c>
       <c r="AA163" s="9"/>
       <c r="AB163" s="9"/>
       <c r="AC163" s="9"/>
@@ -13543,7 +13721,7 @@
       <c r="CQ163" s="9"/>
       <c r="CR163" s="9"/>
     </row>
-    <row r="164" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>4</v>
       </c>
@@ -13619,7 +13797,9 @@
       <c r="Y164" s="18">
         <v>1.5422342409573144</v>
       </c>
-      <c r="Z164" s="9"/>
+      <c r="Z164" s="18">
+        <v>1.6147488558371175</v>
+      </c>
       <c r="AA164" s="9"/>
       <c r="AB164" s="9"/>
       <c r="AC164" s="9"/>
@@ -13691,7 +13871,7 @@
       <c r="CQ164" s="9"/>
       <c r="CR164" s="9"/>
     </row>
-    <row r="165" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>3</v>
       </c>
@@ -13767,7 +13947,9 @@
       <c r="Y165" s="18">
         <v>4.9634237116570432</v>
       </c>
-      <c r="Z165" s="9"/>
+      <c r="Z165" s="18">
+        <v>4.9331489963222852</v>
+      </c>
       <c r="AA165" s="9"/>
       <c r="AB165" s="9"/>
       <c r="AC165" s="9"/>
@@ -13839,7 +14021,7 @@
       <c r="CQ165" s="9"/>
       <c r="CR165" s="9"/>
     </row>
-    <row r="166" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>2</v>
       </c>
@@ -13915,7 +14097,9 @@
       <c r="Y166" s="18">
         <v>7.9480511399560818</v>
       </c>
-      <c r="Z166" s="9"/>
+      <c r="Z166" s="18">
+        <v>8.4082147850626257</v>
+      </c>
       <c r="AA166" s="9"/>
       <c r="AB166" s="9"/>
       <c r="AC166" s="9"/>
@@ -13987,7 +14171,7 @@
       <c r="CQ166" s="9"/>
       <c r="CR166" s="9"/>
     </row>
-    <row r="167" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>1</v>
       </c>
@@ -14063,7 +14247,9 @@
       <c r="Y167" s="18">
         <v>13.869724148435008</v>
       </c>
-      <c r="Z167" s="9"/>
+      <c r="Z167" s="18">
+        <v>14.164124091735555</v>
+      </c>
       <c r="AA167" s="9"/>
       <c r="AB167" s="9"/>
       <c r="AC167" s="9"/>
@@ -14135,7 +14321,7 @@
       <c r="CQ167" s="9"/>
       <c r="CR167" s="9"/>
     </row>
-    <row r="168" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
@@ -14233,7 +14419,7 @@
       <c r="CQ168" s="9"/>
       <c r="CR168" s="9"/>
     </row>
-    <row r="169" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="10" t="s">
         <v>18</v>
       </c>
@@ -14309,7 +14495,9 @@
       <c r="Y169" s="18">
         <v>100</v>
       </c>
-      <c r="Z169" s="9"/>
+      <c r="Z169" s="18">
+        <v>100</v>
+      </c>
       <c r="AA169" s="9"/>
       <c r="AB169" s="9"/>
       <c r="AC169" s="9"/>
@@ -14381,7 +14569,7 @@
       <c r="CQ169" s="9"/>
       <c r="CR169" s="9"/>
     </row>
-    <row r="170" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="12"/>
       <c r="B170" s="12"/>
       <c r="C170" s="12"/>
@@ -14407,13 +14595,14 @@
       <c r="W170" s="12"/>
       <c r="X170" s="12"/>
       <c r="Y170" s="12"/>
-    </row>
-    <row r="171" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z170" s="12"/>
+    </row>
+    <row r="171" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A171" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
@@ -14511,7 +14700,7 @@
       <c r="CQ172" s="9"/>
       <c r="CR172" s="9"/>
     </row>
-    <row r="173" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
@@ -14609,37 +14798,37 @@
       <c r="CQ173" s="9"/>
       <c r="CR173" s="9"/>
     </row>
-    <row r="174" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="176" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="178" spans="1:96" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="178" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="179" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="180" spans="1:96" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="180" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="182" spans="1:96" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A182" s="3"/>
       <c r="B182" s="4" t="s">
         <v>30</v>
@@ -14667,8 +14856,9 @@
       <c r="W182" s="4"/>
       <c r="X182" s="4"/>
       <c r="Y182" s="4"/>
-    </row>
-    <row r="183" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z182" s="4"/>
+    </row>
+    <row r="183" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>51</v>
       </c>
@@ -14744,11 +14934,14 @@
       <c r="Y183" s="17">
         <v>2023</v>
       </c>
-    </row>
-    <row r="184" spans="1:96" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z183" s="17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="184" spans="1:96" ht="10.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="7"/>
     </row>
-    <row r="185" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>12</v>
       </c>
@@ -14824,7 +15017,9 @@
       <c r="Y185" s="18">
         <v>35.639459789910823</v>
       </c>
-      <c r="Z185" s="9"/>
+      <c r="Z185" s="18">
+        <v>34.47368808165826</v>
+      </c>
       <c r="AA185" s="9"/>
       <c r="AB185" s="9"/>
       <c r="AC185" s="9"/>
@@ -14896,7 +15091,7 @@
       <c r="CQ185" s="9"/>
       <c r="CR185" s="9"/>
     </row>
-    <row r="186" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>11</v>
       </c>
@@ -14972,7 +15167,9 @@
       <c r="Y186" s="18">
         <v>1.3561199298006084</v>
       </c>
-      <c r="Z186" s="9"/>
+      <c r="Z186" s="18">
+        <v>1.3258556059177991</v>
+      </c>
       <c r="AA186" s="9"/>
       <c r="AB186" s="9"/>
       <c r="AC186" s="9"/>
@@ -15044,7 +15241,7 @@
       <c r="CQ186" s="9"/>
       <c r="CR186" s="9"/>
     </row>
-    <row r="187" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>10</v>
       </c>
@@ -15120,7 +15317,9 @@
       <c r="Y187" s="18">
         <v>1.5068370427911995</v>
       </c>
-      <c r="Z187" s="9"/>
+      <c r="Z187" s="18">
+        <v>1.459136516444703</v>
+      </c>
       <c r="AA187" s="9"/>
       <c r="AB187" s="9"/>
       <c r="AC187" s="9"/>
@@ -15192,7 +15391,7 @@
       <c r="CQ187" s="9"/>
       <c r="CR187" s="9"/>
     </row>
-    <row r="188" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>9</v>
       </c>
@@ -15268,7 +15467,9 @@
       <c r="Y188" s="18">
         <v>12.598616115068539</v>
       </c>
-      <c r="Z188" s="9"/>
+      <c r="Z188" s="18">
+        <v>12.651623415501401</v>
+      </c>
       <c r="AA188" s="9"/>
       <c r="AB188" s="9"/>
       <c r="AC188" s="9"/>
@@ -15340,7 +15541,7 @@
       <c r="CQ188" s="9"/>
       <c r="CR188" s="9"/>
     </row>
-    <row r="189" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:96" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="10" t="s">
         <v>8</v>
       </c>
@@ -15416,7 +15617,9 @@
       <c r="Y189" s="18">
         <v>2.6527519644848492</v>
       </c>
-      <c r="Z189" s="9"/>
+      <c r="Z189" s="18">
+        <v>2.6148094275573861</v>
+      </c>
       <c r="AA189" s="9"/>
       <c r="AB189" s="9"/>
       <c r="AC189" s="9"/>
@@ -15488,7 +15691,7 @@
       <c r="CQ189" s="9"/>
       <c r="CR189" s="9"/>
     </row>
-    <row r="190" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>7</v>
       </c>
@@ -15564,7 +15767,9 @@
       <c r="Y190" s="18">
         <v>4.4631272396239199</v>
       </c>
-      <c r="Z190" s="9"/>
+      <c r="Z190" s="18">
+        <v>4.6819067095315177</v>
+      </c>
       <c r="AA190" s="9"/>
       <c r="AB190" s="9"/>
       <c r="AC190" s="9"/>
@@ -15636,7 +15841,7 @@
       <c r="CQ190" s="9"/>
       <c r="CR190" s="9"/>
     </row>
-    <row r="191" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>6</v>
       </c>
@@ -15712,7 +15917,9 @@
       <c r="Y191" s="18">
         <v>8.9236374078327003</v>
       </c>
-      <c r="Z191" s="9"/>
+      <c r="Z191" s="18">
+        <v>9.28765882173672</v>
+      </c>
       <c r="AA191" s="9"/>
       <c r="AB191" s="9"/>
       <c r="AC191" s="9"/>
@@ -15784,7 +15991,7 @@
       <c r="CQ191" s="9"/>
       <c r="CR191" s="9"/>
     </row>
-    <row r="192" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>5</v>
       </c>
@@ -15860,7 +16067,9 @@
       <c r="Y192" s="18">
         <v>3.1771741526525852</v>
       </c>
-      <c r="Z192" s="9"/>
+      <c r="Z192" s="18">
+        <v>3.1787764499828968</v>
+      </c>
       <c r="AA192" s="9"/>
       <c r="AB192" s="9"/>
       <c r="AC192" s="9"/>
@@ -15932,7 +16141,7 @@
       <c r="CQ192" s="9"/>
       <c r="CR192" s="9"/>
     </row>
-    <row r="193" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>4</v>
       </c>
@@ -16008,7 +16217,9 @@
       <c r="Y193" s="18">
         <v>1.7043089105202334</v>
       </c>
-      <c r="Z193" s="9"/>
+      <c r="Z193" s="18">
+        <v>1.7844630754887663</v>
+      </c>
       <c r="AA193" s="9"/>
       <c r="AB193" s="9"/>
       <c r="AC193" s="9"/>
@@ -16080,7 +16291,7 @@
       <c r="CQ193" s="9"/>
       <c r="CR193" s="9"/>
     </row>
-    <row r="194" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>3</v>
       </c>
@@ -16156,7 +16367,9 @@
       <c r="Y194" s="18">
         <v>5.4970199962708177</v>
       </c>
-      <c r="Z194" s="9"/>
+      <c r="Z194" s="18">
+        <v>5.4071931383958081</v>
+      </c>
       <c r="AA194" s="9"/>
       <c r="AB194" s="9"/>
       <c r="AC194" s="9"/>
@@ -16228,7 +16441,7 @@
       <c r="CQ194" s="9"/>
       <c r="CR194" s="9"/>
     </row>
-    <row r="195" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>2</v>
       </c>
@@ -16304,7 +16517,9 @@
       <c r="Y195" s="18">
         <v>7.8805946820209432</v>
       </c>
-      <c r="Z195" s="9"/>
+      <c r="Z195" s="18">
+        <v>8.2188473713684065</v>
+      </c>
       <c r="AA195" s="9"/>
       <c r="AB195" s="9"/>
       <c r="AC195" s="9"/>
@@ -16376,7 +16591,7 @@
       <c r="CQ195" s="9"/>
       <c r="CR195" s="9"/>
     </row>
-    <row r="196" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>1</v>
       </c>
@@ -16452,7 +16667,9 @@
       <c r="Y196" s="18">
         <v>14.600352769022779</v>
       </c>
-      <c r="Z196" s="9"/>
+      <c r="Z196" s="18">
+        <v>14.916041386416332</v>
+      </c>
       <c r="AA196" s="9"/>
       <c r="AB196" s="9"/>
       <c r="AC196" s="9"/>
@@ -16524,7 +16741,7 @@
       <c r="CQ196" s="9"/>
       <c r="CR196" s="9"/>
     </row>
-    <row r="197" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
@@ -16622,7 +16839,7 @@
       <c r="CQ197" s="9"/>
       <c r="CR197" s="9"/>
     </row>
-    <row r="198" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:96" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="10" t="s">
         <v>18</v>
       </c>
@@ -16698,7 +16915,9 @@
       <c r="Y198" s="18">
         <v>100</v>
       </c>
-      <c r="Z198" s="9"/>
+      <c r="Z198" s="18">
+        <v>100</v>
+      </c>
       <c r="AA198" s="9"/>
       <c r="AB198" s="9"/>
       <c r="AC198" s="9"/>
@@ -16770,7 +16989,7 @@
       <c r="CQ198" s="9"/>
       <c r="CR198" s="9"/>
     </row>
-    <row r="199" spans="1:96" ht="7.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:96" ht="7.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
@@ -16796,13 +17015,14 @@
       <c r="W199" s="12"/>
       <c r="X199" s="12"/>
       <c r="Y199" s="12"/>
-    </row>
-    <row r="200" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="Z199" s="12"/>
+    </row>
+    <row r="200" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A200" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
       <c r="D201" s="9"/>
@@ -16894,7 +17114,7 @@
       <c r="CL201" s="9"/>
       <c r="CM201" s="9"/>
     </row>
-    <row r="202" spans="1:96" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:96" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
       <c r="D202" s="9"/>
@@ -16991,9 +17211,9 @@
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="58" max="24" man="1"/>
-    <brk id="116" max="24" man="1"/>
-    <brk id="144" max="24" man="1"/>
+    <brk id="58" max="25" man="1"/>
+    <brk id="116" max="25" man="1"/>
+    <brk id="144" max="25" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q1 2025 SNA Update
</commit_message>
<xml_diff>
--- a/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
+++ b/Data/National Accounts/PSA-02HFCE_2018PSNA_Ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of January 2025\Annl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Other computers\My Laptop (1)\6. MAS_Series\2018-base\NAP\NAP detailed series as of April 2025\Annl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE1E9A1-5069-46D1-BBFE-011A5D2D33BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BF0ECE-87FC-4745-837F-824B5C556FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="7500" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HFCE" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
     <t>Annual 2001 to 2024</t>
   </si>
   <si>
-    <t>As of January 2025</t>
+    <t>As of April 2025</t>
   </si>
 </sst>
 </file>
@@ -680,10 +680,10 @@
   <dimension ref="A1:CR202"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" view="pageBreakPreview" colorId="22" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -910,10 +910,10 @@
         <v>6332466.545114967</v>
       </c>
       <c r="Y12" s="8">
-        <v>6848907.220050659</v>
+        <v>6853549.1516588246</v>
       </c>
       <c r="Z12" s="8">
-        <v>7244409.9970068187</v>
+        <v>7253561.4106219551</v>
       </c>
       <c r="AA12" s="9"/>
       <c r="AB12" s="9"/>
@@ -1060,10 +1060,10 @@
         <v>328373.32579338714</v>
       </c>
       <c r="Y13" s="8">
-        <v>354226.30741373129</v>
+        <v>354222.47225195228</v>
       </c>
       <c r="Z13" s="8">
-        <v>379158.27882896067</v>
+        <v>379665.70152991894</v>
       </c>
       <c r="AA13" s="9"/>
       <c r="AB13" s="9"/>
@@ -1210,10 +1210,10 @@
         <v>279995.88461607165</v>
       </c>
       <c r="Y14" s="8">
-        <v>263342.25406077132</v>
+        <v>264092.89607673243</v>
       </c>
       <c r="Z14" s="8">
-        <v>275115.37439118931</v>
+        <v>276462.78159096901</v>
       </c>
       <c r="AA14" s="9"/>
       <c r="AB14" s="9"/>
@@ -1360,10 +1360,10 @@
         <v>2085782.8103059449</v>
       </c>
       <c r="Y15" s="8">
-        <v>2288558.2310069762</v>
+        <v>2288370.7310069762</v>
       </c>
       <c r="Z15" s="8">
-        <v>2446767.2169441613</v>
+        <v>2446525.1380855888</v>
       </c>
       <c r="AA15" s="9"/>
       <c r="AB15" s="9"/>
@@ -1510,10 +1510,10 @@
         <v>464534.41911176633</v>
       </c>
       <c r="Y16" s="8">
-        <v>482848.52588353655</v>
+        <v>482907.40297373611</v>
       </c>
       <c r="Z16" s="8">
-        <v>513111.64037570212</v>
+        <v>512769.59179124155</v>
       </c>
       <c r="AA16" s="9"/>
       <c r="AB16" s="9"/>
@@ -1660,10 +1660,10 @@
         <v>717313.01619522378</v>
       </c>
       <c r="Y17" s="8">
-        <v>798467.37734682765</v>
+        <v>798192.55504901591</v>
       </c>
       <c r="Z17" s="8">
-        <v>902500.56339444569</v>
+        <v>902698.60629759915</v>
       </c>
       <c r="AA17" s="9"/>
       <c r="AB17" s="9"/>
@@ -1810,10 +1810,10 @@
         <v>1518007.0763492808</v>
       </c>
       <c r="Y18" s="8">
-        <v>1803606.0854710373</v>
+        <v>1803980.3159114744</v>
       </c>
       <c r="Z18" s="8">
-        <v>1981139.30968123</v>
+        <v>1980593.3007632052</v>
       </c>
       <c r="AA18" s="9"/>
       <c r="AB18" s="9"/>
@@ -1960,10 +1960,10 @@
         <v>471914.65554296359</v>
       </c>
       <c r="Y19" s="8">
-        <v>497855.48647702747</v>
+        <v>496996.86583779933</v>
       </c>
       <c r="Z19" s="8">
-        <v>523995.41740346444</v>
+        <v>524252.61151829897</v>
       </c>
       <c r="AA19" s="9"/>
       <c r="AB19" s="9"/>
@@ -2110,10 +2110,10 @@
         <v>236099.86822459626</v>
       </c>
       <c r="Y20" s="8">
-        <v>286984.02428991569</v>
+        <v>286654.14915700798</v>
       </c>
       <c r="Z20" s="8">
-        <v>325005.69285789115</v>
+        <v>323464.92441998917</v>
       </c>
       <c r="AA20" s="9"/>
       <c r="AB20" s="9"/>
@@ -2260,10 +2260,10 @@
         <v>831462.5111797424</v>
       </c>
       <c r="Y21" s="8">
-        <v>923610.22288231843</v>
+        <v>916860.10352940368</v>
       </c>
       <c r="Z21" s="8">
-        <v>992910.75619914383</v>
+        <v>995314.90010947862</v>
       </c>
       <c r="AA21" s="9"/>
       <c r="AB21" s="9"/>
@@ -2410,10 +2410,10 @@
         <v>1163319.6035454657</v>
       </c>
       <c r="Y22" s="8">
-        <v>1478999.5195481982</v>
+        <v>1477881.4663575722</v>
       </c>
       <c r="Z22" s="8">
-        <v>1692348.4181696777</v>
+        <v>1692667.6367904763</v>
       </c>
       <c r="AA22" s="9"/>
       <c r="AB22" s="9"/>
@@ -2560,10 +2560,10 @@
         <v>2295775.0077454327</v>
       </c>
       <c r="Y23" s="8">
-        <v>2580923.9259518366</v>
+        <v>2580749.4352202103</v>
       </c>
       <c r="Z23" s="8">
-        <v>2850858.7868131101</v>
+        <v>2849715.4939333918</v>
       </c>
       <c r="AA23" s="9"/>
       <c r="AB23" s="9"/>
@@ -2808,10 +2808,10 @@
         <v>16725044.723724842</v>
       </c>
       <c r="Y25" s="11">
-        <v>18608329.180382837</v>
+        <v>18604457.545030702</v>
       </c>
       <c r="Z25" s="11">
-        <v>20127321.452065796</v>
+        <v>20137692.097452115</v>
       </c>
       <c r="AA25" s="9"/>
       <c r="AB25" s="9"/>
@@ -3330,10 +3330,10 @@
         <v>5455458.12541545</v>
       </c>
       <c r="Y41" s="8">
-        <v>5481802.1240293887</v>
+        <v>5485461.5751280217</v>
       </c>
       <c r="Z41" s="8">
-        <v>5555837.2035099892</v>
+        <v>5562853.208788068</v>
       </c>
       <c r="AA41" s="9"/>
       <c r="AB41" s="9"/>
@@ -3480,10 +3480,10 @@
         <v>211802.0002579182</v>
       </c>
       <c r="Y42" s="8">
-        <v>208588.49027010356</v>
+        <v>208586.20924864014</v>
       </c>
       <c r="Z42" s="8">
-        <v>213677.10598273925</v>
+        <v>213899.19798559108</v>
       </c>
       <c r="AA42" s="9"/>
       <c r="AB42" s="9"/>
@@ -3630,10 +3630,10 @@
         <v>257074.46180447156</v>
       </c>
       <c r="Y43" s="8">
-        <v>231770.69883863215</v>
+        <v>232443.53280160273</v>
       </c>
       <c r="Z43" s="8">
-        <v>235156.8803390268</v>
+        <v>236284.95390045649</v>
       </c>
       <c r="AA43" s="9"/>
       <c r="AB43" s="9"/>
@@ -3780,10 +3780,10 @@
         <v>1851187.4687877942</v>
       </c>
       <c r="Y44" s="8">
-        <v>1937827.3684991344</v>
+        <v>1937670.7077466038</v>
       </c>
       <c r="Z44" s="8">
-        <v>2038956.7803173</v>
+        <v>2038772.0417034051</v>
       </c>
       <c r="AA44" s="9"/>
       <c r="AB44" s="9"/>
@@ -3930,10 +3930,10 @@
         <v>412423.56734884565</v>
       </c>
       <c r="Y45" s="8">
-        <v>408026.98579490924</v>
+        <v>408076.47724212188</v>
       </c>
       <c r="Z45" s="8">
-        <v>421407.05871969997</v>
+        <v>421120.50234056893</v>
       </c>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
@@ -4080,10 +4080,10 @@
         <v>640500.98494482529</v>
       </c>
       <c r="Y46" s="8">
-        <v>686485.72470534209</v>
+        <v>686248.25037239364</v>
       </c>
       <c r="Z46" s="8">
-        <v>754543.91240541195</v>
+        <v>754723.16311876278</v>
       </c>
       <c r="AA46" s="9"/>
       <c r="AB46" s="9"/>
@@ -4230,10 +4230,10 @@
         <v>1173974.1930444073</v>
       </c>
       <c r="Y47" s="8">
-        <v>1372568.9105471093</v>
+        <v>1372864.2504209473</v>
       </c>
       <c r="Z47" s="8">
-        <v>1496814.6225923188</v>
+        <v>1496402.0513733246</v>
       </c>
       <c r="AA47" s="9"/>
       <c r="AB47" s="9"/>
@@ -4380,10 +4380,10 @@
         <v>466322.15893102379</v>
       </c>
       <c r="Y48" s="8">
-        <v>488689.78713736549</v>
+        <v>487836.33144416905</v>
       </c>
       <c r="Z48" s="8">
-        <v>512296.92688009219</v>
+        <v>512532.57860805659</v>
       </c>
       <c r="AA48" s="9"/>
       <c r="AB48" s="9"/>
@@ -4530,10 +4530,10 @@
         <v>224673.14404452546</v>
       </c>
       <c r="Y49" s="8">
-        <v>262144.38324165763</v>
+        <v>261856.2734591449</v>
       </c>
       <c r="Z49" s="8">
-        <v>287587.05246756552</v>
+        <v>286249.69045336795</v>
       </c>
       <c r="AA49" s="9"/>
       <c r="AB49" s="9"/>
@@ -4680,10 +4680,10 @@
         <v>788210.95003522548</v>
       </c>
       <c r="Y50" s="8">
-        <v>845511.5781502364</v>
+        <v>839365.86430522939</v>
       </c>
       <c r="Z50" s="8">
-        <v>871432.28579732252</v>
+        <v>873586.32457309763</v>
       </c>
       <c r="AA50" s="9"/>
       <c r="AB50" s="9"/>
@@ -4830,10 +4830,10 @@
         <v>1017583.8689245896</v>
       </c>
       <c r="Y51" s="8">
-        <v>1212135.6754892948</v>
+        <v>1211225.7496792087</v>
       </c>
       <c r="Z51" s="8">
-        <v>1324563.1824380772</v>
+        <v>1324816.1353516914</v>
       </c>
       <c r="AA51" s="9"/>
       <c r="AB51" s="9"/>
@@ -4980,10 +4980,10 @@
         <v>2071137.2785927998</v>
       </c>
       <c r="Y52" s="8">
-        <v>2245719.9209137536</v>
+        <v>2245566.0873440439</v>
       </c>
       <c r="Z52" s="8">
-        <v>2403894.1661086208</v>
+        <v>2402886.2157230945</v>
       </c>
       <c r="AA52" s="9"/>
       <c r="AB52" s="9"/>
@@ -5228,10 +5228,10 @@
         <v>14570348.202131879</v>
       </c>
       <c r="Y54" s="11">
-        <v>15381271.647616928</v>
+        <v>15377201.309192125</v>
       </c>
       <c r="Z54" s="11">
-        <v>16116167.177558165</v>
+        <v>16124126.063919485</v>
       </c>
       <c r="AA54" s="9"/>
       <c r="AB54" s="9"/>
@@ -5745,10 +5745,10 @@
         <v>12.438904936169365</v>
       </c>
       <c r="X70" s="18">
-        <v>8.1554426108115621</v>
+        <v>8.2287463002206351</v>
       </c>
       <c r="Y70" s="18">
-        <v>5.774684402181677</v>
+        <v>5.8365709519470244</v>
       </c>
       <c r="Z70" s="18"/>
       <c r="AA70" s="9"/>
@@ -5888,10 +5888,10 @@
         <v>8.7627408786468521</v>
       </c>
       <c r="X71" s="18">
-        <v>7.8730455824572232</v>
+        <v>7.8718776551386185</v>
       </c>
       <c r="Y71" s="18">
-        <v>7.0384302050466232</v>
+        <v>7.1828388290027192</v>
       </c>
       <c r="Z71" s="18"/>
       <c r="AA71" s="9"/>
@@ -6031,10 +6031,10 @@
         <v>8.0727043503763269</v>
       </c>
       <c r="X72" s="18">
-        <v>-5.9478126180803343</v>
+        <v>-5.679722243469854</v>
       </c>
       <c r="Y72" s="18">
-        <v>4.4706537400948605</v>
+        <v>4.6839145232602277</v>
       </c>
       <c r="Z72" s="18"/>
       <c r="AA72" s="9"/>
@@ -6174,10 +6174,10 @@
         <v>11.635329940343993</v>
       </c>
       <c r="X73" s="18">
-        <v>9.7217898095194357</v>
+        <v>9.7128003788330801</v>
       </c>
       <c r="Y73" s="18">
-        <v>6.9130417480167239</v>
+        <v>6.9112231220077831</v>
       </c>
       <c r="Z73" s="18"/>
       <c r="AA73" s="9"/>
@@ -6317,10 +6317,10 @@
         <v>12.156408169853904</v>
       </c>
       <c r="X74" s="18">
-        <v>3.9424649753162555</v>
+        <v>3.9551394054073938</v>
       </c>
       <c r="Y74" s="18">
-        <v>6.2676207692233987</v>
+        <v>6.18383330502175</v>
       </c>
       <c r="Z74" s="18"/>
       <c r="AA74" s="9"/>
@@ -6460,10 +6460,10 @@
         <v>5.3959186259596947</v>
       </c>
       <c r="X75" s="18">
-        <v>11.313660747725351</v>
+        <v>11.275348003970961</v>
       </c>
       <c r="Y75" s="18">
-        <v>13.029109140726931</v>
+        <v>13.092837134037879</v>
       </c>
       <c r="Z75" s="18"/>
       <c r="AA75" s="9"/>
@@ -6603,10 +6603,10 @@
         <v>31.675472759479021</v>
       </c>
       <c r="X76" s="18">
-        <v>18.814076269565589</v>
+        <v>18.838729016332564</v>
       </c>
       <c r="Y76" s="18">
-        <v>9.8432371480842136</v>
+        <v>9.7901835898079383</v>
       </c>
       <c r="Z76" s="18"/>
       <c r="AA76" s="9"/>
@@ -6746,10 +6746,10 @@
         <v>7.9210206085330555</v>
       </c>
       <c r="X77" s="18">
-        <v>5.4969326825032567</v>
+        <v>5.3149886319968829</v>
       </c>
       <c r="Y77" s="18">
-        <v>5.2505057464387477</v>
+        <v>5.4840880403851173</v>
       </c>
       <c r="Z77" s="18"/>
       <c r="AA77" s="9"/>
@@ -6889,10 +6889,10 @@
         <v>28.255189491692619</v>
       </c>
       <c r="X78" s="18">
-        <v>21.551962924822348</v>
+        <v>21.412244450861209</v>
       </c>
       <c r="Y78" s="18">
-        <v>13.24870562466063</v>
+        <v>12.841528849742545</v>
       </c>
       <c r="Z78" s="18"/>
       <c r="AA78" s="9"/>
@@ -7032,10 +7032,10 @@
         <v>10.629850594700343</v>
       </c>
       <c r="X79" s="18">
-        <v>11.082605705437018</v>
+        <v>10.27076882017117</v>
       </c>
       <c r="Y79" s="18">
-        <v>7.5032228530947549</v>
+        <v>8.556899387165771</v>
       </c>
       <c r="Z79" s="18"/>
       <c r="AA79" s="9"/>
@@ -7175,10 +7175,10 @@
         <v>33.898663077517909</v>
       </c>
       <c r="X80" s="18">
-        <v>27.136129662100615</v>
+        <v>27.040020803690723</v>
       </c>
       <c r="Y80" s="18">
-        <v>14.425217574556953</v>
+        <v>14.533382772724806</v>
       </c>
       <c r="Z80" s="18"/>
       <c r="AA80" s="9"/>
@@ -7318,10 +7318,10 @@
         <v>11.559836138107542</v>
       </c>
       <c r="X81" s="18">
-        <v>12.420595103804828</v>
+        <v>12.412994588465239</v>
       </c>
       <c r="Y81" s="18">
-        <v>10.458846080157997</v>
+        <v>10.422013661711077</v>
       </c>
       <c r="Z81" s="18"/>
       <c r="AA81" s="9"/>
@@ -7554,10 +7554,10 @@
         <v>14.488082166943258</v>
       </c>
       <c r="X83" s="18">
-        <v>11.260265594306688</v>
+        <v>11.237116864864774</v>
       </c>
       <c r="Y83" s="18">
-        <v>8.1629696946908155</v>
+        <v>8.2412214852829493</v>
       </c>
       <c r="Z83" s="18"/>
       <c r="AA83" s="9"/>
@@ -8057,10 +8057,10 @@
         <v>5.7263111727320108</v>
       </c>
       <c r="X99" s="18">
-        <v>0.48289250890240965</v>
+        <v>0.54997122189965353</v>
       </c>
       <c r="Y99" s="18">
-        <v>1.3505609616237138</v>
+        <v>1.4108499822686298</v>
       </c>
       <c r="Z99" s="18"/>
       <c r="AA99" s="9"/>
@@ -8200,10 +8200,10 @@
         <v>0.75358714095771973</v>
       </c>
       <c r="X100" s="18">
-        <v>-1.5172236257926954</v>
+        <v>-1.5183005851512661</v>
       </c>
       <c r="Y100" s="18">
-        <v>2.4395476979800748</v>
+        <v>2.5471428605415127</v>
       </c>
       <c r="Z100" s="18"/>
       <c r="AA100" s="9"/>
@@ -8343,10 +8343,10 @@
         <v>5.1490619313363766</v>
       </c>
       <c r="X101" s="18">
-        <v>-9.8429703161589117</v>
+        <v>-9.5812430491842804</v>
       </c>
       <c r="Y101" s="18">
-        <v>1.4610050007884041</v>
+        <v>1.6526255011502116</v>
       </c>
       <c r="Z101" s="18"/>
       <c r="AA101" s="9"/>
@@ -8486,10 +8486,10 @@
         <v>4.6729685356081063</v>
       </c>
       <c r="X102" s="18">
-        <v>4.6802336971346392</v>
+        <v>4.671770980355717</v>
       </c>
       <c r="Y102" s="18">
-        <v>5.2187007708788542</v>
+        <v>5.2176736507709478</v>
       </c>
       <c r="Z102" s="18"/>
       <c r="AA102" s="9"/>
@@ -8629,10 +8629,10 @@
         <v>8.6104695974367615</v>
       </c>
       <c r="X103" s="18">
-        <v>-1.0660354795431886</v>
+        <v>-1.0540353294230584</v>
       </c>
       <c r="Y103" s="18">
-        <v>3.279212745873636</v>
+        <v>3.1964658160650998</v>
       </c>
       <c r="Z103" s="18"/>
       <c r="AA103" s="9"/>
@@ -8772,10 +8772,10 @@
         <v>2.6313154171328392</v>
       </c>
       <c r="X104" s="18">
-        <v>7.1794955576029338</v>
+        <v>7.1424192160312003</v>
       </c>
       <c r="Y104" s="18">
-        <v>9.9139989734356391</v>
+        <v>9.9781548017370056</v>
       </c>
       <c r="Z104" s="18"/>
       <c r="AA104" s="9"/>
@@ -8915,10 +8915,10 @@
         <v>16.674908935596065</v>
       </c>
       <c r="X105" s="18">
-        <v>16.916446603284911</v>
+        <v>16.941603874678762</v>
       </c>
       <c r="Y105" s="18">
-        <v>9.052056409735016</v>
+        <v>8.9985445330445657</v>
       </c>
       <c r="Z105" s="18"/>
       <c r="AA105" s="9"/>
@@ -9058,10 +9058,10 @@
         <v>7.2700046919033809</v>
       </c>
       <c r="X106" s="18">
-        <v>4.7966041883182839</v>
+        <v>4.6135857156055664</v>
       </c>
       <c r="Y106" s="18">
-        <v>4.8307004492588135</v>
+        <v>5.0624042475020019</v>
       </c>
       <c r="Z106" s="18"/>
       <c r="AA106" s="9"/>
@@ -9201,10 +9201,10 @@
         <v>25.313586299643816</v>
       </c>
       <c r="X107" s="18">
-        <v>16.678112266816441</v>
+        <v>16.549877188370374</v>
       </c>
       <c r="Y107" s="18">
-        <v>9.7055938835254807</v>
+        <v>9.3155747891711087</v>
       </c>
       <c r="Z107" s="18"/>
       <c r="AA107" s="9"/>
@@ -9344,10 +9344,10 @@
         <v>8.5593799354365103</v>
       </c>
       <c r="X108" s="18">
-        <v>7.2697071910064324</v>
+        <v>6.4900029957358072</v>
       </c>
       <c r="Y108" s="18">
-        <v>3.0656833468553941</v>
+        <v>4.0769420967808401</v>
       </c>
       <c r="Z108" s="18"/>
       <c r="AA108" s="9"/>
@@ -9487,10 +9487,10 @@
         <v>28.17559354719009</v>
       </c>
       <c r="X109" s="18">
-        <v>19.118994758664257</v>
+        <v>19.029574531214323</v>
       </c>
       <c r="Y109" s="18">
-        <v>9.275158649496845</v>
+        <v>9.3781349762888482</v>
       </c>
       <c r="Z109" s="18"/>
       <c r="AA109" s="9"/>
@@ -9630,10 +9630,10 @@
         <v>7.4286333635826765</v>
       </c>
       <c r="X110" s="18">
-        <v>8.4293129250983867</v>
+        <v>8.4218854324208223</v>
       </c>
       <c r="Y110" s="18">
-        <v>7.0433647456138857</v>
+        <v>7.0058115530735421</v>
       </c>
       <c r="Z110" s="18"/>
       <c r="AA110" s="9"/>
@@ -9866,10 +9866,10 @@
         <v>8.2885279455932448</v>
       </c>
       <c r="X112" s="18">
-        <v>5.5655735486568574</v>
+        <v>5.5376377823433955</v>
       </c>
       <c r="Y112" s="18">
-        <v>4.7778593784545649</v>
+        <v>4.8573517359161258</v>
       </c>
       <c r="Z112" s="18"/>
       <c r="AA112" s="9"/>
@@ -10371,10 +10371,10 @@
         <v>116.07579784388373</v>
       </c>
       <c r="Y127" s="18">
-        <v>124.93897198566486</v>
+        <v>124.94024537030639</v>
       </c>
       <c r="Z127" s="18">
-        <v>130.39276947189967</v>
+        <v>130.39282430035982</v>
       </c>
       <c r="AA127" s="9"/>
       <c r="AB127" s="9"/>
@@ -10521,10 +10521,10 @@
         <v>155.03787754294871</v>
       </c>
       <c r="Y128" s="18">
-        <v>169.82063917095317</v>
+        <v>169.82065762061478</v>
       </c>
       <c r="Z128" s="18">
-        <v>177.44450304357312</v>
+        <v>177.49748718342292</v>
       </c>
       <c r="AA128" s="9"/>
       <c r="AB128" s="9"/>
@@ -10671,10 +10671,10 @@
         <v>108.91625821200159</v>
       </c>
       <c r="Y129" s="18">
-        <v>113.6218924050104</v>
+        <v>113.61593626360143</v>
       </c>
       <c r="Z129" s="18">
-        <v>116.99227085958708</v>
+        <v>117.00397212233788</v>
       </c>
       <c r="AA129" s="9"/>
       <c r="AB129" s="9"/>
@@ -10821,10 +10821,10 @@
         <v>112.67269498489907</v>
       </c>
       <c r="Y130" s="18">
-        <v>118.09917994808208</v>
+        <v>118.09905170462198</v>
       </c>
       <c r="Z130" s="18">
-        <v>120.00093580028697</v>
+        <v>119.99993564957383</v>
       </c>
       <c r="AA130" s="9"/>
       <c r="AB130" s="9"/>
@@ -10971,10 +10971,10 @@
         <v>112.63527496692328</v>
       </c>
       <c r="Y131" s="18">
-        <v>118.33739990085745</v>
+        <v>118.33747591562724</v>
       </c>
       <c r="Z131" s="18">
-        <v>121.76152006912623</v>
+        <v>121.7631506757071</v>
       </c>
       <c r="AA131" s="9"/>
       <c r="AB131" s="9"/>
@@ -11121,10 +11121,10 @@
         <v>111.99249229211026</v>
       </c>
       <c r="Y132" s="18">
-        <v>116.31230608466782</v>
+        <v>116.31250857337349</v>
       </c>
       <c r="Z132" s="18">
-        <v>119.60875285804937</v>
+        <v>119.60658562105786</v>
       </c>
       <c r="AA132" s="9"/>
       <c r="AB132" s="9"/>
@@ -11271,10 +11271,10 @@
         <v>129.30497836691885</v>
       </c>
       <c r="Y133" s="18">
-        <v>131.40368192895434</v>
+        <v>131.40267257730241</v>
       </c>
       <c r="Z133" s="18">
-        <v>132.35702536431091</v>
+        <v>132.35702924528294</v>
       </c>
       <c r="AA133" s="9"/>
       <c r="AB133" s="9"/>
@@ -11421,10 +11421,10 @@
         <v>101.19927747477404</v>
       </c>
       <c r="Y134" s="18">
-        <v>101.87556596861837</v>
+        <v>101.87778847190651</v>
       </c>
       <c r="Z134" s="18">
-        <v>102.28353712652864</v>
+        <v>102.28669032943658</v>
       </c>
       <c r="AA134" s="9"/>
       <c r="AB134" s="9"/>
@@ -11571,10 +11571,10 @@
         <v>105.08593237908588</v>
       </c>
       <c r="Y135" s="18">
-        <v>109.47555722579021</v>
+        <v>109.47003307206695</v>
       </c>
       <c r="Z135" s="18">
-        <v>113.01123957746523</v>
+        <v>113.0009691565706</v>
       </c>
       <c r="AA135" s="9"/>
       <c r="AB135" s="9"/>
@@ -11721,10 +11721,10 @@
         <v>105.48730782572659</v>
       </c>
       <c r="Y136" s="18">
-        <v>109.23685100834952</v>
+        <v>109.23247448099629</v>
       </c>
       <c r="Z136" s="18">
-        <v>113.94009292307476</v>
+        <v>113.93434994485143</v>
       </c>
       <c r="AA136" s="9"/>
       <c r="AB136" s="9"/>
@@ -11871,10 +11871,10 @@
         <v>114.32174183096021</v>
       </c>
       <c r="Y137" s="18">
-        <v>122.01600443375946</v>
+        <v>122.01536061704326</v>
       </c>
       <c r="Z137" s="18">
-        <v>127.76653017447089</v>
+        <v>127.76623046949329</v>
       </c>
       <c r="AA137" s="9"/>
       <c r="AB137" s="9"/>
@@ -12021,10 +12021,10 @@
         <v>110.84610525214723</v>
       </c>
       <c r="Y138" s="18">
-        <v>114.92634953791089</v>
+        <v>114.92645216568116</v>
       </c>
       <c r="Z138" s="18">
-        <v>118.59335685430892</v>
+        <v>118.59552380327065</v>
       </c>
       <c r="AA138" s="9"/>
       <c r="AB138" s="9"/>
@@ -12269,10 +12269,10 @@
         <v>114.78822943488541</v>
       </c>
       <c r="Y140" s="18">
-        <v>120.98043391143077</v>
+        <v>120.98727961576077</v>
       </c>
       <c r="Z140" s="18">
-        <v>124.88900884630422</v>
+        <v>124.89168105993464</v>
       </c>
       <c r="AA140" s="9"/>
       <c r="AB140" s="9"/>
@@ -12595,10 +12595,10 @@
         <v>37.86218004028548</v>
       </c>
       <c r="Y156" s="18">
-        <v>36.805600081875561</v>
+        <v>36.838210063745855</v>
       </c>
       <c r="Z156" s="18">
-        <v>35.992916465609873</v>
+        <v>36.019824791837486</v>
       </c>
       <c r="AA156" s="9"/>
       <c r="AB156" s="9"/>
@@ -12745,10 +12745,10 @@
         <v>1.9633629160200832</v>
       </c>
       <c r="Y157" s="18">
-        <v>1.9035900750678985</v>
+        <v>1.903965602837832</v>
       </c>
       <c r="Z157" s="18">
-        <v>1.8837989929854537</v>
+        <v>1.8853486273035003</v>
       </c>
       <c r="AA157" s="9"/>
       <c r="AB157" s="9"/>
@@ -12895,10 +12895,10 @@
         <v>1.6741114253577531</v>
       </c>
       <c r="Y158" s="18">
-        <v>1.415184842808942</v>
+        <v>1.4195140892311171</v>
       </c>
       <c r="Z158" s="18">
-        <v>1.3668752449072277</v>
+        <v>1.3728622935194641</v>
       </c>
       <c r="AA158" s="9"/>
       <c r="AB158" s="9"/>
@@ -13045,10 +13045,10 @@
         <v>12.47101484486446</v>
       </c>
       <c r="Y159" s="18">
-        <v>12.298569145152518</v>
+        <v>12.300120685960048</v>
       </c>
       <c r="Z159" s="18">
-        <v>12.15644725887276</v>
+        <v>12.148984730952019</v>
       </c>
       <c r="AA159" s="9"/>
       <c r="AB159" s="9"/>
@@ -13195,10 +13195,10 @@
         <v>2.7774778889100018</v>
       </c>
       <c r="Y160" s="18">
-        <v>2.5947978520960513</v>
+        <v>2.5956543038403281</v>
       </c>
       <c r="Z160" s="18">
-        <v>2.549328988448377</v>
+        <v>2.5463175686161117</v>
       </c>
       <c r="AA160" s="9"/>
       <c r="AB160" s="9"/>
@@ -13345,10 +13345,10 @@
         <v>4.2888555937772743</v>
       </c>
       <c r="Y161" s="18">
-        <v>4.2909138676920184</v>
+        <v>4.2903296326541653</v>
       </c>
       <c r="Z161" s="18">
-        <v>4.4839576172308622</v>
+        <v>4.4826318821897742</v>
       </c>
       <c r="AA161" s="9"/>
       <c r="AB161" s="9"/>
@@ -13495,10 +13495,10 @@
         <v>9.0762512233880877</v>
       </c>
       <c r="Y162" s="18">
-        <v>9.6924665722940055</v>
+        <v>9.696495109008552</v>
       </c>
       <c r="Z162" s="18">
-        <v>9.8430350724979014</v>
+        <v>9.8352546616491168</v>
       </c>
       <c r="AA162" s="9"/>
       <c r="AB162" s="9"/>
@@ -13645,10 +13645,10 @@
         <v>2.8216047450895143</v>
       </c>
       <c r="Y163" s="18">
-        <v>2.6754443220075546</v>
+        <v>2.6713859548705221</v>
       </c>
       <c r="Z163" s="18">
-        <v>2.603403630489955</v>
+        <v>2.6033400897247261</v>
       </c>
       <c r="AA163" s="9"/>
       <c r="AB163" s="9"/>
@@ -13795,10 +13795,10 @@
         <v>1.4116546300751198</v>
       </c>
       <c r="Y164" s="18">
-        <v>1.5422342409573144</v>
+        <v>1.540782086568141</v>
       </c>
       <c r="Z164" s="18">
-        <v>1.6147488558371175</v>
+        <v>1.6062661145808015</v>
       </c>
       <c r="AA164" s="9"/>
       <c r="AB164" s="9"/>
@@ -13945,10 +13945,10 @@
         <v>4.971361959949169</v>
       </c>
       <c r="Y165" s="18">
-        <v>4.9634237116570432</v>
+        <v>4.9281743437571999</v>
       </c>
       <c r="Z165" s="18">
-        <v>4.9331489963222852</v>
+        <v>4.9425470172692183</v>
       </c>
       <c r="AA165" s="9"/>
       <c r="AB165" s="9"/>
@@ -14095,10 +14095,10 @@
         <v>6.955554515769224</v>
       </c>
       <c r="Y166" s="18">
-        <v>7.9480511399560818</v>
+        <v>7.9436955513509089</v>
       </c>
       <c r="Z166" s="18">
-        <v>8.4082147850626257</v>
+        <v>8.4054698452988958</v>
       </c>
       <c r="AA166" s="9"/>
       <c r="AB166" s="9"/>
@@ -14245,10 +14245,10 @@
         <v>13.726570216513833</v>
       </c>
       <c r="Y167" s="18">
-        <v>13.869724148435008</v>
+        <v>13.871672576175353</v>
       </c>
       <c r="Z167" s="18">
-        <v>14.164124091735555</v>
+        <v>14.151152377058873</v>
       </c>
       <c r="AA167" s="9"/>
       <c r="AB167" s="9"/>
@@ -15015,10 +15015,10 @@
         <v>37.442194584047265</v>
       </c>
       <c r="Y185" s="18">
-        <v>35.639459789910823</v>
+        <v>35.672691439949759</v>
       </c>
       <c r="Z185" s="18">
-        <v>34.47368808165826</v>
+        <v>34.50018429982331</v>
       </c>
       <c r="AA185" s="9"/>
       <c r="AB185" s="9"/>
@@ -15165,10 +15165,10 @@
         <v>1.4536509170517156</v>
       </c>
       <c r="Y186" s="18">
-        <v>1.3561199298006084</v>
+        <v>1.356464060361571</v>
       </c>
       <c r="Z186" s="18">
-        <v>1.3258556059177991</v>
+        <v>1.326578551529856</v>
       </c>
       <c r="AA186" s="9"/>
       <c r="AB186" s="9"/>
@@ -15315,10 +15315,10 @@
         <v>1.7643673180498003</v>
       </c>
       <c r="Y187" s="18">
-        <v>1.5068370427911995</v>
+        <v>1.5116114312859619</v>
       </c>
       <c r="Z187" s="18">
-        <v>1.459136516444703</v>
+        <v>1.4654124692635893</v>
       </c>
       <c r="AA187" s="9"/>
       <c r="AB187" s="9"/>
@@ -15465,10 +15465,10 @@
         <v>12.705169726259086</v>
       </c>
       <c r="Y188" s="18">
-        <v>12.598616115068539</v>
+        <v>12.600932177354734</v>
       </c>
       <c r="Z188" s="18">
-        <v>12.651623415501401</v>
+        <v>12.644232832348724</v>
       </c>
       <c r="AA188" s="9"/>
       <c r="AB188" s="9"/>
@@ -15615,10 +15615,10 @@
         <v>2.8305676818931573</v>
       </c>
       <c r="Y189" s="18">
-        <v>2.6527519644848492</v>
+        <v>2.6537759962743253</v>
       </c>
       <c r="Z189" s="18">
-        <v>2.6148094275573861</v>
+        <v>2.6117415646042286</v>
       </c>
       <c r="AA189" s="9"/>
       <c r="AB189" s="9"/>
@@ -15765,10 +15765,10 @@
         <v>4.3959209214444828</v>
       </c>
       <c r="Y190" s="18">
-        <v>4.4631272396239199</v>
+        <v>4.4627643000431476</v>
       </c>
       <c r="Z190" s="18">
-        <v>4.6819067095315177</v>
+        <v>4.6807074078116155</v>
       </c>
       <c r="AA190" s="9"/>
       <c r="AB190" s="9"/>
@@ -15915,10 +15915,10 @@
         <v>8.0572830296027913</v>
       </c>
       <c r="Y191" s="18">
-        <v>8.9236374078327003</v>
+        <v>8.9279201254930687</v>
       </c>
       <c r="Z191" s="18">
-        <v>9.28765882173672</v>
+        <v>9.2805157032465928</v>
       </c>
       <c r="AA191" s="9"/>
       <c r="AB191" s="9"/>
@@ -16065,10 +16065,10 @@
         <v>3.2004874040195781</v>
       </c>
       <c r="Y192" s="18">
-        <v>3.1771741526525852</v>
+        <v>3.1724650125543463</v>
       </c>
       <c r="Z192" s="18">
-        <v>3.1787764499828968</v>
+        <v>3.1786688877044735</v>
       </c>
       <c r="AA192" s="9"/>
       <c r="AB192" s="9"/>
@@ -16215,10 +16215,10 @@
         <v>1.5419888456176505</v>
       </c>
       <c r="Y193" s="18">
-        <v>1.7043089105202334</v>
+        <v>1.7028864238293706</v>
       </c>
       <c r="Z193" s="18">
-        <v>1.7844630754887663</v>
+        <v>1.7752880951104757</v>
       </c>
       <c r="AA193" s="9"/>
       <c r="AB193" s="9"/>
@@ -16365,10 +16365,10 @@
         <v>5.409691924314461</v>
       </c>
       <c r="Y194" s="18">
-        <v>5.4970199962708177</v>
+        <v>5.4585086546501573</v>
       </c>
       <c r="Z194" s="18">
-        <v>5.4071931383958081</v>
+        <v>5.4178832459509101</v>
       </c>
       <c r="AA194" s="9"/>
       <c r="AB194" s="9"/>
@@ -16515,10 +16515,10 @@
         <v>6.983936518248071</v>
       </c>
       <c r="Y195" s="18">
-        <v>7.8805946820209432</v>
+        <v>7.8767633025339068</v>
       </c>
       <c r="Z195" s="18">
-        <v>8.2188473713684065</v>
+        <v>8.2163593245291988</v>
       </c>
       <c r="AA195" s="9"/>
       <c r="AB195" s="9"/>
@@ -16665,10 +16665,10 @@
         <v>14.21474112945193</v>
       </c>
       <c r="Y196" s="18">
-        <v>14.600352769022779</v>
+        <v>14.603217075669667</v>
       </c>
       <c r="Z196" s="18">
-        <v>14.916041386416332</v>
+        <v>14.902427618077033</v>
       </c>
       <c r="AA196" s="9"/>
       <c r="AB196" s="9"/>

</xml_diff>